<commit_message>
Boat Enabled - ABP
Boat Enabled - ABP
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35D5B2A-516D-447F-AFB5-C504DCEAFCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC4BEAD-FC74-4771-970F-5031FBF2C310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1841,9 +1841,6 @@
     <t>X_Polimer_X</t>
   </si>
   <si>
-    <t>!M_15_NOC_X_Spouse_X_Drive_Media_X39X</t>
-  </si>
-  <si>
     <t>!M_25_NOC_X_EmployerLeft_PM_X_Drive_RJ</t>
   </si>
   <si>
@@ -1854,6 +1851,9 @@
   </si>
   <si>
     <t>FuelW</t>
+  </si>
+  <si>
+    <t>!M_15_NOC_X_Spouse_X_Drive_Media_X0X</t>
   </si>
 </sst>
 </file>
@@ -4733,6 +4733,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4763,62 +4820,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4844,12 +5006,6 @@
     <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4871,161 +5027,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5084,15 +5093,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5111,25 +5111,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5207,46 +5228,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5541,7 +5541,7 @@
   <dimension ref="B1:V28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5731,7 +5731,7 @@
         <v>228</v>
       </c>
       <c r="V5" s="19">
-        <v>5460</v>
+        <v>5520</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5929,7 +5929,7 @@
         <v>227</v>
       </c>
       <c r="V11" s="64">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6485,8 +6485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+    <sheetView topLeftCell="H11" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6543,7 +6543,7 @@
       <c r="P1" s="432" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="545" t="s">
+      <c r="Q1" s="564" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6563,32 +6563,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="558">
+      <c r="A2" s="548">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
-      </c>
-      <c r="B2" s="560" t="s">
+        <v>45278</v>
+      </c>
+      <c r="B2" s="550" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="572" t="s">
+      <c r="C2" s="562" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="562" t="s">
+      <c r="D2" s="552" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="564" t="s">
+      <c r="E2" s="554" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="199" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="570" t="s">
+      <c r="G2" s="560" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="552" t="s">
+      <c r="I2" s="571" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="430" t="s">
@@ -6612,14 +6612,14 @@
       <c r="P2" s="433">
         <v>40</v>
       </c>
-      <c r="Q2" s="546"/>
+      <c r="Q2" s="565"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>8</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T2" s="177">
         <f>SUM(T4:T16)</f>
@@ -6638,14 +6638,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="559"/>
-      <c r="B3" s="561"/>
-      <c r="C3" s="573"/>
-      <c r="D3" s="563"/>
-      <c r="E3" s="565"/>
-      <c r="G3" s="571"/>
+      <c r="A3" s="549"/>
+      <c r="B3" s="551"/>
+      <c r="C3" s="563"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="555"/>
+      <c r="G3" s="561"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="553"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="Q3" s="508">
         <f>SUM(X24:X30)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="506"/>
@@ -6665,10 +6665,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="252"/>
-      <c r="C4" s="566" t="s">
+      <c r="C4" s="556" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="553"/>
+      <c r="I4" s="572"/>
       <c r="R4" s="508" t="s">
         <v>581</v>
       </c>
@@ -6691,7 +6691,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="567"/>
+      <c r="C5" s="557"/>
       <c r="D5" s="231" t="s">
         <v>103</v>
       </c>
@@ -6707,7 +6707,7 @@
       <c r="H5" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="553"/>
+      <c r="I5" s="572"/>
       <c r="J5" s="431" t="s">
         <v>273</v>
       </c>
@@ -6744,22 +6744,22 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="555" t="s">
+      <c r="A6" s="545" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="568"/>
-      <c r="D6" s="569"/>
+      <c r="C6" s="558"/>
+      <c r="D6" s="559"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="535"/>
-      <c r="I6" s="553"/>
+      <c r="I6" s="572"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="556"/>
+      <c r="A7" s="546"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="535"/>
-      <c r="I7" s="553"/>
+      <c r="I7" s="572"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6808,7 +6808,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="557"/>
+      <c r="A8" s="547"/>
       <c r="B8" s="220" t="s">
         <v>28</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="535"/>
-      <c r="I8" s="553"/>
+      <c r="I8" s="572"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="G9" s="535"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="553"/>
+      <c r="I9" s="572"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6867,10 +6867,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="535"/>
-      <c r="I10" s="553"/>
+      <c r="I10" s="572"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="535"/>
-      <c r="I11" s="553"/>
+      <c r="I11" s="572"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6934,12 +6934,12 @@
       <c r="S11" s="24">
         <v>0</v>
       </c>
-      <c r="U11" s="547" t="s">
+      <c r="U11" s="566" t="s">
         <v>584</v>
       </c>
-      <c r="V11" s="548"/>
-      <c r="W11" s="548"/>
-      <c r="X11" s="549"/>
+      <c r="V11" s="567"/>
+      <c r="W11" s="567"/>
+      <c r="X11" s="568"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="236" t="s">
@@ -6950,7 +6950,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="535"/>
-      <c r="I12" s="553"/>
+      <c r="I12" s="572"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -6983,7 +6983,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="535"/>
-      <c r="I13" s="553"/>
+      <c r="I13" s="572"/>
       <c r="J13" s="108" t="s">
         <v>573</v>
       </c>
@@ -7024,7 +7024,7 @@
       <c r="H14" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="553"/>
+      <c r="I14" s="572"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7042,7 +7042,7 @@
       <c r="H15" s="282">
         <v>0</v>
       </c>
-      <c r="I15" s="553"/>
+      <c r="I15" s="572"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7073,7 +7073,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="553"/>
+      <c r="I16" s="572"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7107,7 +7107,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="553"/>
+      <c r="I17" s="572"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7119,13 +7119,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="553"/>
+      <c r="I18" s="572"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="550" t="s">
+      <c r="O18" s="569" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="551"/>
+      <c r="P18" s="570"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U18" s="6" t="s">
         <v>479</v>
@@ -7151,7 +7151,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="553"/>
+      <c r="I19" s="572"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7183,7 +7183,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="553"/>
+      <c r="I20" s="572"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7208,7 +7208,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="553"/>
+      <c r="I21" s="572"/>
       <c r="M21" s="225" t="s">
         <v>422</v>
       </c>
@@ -7221,9 +7221,7 @@
       <c r="W21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="X21" s="506">
-        <v>1</v>
-      </c>
+      <c r="X21" s="506"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="240" t="s">
@@ -7244,7 +7242,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="553"/>
+      <c r="I22" s="572"/>
       <c r="U22" s="6" t="s">
         <v>585</v>
       </c>
@@ -7268,7 +7266,7 @@
       <c r="E23" s="294" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="553"/>
+      <c r="I23" s="572"/>
       <c r="U23" s="6" t="s">
         <v>74</v>
       </c>
@@ -7278,7 +7276,7 @@
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="553"/>
+      <c r="I24" s="572"/>
       <c r="U24" s="363"/>
       <c r="V24" s="507">
         <v>-1</v>
@@ -7306,7 +7304,7 @@
       <c r="H25" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="553"/>
+      <c r="I25" s="572"/>
       <c r="J25" s="431" t="s">
         <v>274</v>
       </c>
@@ -7351,7 +7349,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="553"/>
+      <c r="I26" s="572"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7369,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T26" s="61" t="s">
         <v>582</v>
@@ -7386,7 +7384,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="553"/>
+      <c r="I27" s="572"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7413,7 +7411,7 @@
       <c r="E28" s="224">
         <v>2</v>
       </c>
-      <c r="I28" s="553"/>
+      <c r="I28" s="572"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7435,7 +7433,7 @@
       <c r="H29" s="199" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="554"/>
+      <c r="I29" s="573"/>
       <c r="J29" s="342"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7448,13 +7446,13 @@
       <c r="T29" s="80"/>
       <c r="U29" s="35"/>
       <c r="V29" s="112">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="W29" s="19" t="s">
         <v>88</v>
       </c>
       <c r="X29" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7479,6 +7477,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7490,11 +7493,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7505,7 +7503,7 @@
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7570,7 +7568,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="570" t="s">
+      <c r="I1" s="560" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7631,7 +7629,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="436"/>
-      <c r="AN1" s="601"/>
+      <c r="AN1" s="598"/>
       <c r="AO1" s="359" t="s">
         <v>487</v>
       </c>
@@ -7640,23 +7638,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="625">
+      <c r="A2" s="580">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
-      </c>
-      <c r="B2" s="627" t="s">
+        <v>45278</v>
+      </c>
+      <c r="B2" s="582" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="572" t="s">
+      <c r="C2" s="562" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="629" t="s">
+      <c r="D2" s="584" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="574" t="s">
+      <c r="E2" s="628" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="582" t="s">
+      <c r="F2" s="603" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="427" t="s">
@@ -7665,31 +7663,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="571"/>
+      <c r="I2" s="561"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="576" t="s">
+      <c r="K2" s="630" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="577"/>
-      <c r="M2" s="582" t="s">
+      <c r="L2" s="631"/>
+      <c r="M2" s="603" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="608" t="s">
+      <c r="O2" s="607" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="572" t="s">
+      <c r="Q2" s="562" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="534"/>
-      <c r="S2" s="595" t="s">
+      <c r="S2" s="620" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7722,15 +7720,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="462"/>
-      <c r="AN2" s="602"/>
+      <c r="AN2" s="599"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="626"/>
-      <c r="B3" s="628"/>
-      <c r="C3" s="573"/>
-      <c r="D3" s="630"/>
-      <c r="E3" s="575"/>
-      <c r="F3" s="583"/>
+      <c r="A3" s="581"/>
+      <c r="B3" s="583"/>
+      <c r="C3" s="563"/>
+      <c r="D3" s="585"/>
+      <c r="E3" s="629"/>
+      <c r="F3" s="604"/>
       <c r="G3" s="428" t="s">
         <v>28</v>
       </c>
@@ -7749,17 +7747,17 @@
       <c r="L3" s="209" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="583"/>
+      <c r="M3" s="604"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="609"/>
+      <c r="O3" s="608"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="573"/>
+      <c r="Q3" s="563"/>
       <c r="R3" s="536"/>
-      <c r="S3" s="597"/>
+      <c r="S3" s="621"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7776,7 +7774,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="592" t="s">
+      <c r="AD3" s="619" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="266"/>
@@ -7788,16 +7786,16 @@
       <c r="AK3" s="266"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="462"/>
-      <c r="AN3" s="602"/>
+      <c r="AN3" s="599"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="641" t="s">
+      <c r="B4" s="596" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="572" t="s">
+      <c r="C4" s="562" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="368" t="s">
@@ -7806,7 +7804,7 @@
       <c r="E4" s="405">
         <v>1</v>
       </c>
-      <c r="F4" s="583"/>
+      <c r="F4" s="604"/>
       <c r="G4" s="409" t="s">
         <v>203</v>
       </c>
@@ -7823,11 +7821,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="212"/>
-      <c r="M4" s="583"/>
+      <c r="M4" s="604"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="609"/>
+      <c r="O4" s="608"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7854,7 +7852,7 @@
       <c r="AA4" s="318"/>
       <c r="AB4" s="217"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="592"/>
+      <c r="AD4" s="619"/>
       <c r="AE4" s="266"/>
       <c r="AF4" s="266"/>
       <c r="AG4" s="16"/>
@@ -7864,37 +7862,37 @@
       <c r="AK4" s="266"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="462"/>
-      <c r="AN4" s="602"/>
+      <c r="AN4" s="599"/>
       <c r="AO4" s="359" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="570" t="s">
+      <c r="A5" s="560" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="642"/>
-      <c r="C5" s="573"/>
+      <c r="B5" s="597"/>
+      <c r="C5" s="563"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="406">
         <v>1</v>
       </c>
-      <c r="F5" s="583"/>
-      <c r="G5" s="633" t="s">
+      <c r="F5" s="604"/>
+      <c r="G5" s="588" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="633"/>
-      <c r="I5" s="633"/>
-      <c r="J5" s="633"/>
-      <c r="K5" s="633"/>
-      <c r="L5" s="634"/>
-      <c r="M5" s="583"/>
+      <c r="H5" s="588"/>
+      <c r="I5" s="588"/>
+      <c r="J5" s="588"/>
+      <c r="K5" s="588"/>
+      <c r="L5" s="589"/>
+      <c r="M5" s="604"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="609"/>
+      <c r="O5" s="608"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7925,24 +7923,24 @@
       <c r="AK5" s="266"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="462"/>
-      <c r="AN5" s="602"/>
+      <c r="AN5" s="599"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="571"/>
-      <c r="B6" s="639" t="s">
+      <c r="A6" s="561"/>
+      <c r="B6" s="594" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="568"/>
-      <c r="D6" s="569"/>
-      <c r="F6" s="583"/>
-      <c r="G6" s="635"/>
-      <c r="H6" s="635"/>
-      <c r="I6" s="635"/>
-      <c r="J6" s="635"/>
-      <c r="K6" s="635"/>
-      <c r="L6" s="636"/>
-      <c r="M6" s="583"/>
-      <c r="O6" s="609"/>
+      <c r="C6" s="558"/>
+      <c r="D6" s="559"/>
+      <c r="F6" s="604"/>
+      <c r="G6" s="590"/>
+      <c r="H6" s="590"/>
+      <c r="I6" s="590"/>
+      <c r="J6" s="590"/>
+      <c r="K6" s="590"/>
+      <c r="L6" s="591"/>
+      <c r="M6" s="604"/>
+      <c r="O6" s="608"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7966,25 +7964,25 @@
       <c r="AF6" s="266"/>
       <c r="AG6" s="266"/>
       <c r="AH6" s="266"/>
-      <c r="AI6" s="591"/>
+      <c r="AI6" s="613"/>
       <c r="AJ6" s="475" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="591" t="s">
+      <c r="AK6" s="613" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="266"/>
       <c r="AM6" s="462"/>
-      <c r="AN6" s="602"/>
+      <c r="AN6" s="599"/>
       <c r="AO6" s="359" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="241" t="s">
-        <v>601</v>
-      </c>
-      <c r="B7" s="640"/>
+        <v>600</v>
+      </c>
+      <c r="B7" s="595"/>
       <c r="C7" s="210" t="s">
         <v>383</v>
       </c>
@@ -7994,7 +7992,7 @@
       <c r="E7" s="275">
         <v>0</v>
       </c>
-      <c r="F7" s="583"/>
+      <c r="F7" s="604"/>
       <c r="G7" s="429">
         <v>3</v>
       </c>
@@ -8005,7 +8003,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="534">
         <v>1</v>
@@ -8013,8 +8011,8 @@
       <c r="L7" s="220">
         <v>0</v>
       </c>
-      <c r="M7" s="583"/>
-      <c r="O7" s="609"/>
+      <c r="M7" s="604"/>
+      <c r="O7" s="608"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8038,18 +8036,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="266"/>
       <c r="AF7" s="266"/>
-      <c r="AG7" s="592" t="s">
+      <c r="AG7" s="619" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="266"/>
-      <c r="AI7" s="591"/>
+      <c r="AI7" s="613"/>
       <c r="AJ7" s="266"/>
-      <c r="AK7" s="591"/>
+      <c r="AK7" s="613"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="462"/>
-      <c r="AN7" s="602"/>
+      <c r="AN7" s="599"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8064,29 +8062,29 @@
       <c r="D8" s="358"/>
       <c r="E8" s="253">
         <f>SUM(G7:N9)</f>
-        <v>19</v>
-      </c>
-      <c r="F8" s="583"/>
-      <c r="G8" s="634">
-        <v>0</v>
-      </c>
-      <c r="H8" s="631" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="604"/>
+      <c r="G8" s="589">
+        <v>2</v>
+      </c>
+      <c r="H8" s="586" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="534">
         <v>0</v>
       </c>
-      <c r="J8" s="631" t="s">
+      <c r="J8" s="586" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="637"/>
-      <c r="L8" s="593"/>
-      <c r="M8" s="606"/>
-      <c r="N8" s="598">
+      <c r="K8" s="592"/>
+      <c r="L8" s="622"/>
+      <c r="M8" s="605"/>
+      <c r="N8" s="625">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="609"/>
+      <c r="O8" s="608"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8104,18 +8102,18 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="266"/>
       <c r="AF8" s="266"/>
-      <c r="AG8" s="592"/>
+      <c r="AG8" s="619"/>
       <c r="AH8" s="266"/>
-      <c r="AI8" s="591"/>
+      <c r="AI8" s="613"/>
       <c r="AJ8" s="266"/>
       <c r="AK8" s="266"/>
       <c r="AL8" s="266"/>
       <c r="AM8" s="462"/>
-      <c r="AN8" s="602"/>
+      <c r="AN8" s="599"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="241" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B9" s="106" t="s">
         <v>197</v>
@@ -8126,17 +8124,17 @@
       <c r="D9" s="369" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="583"/>
-      <c r="G9" s="636"/>
-      <c r="H9" s="632"/>
+      <c r="F9" s="604"/>
+      <c r="G9" s="591"/>
+      <c r="H9" s="587"/>
       <c r="I9" s="536"/>
-      <c r="J9" s="632"/>
-      <c r="K9" s="638"/>
-      <c r="L9" s="594"/>
-      <c r="M9" s="607"/>
-      <c r="N9" s="599"/>
-      <c r="O9" s="610"/>
-      <c r="S9" s="595" t="s">
+      <c r="J9" s="587"/>
+      <c r="K9" s="593"/>
+      <c r="L9" s="623"/>
+      <c r="M9" s="606"/>
+      <c r="N9" s="626"/>
+      <c r="O9" s="609"/>
+      <c r="S9" s="620" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8158,23 +8156,23 @@
       </c>
       <c r="AE9" s="266"/>
       <c r="AF9" s="266"/>
-      <c r="AG9" s="592"/>
+      <c r="AG9" s="619"/>
       <c r="AH9" s="266"/>
-      <c r="AI9" s="591"/>
+      <c r="AI9" s="613"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="591" t="s">
+      <c r="AK9" s="613" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="266"/>
       <c r="AM9" s="462"/>
-      <c r="AN9" s="602"/>
+      <c r="AN9" s="599"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="241" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B10" s="105" t="s">
         <v>199</v>
@@ -8182,22 +8180,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="246">
         <f>Boat!U8</f>
-        <v>37</v>
-      </c>
-      <c r="F10" s="583"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="604"/>
       <c r="N10" s="452" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="585" t="s">
+      <c r="O10" s="637" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="611" t="s">
+      <c r="P10" s="610" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="596"/>
+      <c r="S10" s="624"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8227,16 +8225,16 @@
       <c r="AF10" s="247" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="592"/>
+      <c r="AG10" s="619"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="591"/>
+      <c r="AI10" s="613"/>
       <c r="AJ10" s="266"/>
-      <c r="AK10" s="591"/>
+      <c r="AK10" s="613"/>
       <c r="AL10" s="266"/>
       <c r="AM10" s="476" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="602"/>
+      <c r="AN10" s="599"/>
       <c r="AO10" s="212" t="s">
         <v>95</v>
       </c>
@@ -8254,18 +8252,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="583"/>
+      <c r="F11" s="604"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="586"/>
-      <c r="P11" s="612"/>
+      <c r="O11" s="638"/>
+      <c r="P11" s="611"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="596"/>
+      <c r="S11" s="624"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8289,14 +8287,14 @@
       <c r="AF11" s="266" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="592"/>
+      <c r="AG11" s="619"/>
       <c r="AH11" s="266"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="266"/>
       <c r="AK11" s="266"/>
       <c r="AL11" s="266"/>
       <c r="AM11" s="462"/>
-      <c r="AN11" s="602"/>
+      <c r="AN11" s="599"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8313,9 +8311,9 @@
         <v>154</v>
       </c>
       <c r="E12" s="233">
-        <v>3</v>
-      </c>
-      <c r="F12" s="583"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="604"/>
       <c r="G12" s="358" t="s">
         <v>411</v>
       </c>
@@ -8324,16 +8322,16 @@
       </c>
       <c r="I12" s="541"/>
       <c r="J12" s="541"/>
-      <c r="K12" s="590"/>
+      <c r="K12" s="642"/>
       <c r="L12" s="211"/>
       <c r="M12" s="211"/>
       <c r="N12" s="211"/>
-      <c r="O12" s="586"/>
-      <c r="P12" s="612"/>
+      <c r="O12" s="638"/>
+      <c r="P12" s="611"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="597"/>
+      <c r="S12" s="621"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8354,16 +8352,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="600" t="s">
+      <c r="AD12" s="627" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="475" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="592" t="s">
+      <c r="AF12" s="619" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="592"/>
+      <c r="AG12" s="619"/>
       <c r="AH12" s="247" t="s">
         <v>264</v>
       </c>
@@ -8376,7 +8374,7 @@
       <c r="AM12" s="614" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="602"/>
+      <c r="AN12" s="599"/>
       <c r="AO12" s="359" t="s">
         <v>97</v>
       </c>
@@ -8388,17 +8386,17 @@
       <c r="E13" s="482">
         <v>-3</v>
       </c>
-      <c r="F13" s="583"/>
+      <c r="F13" s="604"/>
       <c r="G13" s="541" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="541"/>
       <c r="I13" s="541"/>
-      <c r="J13" s="590"/>
+      <c r="J13" s="642"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="586"/>
-      <c r="P13" s="613"/>
+      <c r="O13" s="638"/>
+      <c r="P13" s="612"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8419,8 +8417,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="600"/>
-      <c r="AF13" s="592"/>
+      <c r="AD13" s="627"/>
+      <c r="AF13" s="619"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="247" t="s">
         <v>314</v>
@@ -8432,7 +8430,7 @@
       <c r="AK13" s="266"/>
       <c r="AL13" s="266"/>
       <c r="AM13" s="614"/>
-      <c r="AN13" s="602"/>
+      <c r="AN13" s="599"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="484"/>
@@ -8440,18 +8438,18 @@
       <c r="C14" s="493"/>
       <c r="D14" s="486"/>
       <c r="E14" s="487"/>
-      <c r="F14" s="583"/>
+      <c r="F14" s="604"/>
       <c r="G14" s="541" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="541"/>
       <c r="I14" s="541"/>
-      <c r="J14" s="590"/>
+      <c r="J14" s="642"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="586"/>
+      <c r="O14" s="638"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8472,9 +8470,9 @@
       <c r="AA14" s="318"/>
       <c r="AB14" s="217"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="600"/>
+      <c r="AD14" s="627"/>
       <c r="AE14" s="266"/>
-      <c r="AF14" s="592"/>
+      <c r="AF14" s="619"/>
       <c r="AG14" s="266"/>
       <c r="AH14" s="266"/>
       <c r="AI14" s="70"/>
@@ -8482,7 +8480,7 @@
       <c r="AK14" s="266"/>
       <c r="AL14" s="266"/>
       <c r="AM14" s="614"/>
-      <c r="AN14" s="602"/>
+      <c r="AN14" s="599"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="483" t="s">
@@ -8491,8 +8489,8 @@
       <c r="C15" s="534" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="583"/>
-      <c r="O15" s="586"/>
+      <c r="F15" s="604"/>
+      <c r="O15" s="638"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8514,8 +8512,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="600"/>
-      <c r="AF15" s="592"/>
+      <c r="AD15" s="627"/>
+      <c r="AF15" s="619"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="247" t="s">
         <v>466</v>
@@ -8529,7 +8527,7 @@
       <c r="AK15" s="266"/>
       <c r="AL15" s="266"/>
       <c r="AM15" s="614"/>
-      <c r="AN15" s="602"/>
+      <c r="AN15" s="599"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8551,13 +8549,13 @@
       <c r="E16" s="233">
         <v>1</v>
       </c>
-      <c r="F16" s="583"/>
+      <c r="F16" s="604"/>
       <c r="G16" s="358" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="505"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="586"/>
+      <c r="O16" s="638"/>
       <c r="R16" s="469" t="s">
         <v>185</v>
       </c>
@@ -8589,18 +8587,18 @@
       <c r="AM16" s="462" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="602"/>
+      <c r="AN16" s="599"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="583"/>
+      <c r="F17" s="604"/>
       <c r="I17" s="506"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="586"/>
+      <c r="O17" s="638"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8645,7 +8643,7 @@
       <c r="AK17" s="266"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="462"/>
-      <c r="AN17" s="602"/>
+      <c r="AN17" s="599"/>
       <c r="AO17" s="212" t="s">
         <v>516</v>
       </c>
@@ -8655,7 +8653,7 @@
     </row>
     <row r="18" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="499" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>559</v>
@@ -8669,21 +8667,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="583"/>
+      <c r="F18" s="604"/>
       <c r="G18" s="358" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="586"/>
+      <c r="O18" s="638"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="578" t="s">
+      <c r="R18" s="632" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="622" t="s">
+      <c r="U18" s="577" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8704,7 +8702,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="266"/>
-      <c r="AF18" s="591" t="s">
+      <c r="AF18" s="613" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="266"/>
@@ -8716,20 +8714,20 @@
       <c r="AK18" s="266"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="462"/>
-      <c r="AN18" s="602"/>
+      <c r="AN18" s="599"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="583"/>
+      <c r="F19" s="604"/>
       <c r="I19" s="228"/>
-      <c r="O19" s="586"/>
-      <c r="R19" s="579"/>
+      <c r="O19" s="638"/>
+      <c r="R19" s="633"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="623"/>
+      <c r="U19" s="578"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="465" t="s">
@@ -8744,7 +8742,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="266"/>
-      <c r="AF19" s="591"/>
+      <c r="AF19" s="613"/>
       <c r="AG19" s="266"/>
       <c r="AH19" s="266"/>
       <c r="AI19" s="70"/>
@@ -8754,7 +8752,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="462"/>
-      <c r="AN19" s="602"/>
+      <c r="AN19" s="599"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8775,19 +8773,19 @@
       <c r="E20" s="471">
         <v>-1</v>
       </c>
-      <c r="F20" s="583"/>
+      <c r="F20" s="604"/>
       <c r="G20" s="358" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="228"/>
-      <c r="O20" s="586"/>
-      <c r="Q20" s="588" t="s">
+      <c r="O20" s="638"/>
+      <c r="Q20" s="640" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="438" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="624"/>
+      <c r="U20" s="579"/>
       <c r="W20" s="439"/>
       <c r="X20" s="466" t="s">
         <v>175</v>
@@ -8817,7 +8815,7 @@
       <c r="AM20" s="409" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="602"/>
+      <c r="AN20" s="599"/>
       <c r="AO20" s="359" t="s">
         <v>478</v>
       </c>
@@ -8841,13 +8839,13 @@
       <c r="E21" s="275">
         <v>1</v>
       </c>
-      <c r="F21" s="583"/>
+      <c r="F21" s="604"/>
       <c r="I21" s="228"/>
-      <c r="O21" s="586"/>
-      <c r="Q21" s="589"/>
+      <c r="O21" s="638"/>
+      <c r="Q21" s="641"/>
       <c r="T21" s="456"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="619"/>
+      <c r="V21" s="574"/>
       <c r="W21" s="460" t="s">
         <v>176</v>
       </c>
@@ -8885,15 +8883,15 @@
       <c r="AM21" s="462" t="s">
         <v>568</v>
       </c>
-      <c r="AN21" s="602"/>
+      <c r="AN21" s="599"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="583"/>
+      <c r="F22" s="604"/>
       <c r="G22" s="358" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="228"/>
-      <c r="O22" s="586"/>
+      <c r="O22" s="638"/>
       <c r="R22" s="468" t="s">
         <v>44</v>
       </c>
@@ -8901,7 +8899,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="620"/>
+      <c r="V22" s="575"/>
       <c r="W22" s="460" t="s">
         <v>176</v>
       </c>
@@ -8919,7 +8917,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="591" t="s">
+      <c r="AJ22" s="613" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="266"/>
@@ -8927,7 +8925,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="311"/>
-      <c r="AN22" s="602"/>
+      <c r="AN22" s="599"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="240" t="s">
@@ -8945,17 +8943,17 @@
       <c r="E23" s="234">
         <v>1</v>
       </c>
-      <c r="F23" s="583"/>
+      <c r="F23" s="604"/>
       <c r="I23" s="228"/>
-      <c r="O23" s="586"/>
-      <c r="Q23" s="588" t="s">
+      <c r="O23" s="638"/>
+      <c r="Q23" s="640" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="454" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="620"/>
+      <c r="V23" s="575"/>
       <c r="W23" s="148"/>
       <c r="X23" s="463" t="s">
         <v>189</v>
@@ -8971,13 +8969,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="591"/>
+      <c r="AJ23" s="613"/>
       <c r="AK23" s="266"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="311"/>
-      <c r="AN23" s="602"/>
+      <c r="AN23" s="599"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="474" t="s">
@@ -8995,18 +8993,18 @@
       <c r="E24" s="470">
         <v>1</v>
       </c>
-      <c r="F24" s="583"/>
+      <c r="F24" s="604"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="228"/>
-      <c r="O24" s="586"/>
-      <c r="Q24" s="589"/>
+      <c r="O24" s="638"/>
+      <c r="Q24" s="641"/>
       <c r="T24" s="17"/>
       <c r="U24" s="236" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="620"/>
+      <c r="V24" s="575"/>
       <c r="W24" s="148"/>
       <c r="X24" s="463" t="s">
         <v>186</v>
@@ -9030,12 +9028,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="311"/>
-      <c r="AN24" s="602"/>
+      <c r="AN24" s="599"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="583"/>
+      <c r="F25" s="604"/>
       <c r="I25" s="228"/>
-      <c r="O25" s="586"/>
+      <c r="O25" s="638"/>
       <c r="P25" s="212" t="s">
         <v>285</v>
       </c>
@@ -9048,7 +9046,7 @@
       <c r="U25" s="434" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="621"/>
+      <c r="V25" s="576"/>
       <c r="W25" s="148"/>
       <c r="X25" s="463" t="s">
         <v>190</v>
@@ -9070,7 +9068,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="311"/>
-      <c r="AN25" s="602"/>
+      <c r="AN25" s="599"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="240" t="s">
@@ -9088,17 +9086,17 @@
       <c r="E26" s="407">
         <v>1</v>
       </c>
-      <c r="F26" s="583"/>
+      <c r="F26" s="604"/>
       <c r="G26" s="358" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="228"/>
-      <c r="O26" s="586"/>
-      <c r="P26" s="604" t="s">
+      <c r="O26" s="638"/>
+      <c r="P26" s="601" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="605"/>
-      <c r="R26" s="580" t="s">
+      <c r="Q26" s="602"/>
+      <c r="R26" s="634" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="183"/>
@@ -9137,7 +9135,7 @@
       <c r="AM26" s="476" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="602"/>
+      <c r="AN26" s="599"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9149,13 +9147,13 @@
       <c r="E27" s="275" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="584"/>
+      <c r="F27" s="636"/>
       <c r="G27" s="61" t="s">
         <v>567</v>
       </c>
       <c r="I27" s="229"/>
-      <c r="O27" s="587"/>
-      <c r="R27" s="581"/>
+      <c r="O27" s="639"/>
+      <c r="R27" s="635"/>
       <c r="S27" s="455" t="s">
         <v>54</v>
       </c>
@@ -9185,10 +9183,48 @@
       <c r="AM27" s="409" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="603"/>
+      <c r="AN27" s="600"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9205,44 +9241,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9252,8 +9250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9315,7 +9313,7 @@
         <v>0</v>
       </c>
       <c r="H1" s="71" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I1" s="21"/>
       <c r="J1" s="95" t="s">
@@ -9341,15 +9339,15 @@
       </c>
       <c r="R1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
+        <v>45278</v>
       </c>
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="646" t="s">
+      <c r="V1" s="649" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="647"/>
+      <c r="W1" s="650"/>
       <c r="X1" s="317">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9365,21 +9363,21 @@
       <c r="AB1" s="313" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="648" t="s">
+      <c r="AC1" s="651" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="649"/>
-      <c r="AE1" s="650"/>
-      <c r="AF1" s="651" t="s">
+      <c r="AD1" s="652"/>
+      <c r="AE1" s="653"/>
+      <c r="AF1" s="654" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="652"/>
-      <c r="AH1" s="653"/>
-      <c r="AI1" s="643" t="s">
+      <c r="AG1" s="655"/>
+      <c r="AH1" s="656"/>
+      <c r="AI1" s="646" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="644"/>
-      <c r="AK1" s="645"/>
+      <c r="AJ1" s="647"/>
+      <c r="AK1" s="648"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9396,19 +9394,19 @@
       <c r="K2" s="336">
         <v>-3</v>
       </c>
-      <c r="L2" s="654">
+      <c r="L2" s="657">
         <f>SUM(L5:L30)</f>
-        <v>4</v>
-      </c>
-      <c r="M2" s="656">
+        <v>6</v>
+      </c>
+      <c r="M2" s="659">
         <f>SUM(M4:M29)</f>
-        <v>10</v>
-      </c>
-      <c r="N2" s="658">
+        <v>11</v>
+      </c>
+      <c r="N2" s="661">
         <f>SUM(N4:N29)</f>
         <v>7</v>
       </c>
-      <c r="O2" s="598">
+      <c r="O2" s="625">
         <f>SUM(M30:M37)* (-1)</f>
         <v>1</v>
       </c>
@@ -9427,7 +9425,7 @@
       <c r="T2" s="66" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="660" t="s">
+      <c r="U2" s="663" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="61" t="s">
@@ -9496,10 +9494,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="655"/>
-      <c r="M3" s="657"/>
-      <c r="N3" s="659"/>
-      <c r="O3" s="599"/>
+      <c r="L3" s="658"/>
+      <c r="M3" s="660"/>
+      <c r="N3" s="662"/>
+      <c r="O3" s="626"/>
       <c r="P3" s="177">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9513,16 +9511,16 @@
       </c>
       <c r="T3" s="301">
         <f>SUM(T4:T29)</f>
-        <v>37</v>
-      </c>
-      <c r="U3" s="661"/>
+        <v>36</v>
+      </c>
+      <c r="U3" s="664"/>
       <c r="V3" s="159">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9534,7 +9532,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9542,11 +9540,11 @@
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -9562,7 +9560,7 @@
       </c>
       <c r="AG3" s="395">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
@@ -9614,7 +9612,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="662" t="s">
+      <c r="O4" s="643" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9678,9 +9676,7 @@
       <c r="AL4" s="326" t="s">
         <v>204</v>
       </c>
-      <c r="AM4" s="19" t="s">
-        <v>586</v>
-      </c>
+      <c r="AM4" s="19"/>
       <c r="AN4" s="142" t="s">
         <v>579</v>
       </c>
@@ -9695,7 +9691,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="663"/>
+      <c r="O5" s="644"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9774,16 +9770,16 @@
         <v>312</v>
       </c>
       <c r="L6" s="345">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="304">
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="663"/>
+      <c r="O6" s="644"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9794,17 +9790,17 @@
         <v>2</v>
       </c>
       <c r="T6" s="334">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6" s="327">
         <v>-2</v>
       </c>
       <c r="V6" s="332">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W6" s="190">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X6" s="307"/>
       <c r="Y6" s="117">
@@ -9813,7 +9809,7 @@
       </c>
       <c r="Z6" s="301">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA6" s="301">
         <v>0</v>
@@ -9848,7 +9844,9 @@
         <v>0</v>
       </c>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="19"/>
+      <c r="AM6" s="19" t="s">
+        <v>586</v>
+      </c>
       <c r="AN6" s="266"/>
     </row>
     <row r="7" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9873,7 +9871,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="663"/>
+      <c r="O7" s="644"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -9977,7 +9975,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="663"/>
+      <c r="O8" s="644"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9995,7 +9993,7 @@
       </c>
       <c r="U8" s="528">
         <f>T3</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V8" s="332">
         <v>0</v>
@@ -10061,7 +10059,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="663"/>
+      <c r="O9" s="644"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10157,7 +10155,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="663"/>
+      <c r="O10" s="644"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10238,7 +10236,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="663"/>
+      <c r="O11" s="644"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10298,7 +10296,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="634" t="s">
+      <c r="A12" s="589" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10307,7 +10305,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="588" t="s">
+      <c r="E12" s="640" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="271">
@@ -10331,7 +10329,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O12" s="663"/>
+      <c r="O12" s="644"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10403,14 +10401,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="636"/>
+      <c r="A13" s="591"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="589"/>
+      <c r="E13" s="641"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10433,7 +10431,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="663"/>
+      <c r="O13" s="644"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10506,7 +10504,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="663"/>
+      <c r="O14" s="644"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="208" t="s">
         <v>346</v>
@@ -10542,10 +10540,10 @@
       </c>
       <c r="AB14" s="301">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AC14" s="305">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD14" s="311"/>
       <c r="AE14" s="307"/>
@@ -10554,7 +10552,7 @@
         <v>1</v>
       </c>
       <c r="AG14" s="357">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH14" s="158"/>
       <c r="AI14" s="319">
@@ -10603,7 +10601,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O15" s="663"/>
+      <c r="O15" s="644"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="208" t="s">
         <v>346</v>
@@ -10686,7 +10684,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="663"/>
+      <c r="O16" s="644"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10782,7 +10780,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="663"/>
+      <c r="O17" s="644"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10865,7 +10863,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="663"/>
+      <c r="O18" s="644"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10944,7 +10942,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="663"/>
+      <c r="O19" s="644"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11040,11 +11038,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O20" s="664"/>
+      <c r="O20" s="645"/>
       <c r="P20" s="539" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="590"/>
+      <c r="Q20" s="642"/>
       <c r="R20" s="327" t="s">
         <v>86</v>
       </c>
@@ -11285,7 +11283,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="641" t="s">
+      <c r="E23" s="596" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -11377,7 +11375,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="642"/>
+      <c r="E24" s="597"/>
       <c r="F24" s="177"/>
       <c r="K24" s="412" t="s">
         <v>301</v>
@@ -11395,7 +11393,7 @@
       <c r="P24" s="539" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="590"/>
+      <c r="Q24" s="642"/>
       <c r="R24" s="327" t="s">
         <v>254</v>
       </c>
@@ -12457,12 +12455,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12472,6 +12464,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12508,12 +12506,12 @@
       <c r="B1" s="539" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="590"/>
+      <c r="C1" s="642"/>
       <c r="D1" s="212"/>
       <c r="J1" s="539" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="590"/>
+      <c r="K1" s="642"/>
       <c r="L1" s="203" t="s">
         <v>337</v>
       </c>
@@ -12899,12 +12897,12 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
+        <v>45278</v>
       </c>
       <c r="V1" s="539" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="590"/>
+      <c r="W1" s="642"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12923,7 +12921,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="678" t="s">
+      <c r="AD1" s="685" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12940,10 +12938,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="677" t="s">
+      <c r="F2" s="716" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="705" t="s">
+      <c r="G2" s="673" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12971,10 +12969,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="646" t="s">
+      <c r="V2" s="649" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="647"/>
+      <c r="W2" s="650"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12993,7 +12991,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="679"/>
+      <c r="AD2" s="686"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13012,8 +13010,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="638"/>
-      <c r="G3" s="706"/>
+      <c r="F3" s="593"/>
+      <c r="G3" s="674"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13024,13 +13022,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="715" t="s">
+      <c r="O3" s="683" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="697" t="s">
+      <c r="P3" s="704" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="698"/>
+      <c r="Q3" s="705"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13040,15 +13038,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="679"/>
+      <c r="AD3" s="686"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="706"/>
+      <c r="G4" s="674"/>
       <c r="H4" s="6"/>
       <c r="L4" s="668" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="716"/>
+      <c r="O4" s="684"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13062,8 +13060,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="541"/>
-      <c r="AA4" s="590"/>
-      <c r="AD4" s="679"/>
+      <c r="AA4" s="642"/>
+      <c r="AD4" s="686"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13078,21 +13076,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="706"/>
+      <c r="G5" s="674"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="684" t="s">
+      <c r="K5" s="691" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="699"/>
+      <c r="L5" s="706"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="716"/>
+      <c r="O5" s="684"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13108,11 +13106,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="687" t="s">
+      <c r="Y5" s="694" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="688"/>
-      <c r="AD5" s="679"/>
+      <c r="Z5" s="695"/>
+      <c r="AD5" s="686"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13122,16 +13120,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="706"/>
+      <c r="G6" s="674"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="685"/>
-      <c r="L6" s="699"/>
-      <c r="O6" s="716"/>
+      <c r="K6" s="692"/>
+      <c r="L6" s="706"/>
+      <c r="O6" s="684"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13141,23 +13139,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="679"/>
+      <c r="AD6" s="686"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="706"/>
+      <c r="G7" s="674"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="685"/>
-      <c r="L7" s="699"/>
+      <c r="K7" s="692"/>
+      <c r="L7" s="706"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="716"/>
+      <c r="O7" s="684"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="679"/>
+      <c r="AD7" s="686"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13170,7 +13168,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="706"/>
+      <c r="G8" s="674"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13180,41 +13178,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="685"/>
-      <c r="L8" s="699"/>
-      <c r="O8" s="716"/>
+      <c r="K8" s="692"/>
+      <c r="L8" s="706"/>
+      <c r="O8" s="684"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="681" t="s">
+      <c r="S8" s="688" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="682"/>
-      <c r="U8" s="682"/>
-      <c r="V8" s="682"/>
-      <c r="W8" s="682"/>
-      <c r="X8" s="682"/>
-      <c r="Y8" s="682"/>
-      <c r="Z8" s="682"/>
-      <c r="AA8" s="682"/>
-      <c r="AB8" s="682"/>
-      <c r="AC8" s="683"/>
-      <c r="AD8" s="679"/>
+      <c r="T8" s="689"/>
+      <c r="U8" s="689"/>
+      <c r="V8" s="689"/>
+      <c r="W8" s="689"/>
+      <c r="X8" s="689"/>
+      <c r="Y8" s="689"/>
+      <c r="Z8" s="689"/>
+      <c r="AA8" s="689"/>
+      <c r="AB8" s="689"/>
+      <c r="AC8" s="690"/>
+      <c r="AD8" s="686"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="671"/>
-      <c r="G9" s="706"/>
+      <c r="C9" s="710"/>
+      <c r="G9" s="674"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="685"/>
-      <c r="L9" s="709" t="s">
+      <c r="K9" s="692"/>
+      <c r="L9" s="677" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="710"/>
-      <c r="N9" s="711"/>
-      <c r="O9" s="716"/>
+      <c r="M9" s="678"/>
+      <c r="N9" s="679"/>
+      <c r="O9" s="684"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="679"/>
+      <c r="AD9" s="686"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="672"/>
+      <c r="C10" s="711"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13222,7 +13220,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="706"/>
+      <c r="G10" s="674"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13230,33 +13228,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="685"/>
-      <c r="M10" s="674" t="s">
+      <c r="K10" s="692"/>
+      <c r="M10" s="713" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="675"/>
-      <c r="O10" s="675"/>
-      <c r="P10" s="675"/>
-      <c r="Q10" s="675"/>
-      <c r="R10" s="675"/>
-      <c r="S10" s="675"/>
-      <c r="T10" s="675"/>
-      <c r="U10" s="675"/>
-      <c r="V10" s="675"/>
-      <c r="W10" s="675"/>
-      <c r="X10" s="675"/>
-      <c r="Y10" s="675"/>
-      <c r="Z10" s="675"/>
-      <c r="AA10" s="675"/>
-      <c r="AB10" s="675"/>
-      <c r="AC10" s="676"/>
-      <c r="AD10" s="679"/>
+      <c r="N10" s="714"/>
+      <c r="O10" s="714"/>
+      <c r="P10" s="714"/>
+      <c r="Q10" s="714"/>
+      <c r="R10" s="714"/>
+      <c r="S10" s="714"/>
+      <c r="T10" s="714"/>
+      <c r="U10" s="714"/>
+      <c r="V10" s="714"/>
+      <c r="W10" s="714"/>
+      <c r="X10" s="714"/>
+      <c r="Y10" s="714"/>
+      <c r="Z10" s="714"/>
+      <c r="AA10" s="714"/>
+      <c r="AB10" s="714"/>
+      <c r="AC10" s="715"/>
+      <c r="AD10" s="686"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="673"/>
-      <c r="G11" s="706"/>
+      <c r="C11" s="712"/>
+      <c r="G11" s="674"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="685"/>
+      <c r="K11" s="692"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13264,17 +13262,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="695" t="s">
+      <c r="Z11" s="702" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="696"/>
+      <c r="AA11" s="703"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="679"/>
+      <c r="AD11" s="686"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13287,7 +13285,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="706"/>
+      <c r="G12" s="674"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13295,8 +13293,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="685"/>
-      <c r="L12" s="700" t="s">
+      <c r="K12" s="692"/>
+      <c r="L12" s="707" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13327,25 +13325,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="689" t="s">
+      <c r="AA12" s="696" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="690"/>
+      <c r="AB12" s="697"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="679"/>
+      <c r="AD12" s="686"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="671"/>
-      <c r="G13" s="706"/>
-      <c r="K13" s="685"/>
-      <c r="L13" s="701"/>
+      <c r="C13" s="710"/>
+      <c r="G13" s="674"/>
+      <c r="K13" s="692"/>
+      <c r="L13" s="708"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="708" t="s">
+      <c r="Q13" s="676" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="605"/>
+      <c r="R13" s="602"/>
       <c r="S13" s="535"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13354,17 +13352,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="691"/>
-      <c r="AB13" s="692"/>
-      <c r="AD13" s="679"/>
+      <c r="AA13" s="698"/>
+      <c r="AB13" s="699"/>
+      <c r="AD13" s="686"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="673"/>
+      <c r="C14" s="712"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="706"/>
+      <c r="G14" s="674"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13372,8 +13370,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="685"/>
-      <c r="L14" s="701"/>
+      <c r="K14" s="692"/>
+      <c r="L14" s="708"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13394,9 +13392,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="691"/>
-      <c r="AB14" s="692"/>
-      <c r="AD14" s="679"/>
+      <c r="AA14" s="698"/>
+      <c r="AB14" s="699"/>
+      <c r="AD14" s="686"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13411,19 +13409,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="706"/>
+      <c r="G15" s="674"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="685"/>
-      <c r="L15" s="702"/>
-      <c r="Q15" s="708" t="s">
+      <c r="K15" s="692"/>
+      <c r="L15" s="709"/>
+      <c r="Q15" s="676" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="605"/>
+      <c r="R15" s="602"/>
       <c r="S15" s="535"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13432,14 +13430,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="691"/>
-      <c r="AB15" s="692"/>
-      <c r="AD15" s="679"/>
+      <c r="AA15" s="698"/>
+      <c r="AB15" s="699"/>
+      <c r="AD15" s="686"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="706"/>
-      <c r="K16" s="685"/>
+      <c r="G16" s="674"/>
+      <c r="K16" s="692"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13458,24 +13456,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="691"/>
-      <c r="AB16" s="692"/>
-      <c r="AD16" s="679"/>
+      <c r="AA16" s="698"/>
+      <c r="AB16" s="699"/>
+      <c r="AD16" s="686"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="703" t="s">
+      <c r="F17" s="671" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="706"/>
+      <c r="G17" s="674"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="685"/>
+      <c r="K17" s="692"/>
       <c r="S17" s="535"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13483,9 +13481,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="691"/>
-      <c r="AB17" s="692"/>
-      <c r="AD17" s="679"/>
+      <c r="AA17" s="698"/>
+      <c r="AB17" s="699"/>
+      <c r="AD17" s="686"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13495,15 +13493,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="704"/>
-      <c r="G18" s="706"/>
+      <c r="F18" s="672"/>
+      <c r="G18" s="674"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="685"/>
+      <c r="K18" s="692"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13514,42 +13512,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="693"/>
-      <c r="AB18" s="694"/>
-      <c r="AD18" s="679"/>
+      <c r="AA18" s="700"/>
+      <c r="AB18" s="701"/>
+      <c r="AD18" s="686"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="707"/>
-      <c r="K19" s="686"/>
+      <c r="G19" s="675"/>
+      <c r="K19" s="693"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="712" t="s">
+      <c r="R19" s="680" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="713"/>
-      <c r="T19" s="714"/>
+      <c r="S19" s="681"/>
+      <c r="T19" s="682"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="680"/>
+      <c r="AD19" s="687"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13561,11 +13556,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat ReLoaded - TBS News , CNN Turk
Boat ReLoaded - TBS News , CNN Turk
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE4ECAC-6F5B-413B-BE47-84550BEC8E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C98C789-6700-452E-85B2-03D72C243FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -3427,7 +3427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="717">
+  <cellXfs count="718">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4682,6 +4682,9 @@
     <xf numFmtId="0" fontId="30" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4730,6 +4733,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4760,62 +4820,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4841,12 +5006,6 @@
     <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4868,161 +5027,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5081,15 +5093,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5108,25 +5111,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5204,49 +5228,28 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5540,7 +5543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
@@ -5594,10 +5597,10 @@
       <c r="I2" s="425" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="536" t="s">
+      <c r="J2" s="537" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="537"/>
+      <c r="K2" s="538"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5607,14 +5610,14 @@
       <c r="N2" s="370" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="538" t="s">
+      <c r="O2" s="539" t="s">
         <v>385</v>
       </c>
-      <c r="P2" s="539"/>
-      <c r="Q2" s="540"/>
-      <c r="R2" s="540"/>
-      <c r="S2" s="540"/>
-      <c r="T2" s="541" t="s">
+      <c r="P2" s="540"/>
+      <c r="Q2" s="541"/>
+      <c r="R2" s="541"/>
+      <c r="S2" s="541"/>
+      <c r="T2" s="542" t="s">
         <v>386</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5628,7 +5631,7 @@
       <c r="C3" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="533"/>
+      <c r="D3" s="534"/>
       <c r="E3" s="358"/>
       <c r="F3" s="275" t="s">
         <v>69</v>
@@ -5664,7 +5667,7 @@
       <c r="S3" s="177">
         <v>0</v>
       </c>
-      <c r="T3" s="542"/>
+      <c r="T3" s="543"/>
       <c r="U3" s="19" t="s">
         <v>591</v>
       </c>
@@ -5680,7 +5683,7 @@
       <c r="C4" s="169" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="534"/>
+      <c r="D4" s="535"/>
       <c r="E4" s="61"/>
       <c r="F4" s="380" t="s">
         <v>42</v>
@@ -5698,7 +5701,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="327"/>
       <c r="S4" s="6"/>
-      <c r="T4" s="542"/>
+      <c r="T4" s="543"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5707,7 +5710,7 @@
       <c r="C5" s="169" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="535"/>
+      <c r="D5" s="536"/>
       <c r="F5" s="384" t="s">
         <v>42</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>522</v>
       </c>
       <c r="P5" s="516"/>
-      <c r="T5" s="542"/>
+      <c r="T5" s="543"/>
       <c r="U5" s="212" t="s">
         <v>228</v>
       </c>
@@ -5765,7 +5768,7 @@
       <c r="P6" s="516"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="542"/>
+      <c r="T6" s="543"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="217" t="s">
@@ -5796,7 +5799,7 @@
       <c r="P7" s="516"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="6"/>
-      <c r="T7" s="542"/>
+      <c r="T7" s="543"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5825,7 +5828,7 @@
       <c r="P8" s="516"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="542"/>
+      <c r="T8" s="543"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -5859,7 +5862,7 @@
         <v>44</v>
       </c>
       <c r="P9" s="516"/>
-      <c r="T9" s="542"/>
+      <c r="T9" s="543"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -5889,7 +5892,7 @@
         <v>522</v>
       </c>
       <c r="P10" s="516"/>
-      <c r="T10" s="542"/>
+      <c r="T10" s="543"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -5924,7 +5927,7 @@
       <c r="P11" s="516"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="142"/>
-      <c r="T11" s="542"/>
+      <c r="T11" s="543"/>
       <c r="U11" s="212" t="s">
         <v>227</v>
       </c>
@@ -5957,7 +5960,7 @@
       <c r="P12" s="516"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="542"/>
+      <c r="T12" s="543"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="265" t="s">
@@ -5992,11 +5995,11 @@
         <v>522</v>
       </c>
       <c r="P13" s="516"/>
-      <c r="T13" s="542"/>
+      <c r="T13" s="543"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="516"/>
-      <c r="T14" s="542"/>
+      <c r="T14" s="543"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6022,10 +6025,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="530">
+      <c r="M15" s="531">
         <v>45275</v>
       </c>
-      <c r="N15" s="533" t="s">
+      <c r="N15" s="534" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="514" t="s">
@@ -6033,7 +6036,7 @@
       </c>
       <c r="P15" s="516"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="542"/>
+      <c r="T15" s="543"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="496" t="s">
@@ -6059,10 +6062,10 @@
       <c r="L16" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="531"/>
-      <c r="N16" s="534"/>
+      <c r="M16" s="532"/>
+      <c r="N16" s="535"/>
       <c r="P16" s="516"/>
-      <c r="T16" s="542"/>
+      <c r="T16" s="543"/>
     </row>
     <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6090,8 +6093,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="532"/>
-      <c r="N17" s="535"/>
+      <c r="M17" s="533"/>
+      <c r="N17" s="536"/>
       <c r="O17" s="514" t="s">
         <v>44</v>
       </c>
@@ -6107,11 +6110,11 @@
       <c r="S17" s="177">
         <v>0</v>
       </c>
-      <c r="T17" s="542"/>
+      <c r="T17" s="543"/>
     </row>
     <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="516"/>
-      <c r="T18" s="542"/>
+      <c r="T18" s="543"/>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6139,14 +6142,14 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="530">
+      <c r="M19" s="531">
         <v>45275</v>
       </c>
       <c r="N19" s="424" t="s">
         <v>522</v>
       </c>
       <c r="P19" s="516"/>
-      <c r="T19" s="542"/>
+      <c r="T19" s="543"/>
     </row>
     <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="250" t="s">
@@ -6172,12 +6175,12 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="531"/>
+      <c r="M20" s="532"/>
       <c r="N20" s="413" t="s">
         <v>26</v>
       </c>
       <c r="P20" s="516"/>
-      <c r="T20" s="542"/>
+      <c r="T20" s="543"/>
     </row>
     <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="250" t="s">
@@ -6203,16 +6206,16 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="531"/>
+      <c r="M21" s="532"/>
       <c r="N21" s="413" t="s">
         <v>18</v>
       </c>
       <c r="P21" s="516"/>
-      <c r="T21" s="542"/>
-      <c r="U21" s="528" t="s">
+      <c r="T21" s="543"/>
+      <c r="U21" s="529" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="529"/>
+      <c r="V21" s="530"/>
     </row>
     <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="281" t="s">
@@ -6238,12 +6241,12 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="531"/>
+      <c r="M22" s="532"/>
       <c r="N22" s="393" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="516"/>
-      <c r="T22" s="542"/>
+      <c r="T22" s="543"/>
     </row>
     <row r="23" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6269,12 +6272,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="531"/>
+      <c r="M23" s="532"/>
       <c r="N23" s="61" t="s">
         <v>523</v>
       </c>
       <c r="P23" s="516"/>
-      <c r="T23" s="542"/>
+      <c r="T23" s="543"/>
     </row>
     <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -6300,7 +6303,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="531"/>
+      <c r="M24" s="532"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6309,7 +6312,7 @@
       </c>
       <c r="P24" s="517"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="542"/>
+      <c r="T24" s="543"/>
     </row>
     <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6337,7 +6340,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="531"/>
+      <c r="M25" s="532"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6353,7 +6356,7 @@
       <c r="S25" s="21">
         <v>0</v>
       </c>
-      <c r="T25" s="542"/>
+      <c r="T25" s="543"/>
     </row>
     <row r="26" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
@@ -6379,12 +6382,12 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="531"/>
+      <c r="M26" s="532"/>
       <c r="N26" s="61" t="s">
         <v>524</v>
       </c>
       <c r="P26" s="516"/>
-      <c r="T26" s="542"/>
+      <c r="T26" s="543"/>
     </row>
     <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="265" t="s">
@@ -6406,7 +6409,7 @@
       <c r="J27" s="421"/>
       <c r="K27" s="422"/>
       <c r="L27" s="423"/>
-      <c r="M27" s="531"/>
+      <c r="M27" s="532"/>
       <c r="N27" s="61"/>
       <c r="P27" s="327">
         <v>1</v>
@@ -6420,7 +6423,7 @@
       <c r="S27" s="177">
         <v>0</v>
       </c>
-      <c r="T27" s="542"/>
+      <c r="T27" s="543"/>
     </row>
     <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="265" t="s">
@@ -6448,7 +6451,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="532"/>
+      <c r="M28" s="533"/>
       <c r="N28" s="61" t="s">
         <v>524</v>
       </c>
@@ -6464,7 +6467,7 @@
       <c r="S28" s="21">
         <v>0</v>
       </c>
-      <c r="T28" s="543"/>
+      <c r="T28" s="544"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6485,8 +6488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView topLeftCell="H9" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView topLeftCell="H11" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6543,7 +6546,7 @@
       <c r="P1" s="432" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="544" t="s">
+      <c r="Q1" s="564" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6563,32 +6566,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="557">
+      <c r="A2" s="548">
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="B2" s="559" t="s">
+      <c r="B2" s="550" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="571" t="s">
+      <c r="C2" s="562" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="561" t="s">
+      <c r="D2" s="552" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="563" t="s">
+      <c r="E2" s="554" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="199" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="569" t="s">
+      <c r="G2" s="560" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="551" t="s">
+      <c r="I2" s="571" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="430" t="s">
@@ -6612,10 +6615,10 @@
       <c r="P2" s="433">
         <v>40</v>
       </c>
-      <c r="Q2" s="545"/>
+      <c r="Q2" s="565"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
@@ -6638,14 +6641,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="558"/>
-      <c r="B3" s="560"/>
-      <c r="C3" s="572"/>
-      <c r="D3" s="562"/>
-      <c r="E3" s="564"/>
-      <c r="G3" s="570"/>
+      <c r="A3" s="549"/>
+      <c r="B3" s="551"/>
+      <c r="C3" s="563"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="555"/>
+      <c r="G3" s="561"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="552"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6654,7 +6657,7 @@
       </c>
       <c r="Q3" s="508">
         <f>SUM(X24:X30)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="506"/>
@@ -6665,10 +6668,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="252"/>
-      <c r="C4" s="565" t="s">
+      <c r="C4" s="556" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="552"/>
+      <c r="I4" s="572"/>
       <c r="R4" s="508" t="s">
         <v>580</v>
       </c>
@@ -6692,7 +6695,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="566"/>
+      <c r="C5" s="557"/>
       <c r="D5" s="231" t="s">
         <v>103</v>
       </c>
@@ -6702,13 +6705,13 @@
       <c r="F5" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="533" t="s">
+      <c r="G5" s="534" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="552"/>
+      <c r="I5" s="572"/>
       <c r="J5" s="431" t="s">
         <v>273</v>
       </c>
@@ -6734,29 +6737,27 @@
       <c r="U5" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="V5" s="504">
-        <v>1</v>
-      </c>
+      <c r="V5" s="504"/>
       <c r="W5" s="6"/>
       <c r="X5" s="504"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="554" t="s">
+      <c r="A6" s="545" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="567"/>
-      <c r="D6" s="568"/>
+      <c r="C6" s="558"/>
+      <c r="D6" s="559"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="534"/>
-      <c r="I6" s="552"/>
+      <c r="G6" s="535"/>
+      <c r="I6" s="572"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="555"/>
+      <c r="A7" s="546"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6766,8 +6767,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="534"/>
-      <c r="I7" s="552"/>
+      <c r="G7" s="535"/>
+      <c r="I7" s="572"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6785,7 +6786,7 @@
       </c>
       <c r="R7" s="24">
         <f>3-R11</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
@@ -6805,7 +6806,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="556"/>
+      <c r="A8" s="547"/>
       <c r="B8" s="220" t="s">
         <v>28</v>
       </c>
@@ -6813,8 +6814,8 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="534"/>
-      <c r="I8" s="552"/>
+      <c r="G8" s="535"/>
+      <c r="I8" s="572"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6838,9 +6839,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="534"/>
+      <c r="G9" s="535"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="552"/>
+      <c r="I9" s="572"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6864,10 +6865,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>39</v>
-      </c>
-      <c r="G10" s="534"/>
-      <c r="I10" s="552"/>
+        <v>40</v>
+      </c>
+      <c r="G10" s="535"/>
+      <c r="I10" s="572"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6893,7 +6894,7 @@
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="533" t="s">
+      <c r="B11" s="534" t="s">
         <v>392</v>
       </c>
       <c r="C11" s="176" t="s">
@@ -6902,8 +6903,8 @@
       <c r="D11" s="226" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="534"/>
-      <c r="I11" s="552"/>
+      <c r="G11" s="535"/>
+      <c r="I11" s="572"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6924,28 +6925,28 @@
         <v>44</v>
       </c>
       <c r="R11" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="24">
         <v>0</v>
       </c>
-      <c r="U11" s="546" t="s">
+      <c r="U11" s="566" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="547"/>
-      <c r="W11" s="547"/>
-      <c r="X11" s="548"/>
+      <c r="V11" s="567"/>
+      <c r="W11" s="567"/>
+      <c r="X11" s="568"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="236" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="535"/>
+      <c r="B12" s="536"/>
       <c r="E12" s="238">
         <v>3</v>
       </c>
-      <c r="G12" s="534"/>
-      <c r="I12" s="552"/>
+      <c r="G12" s="535"/>
+      <c r="I12" s="572"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -6973,12 +6974,12 @@
       <c r="B13" s="225" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="533" t="s">
+      <c r="C13" s="534" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="534"/>
-      <c r="I13" s="552"/>
+      <c r="G13" s="535"/>
+      <c r="I13" s="572"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7005,7 +7006,7 @@
       <c r="B14" s="178" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="535"/>
+      <c r="C14" s="536"/>
       <c r="D14" s="212" t="s">
         <v>154</v>
       </c>
@@ -7015,11 +7016,11 @@
       <c r="F14" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="535"/>
+      <c r="G14" s="536"/>
       <c r="H14" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="552"/>
+      <c r="I14" s="572"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7037,7 +7038,7 @@
       <c r="H15" s="282">
         <v>0</v>
       </c>
-      <c r="I15" s="552"/>
+      <c r="I15" s="572"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7068,7 +7069,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="552"/>
+      <c r="I16" s="572"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7102,7 +7103,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="552"/>
+      <c r="I17" s="572"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7114,19 +7115,19 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="552"/>
+      <c r="I18" s="572"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="549" t="s">
+      <c r="O18" s="569" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="550"/>
+      <c r="P18" s="570"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
       <c r="R18" s="24">
         <f>5-R26</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
@@ -7146,7 +7147,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="552"/>
+      <c r="I19" s="572"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7174,7 +7175,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="552"/>
+      <c r="I20" s="572"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7197,7 +7198,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="552"/>
+      <c r="I21" s="572"/>
       <c r="M21" s="225" t="s">
         <v>422</v>
       </c>
@@ -7231,7 +7232,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="552"/>
+      <c r="I22" s="572"/>
       <c r="U22" s="6" t="s">
         <v>584</v>
       </c>
@@ -7255,20 +7256,20 @@
       <c r="E23" s="294" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="552"/>
+      <c r="I23" s="572"/>
       <c r="U23" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V23" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="552"/>
+      <c r="I24" s="572"/>
       <c r="U24" s="363"/>
       <c r="V24" s="507">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="W24" s="19" t="s">
         <v>513</v>
@@ -7293,7 +7294,7 @@
       <c r="H25" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="552"/>
+      <c r="I25" s="572"/>
       <c r="J25" s="431" t="s">
         <v>274</v>
       </c>
@@ -7308,13 +7309,13 @@
       </c>
       <c r="U25" s="35"/>
       <c r="V25" s="112">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="W25" s="19" t="s">
-        <v>486</v>
+        <v>74</v>
       </c>
       <c r="X25" s="24">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7338,7 +7339,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="552"/>
+      <c r="I26" s="572"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7353,7 +7354,7 @@
         <v>44</v>
       </c>
       <c r="R26" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="24">
         <v>3</v>
@@ -7373,7 +7374,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="552"/>
+      <c r="I27" s="572"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7400,7 +7401,7 @@
       <c r="E28" s="224">
         <v>2</v>
       </c>
-      <c r="I28" s="552"/>
+      <c r="I28" s="572"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7422,7 +7423,7 @@
       <c r="H29" s="199" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="553"/>
+      <c r="I29" s="573"/>
       <c r="J29" s="342"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7466,6 +7467,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7477,11 +7483,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7557,7 +7558,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="569" t="s">
+      <c r="I1" s="560" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7593,7 +7594,7 @@
       <c r="X1" s="464" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="615" t="s">
+      <c r="Y1" s="616" t="s">
         <v>551</v>
       </c>
       <c r="Z1" s="440">
@@ -7618,7 +7619,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="436"/>
-      <c r="AN1" s="600"/>
+      <c r="AN1" s="598"/>
       <c r="AO1" s="359" t="s">
         <v>487</v>
       </c>
@@ -7627,23 +7628,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="624">
+      <c r="A2" s="580">
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="B2" s="626" t="s">
+      <c r="B2" s="582" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="571" t="s">
+      <c r="C2" s="562" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="628" t="s">
+      <c r="D2" s="584" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="573" t="s">
+      <c r="E2" s="628" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="581" t="s">
+      <c r="F2" s="603" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="427" t="s">
@@ -7652,15 +7653,15 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="570"/>
+      <c r="I2" s="561"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="575" t="s">
+      <c r="K2" s="630" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="576"/>
-      <c r="M2" s="581" t="s">
+      <c r="L2" s="631"/>
+      <c r="M2" s="603" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
@@ -7672,11 +7673,11 @@
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="571" t="s">
+      <c r="Q2" s="562" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="533"/>
-      <c r="S2" s="594" t="s">
+      <c r="R2" s="534"/>
+      <c r="S2" s="620" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7686,7 +7687,7 @@
       <c r="X2" s="465" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="616"/>
+      <c r="Y2" s="617"/>
       <c r="Z2" s="441">
         <v>1</v>
       </c>
@@ -7709,15 +7710,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="462"/>
-      <c r="AN2" s="601"/>
+      <c r="AN2" s="599"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="625"/>
-      <c r="B3" s="627"/>
-      <c r="C3" s="572"/>
-      <c r="D3" s="629"/>
-      <c r="E3" s="574"/>
-      <c r="F3" s="582"/>
+      <c r="A3" s="581"/>
+      <c r="B3" s="583"/>
+      <c r="C3" s="563"/>
+      <c r="D3" s="585"/>
+      <c r="E3" s="629"/>
+      <c r="F3" s="604"/>
       <c r="G3" s="428" t="s">
         <v>28</v>
       </c>
@@ -7736,7 +7737,7 @@
       <c r="L3" s="209" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="582"/>
+      <c r="M3" s="604"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
@@ -7744,9 +7745,9 @@
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="572"/>
-      <c r="R3" s="535"/>
-      <c r="S3" s="596"/>
+      <c r="Q3" s="563"/>
+      <c r="R3" s="536"/>
+      <c r="S3" s="621"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7754,7 +7755,7 @@
       <c r="X3" s="465" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="616"/>
+      <c r="Y3" s="617"/>
       <c r="Z3" s="442">
         <v>1</v>
       </c>
@@ -7763,7 +7764,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="591" t="s">
+      <c r="AD3" s="619" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="266"/>
@@ -7775,16 +7776,16 @@
       <c r="AK3" s="266"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="462"/>
-      <c r="AN3" s="601"/>
+      <c r="AN3" s="599"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="640" t="s">
+      <c r="B4" s="596" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="571" t="s">
+      <c r="C4" s="562" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="368" t="s">
@@ -7793,7 +7794,7 @@
       <c r="E4" s="405">
         <v>2</v>
       </c>
-      <c r="F4" s="582"/>
+      <c r="F4" s="604"/>
       <c r="G4" s="409" t="s">
         <v>203</v>
       </c>
@@ -7810,7 +7811,7 @@
         <v>151</v>
       </c>
       <c r="L4" s="212"/>
-      <c r="M4" s="582"/>
+      <c r="M4" s="604"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
@@ -7836,12 +7837,12 @@
       <c r="X4" s="465" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="616"/>
+      <c r="Y4" s="617"/>
       <c r="Z4" s="443"/>
       <c r="AA4" s="318"/>
       <c r="AB4" s="217"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="591"/>
+      <c r="AD4" s="619"/>
       <c r="AE4" s="266"/>
       <c r="AF4" s="266"/>
       <c r="AG4" s="16"/>
@@ -7851,33 +7852,33 @@
       <c r="AK4" s="266"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="462"/>
-      <c r="AN4" s="601"/>
+      <c r="AN4" s="599"/>
       <c r="AO4" s="359" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="569" t="s">
+      <c r="A5" s="560" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="641"/>
-      <c r="C5" s="572"/>
+      <c r="B5" s="597"/>
+      <c r="C5" s="563"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="406">
         <v>1</v>
       </c>
-      <c r="F5" s="582"/>
-      <c r="G5" s="632" t="s">
+      <c r="F5" s="604"/>
+      <c r="G5" s="588" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="632"/>
-      <c r="I5" s="632"/>
-      <c r="J5" s="632"/>
-      <c r="K5" s="632"/>
-      <c r="L5" s="633"/>
-      <c r="M5" s="582"/>
+      <c r="H5" s="588"/>
+      <c r="I5" s="588"/>
+      <c r="J5" s="588"/>
+      <c r="K5" s="588"/>
+      <c r="L5" s="589"/>
+      <c r="M5" s="604"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
@@ -7889,7 +7890,7 @@
       <c r="X5" s="465" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="616"/>
+      <c r="Y5" s="617"/>
       <c r="Z5" s="443">
         <v>1</v>
       </c>
@@ -7912,23 +7913,23 @@
       <c r="AK5" s="266"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="462"/>
-      <c r="AN5" s="601"/>
+      <c r="AN5" s="599"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="570"/>
-      <c r="B6" s="638" t="s">
+      <c r="A6" s="561"/>
+      <c r="B6" s="594" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="567"/>
-      <c r="D6" s="568"/>
-      <c r="F6" s="582"/>
-      <c r="G6" s="634"/>
-      <c r="H6" s="634"/>
-      <c r="I6" s="634"/>
-      <c r="J6" s="634"/>
-      <c r="K6" s="634"/>
-      <c r="L6" s="635"/>
-      <c r="M6" s="582"/>
+      <c r="C6" s="558"/>
+      <c r="D6" s="559"/>
+      <c r="F6" s="604"/>
+      <c r="G6" s="590"/>
+      <c r="H6" s="590"/>
+      <c r="I6" s="590"/>
+      <c r="J6" s="590"/>
+      <c r="K6" s="590"/>
+      <c r="L6" s="591"/>
+      <c r="M6" s="604"/>
       <c r="O6" s="608"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
@@ -7939,7 +7940,7 @@
       <c r="X6" s="465" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="616"/>
+      <c r="Y6" s="617"/>
       <c r="Z6" s="441">
         <v>1</v>
       </c>
@@ -7953,16 +7954,16 @@
       <c r="AF6" s="266"/>
       <c r="AG6" s="266"/>
       <c r="AH6" s="266"/>
-      <c r="AI6" s="590"/>
+      <c r="AI6" s="613"/>
       <c r="AJ6" s="475" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="590" t="s">
+      <c r="AK6" s="613" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="266"/>
       <c r="AM6" s="462"/>
-      <c r="AN6" s="601"/>
+      <c r="AN6" s="599"/>
       <c r="AO6" s="359" t="s">
         <v>488</v>
       </c>
@@ -7971,7 +7972,7 @@
       <c r="A7" s="241" t="s">
         <v>599</v>
       </c>
-      <c r="B7" s="639"/>
+      <c r="B7" s="595"/>
       <c r="C7" s="210" t="s">
         <v>383</v>
       </c>
@@ -7981,7 +7982,7 @@
       <c r="E7" s="275">
         <v>0</v>
       </c>
-      <c r="F7" s="582"/>
+      <c r="F7" s="604"/>
       <c r="G7" s="429">
         <v>3</v>
       </c>
@@ -7994,13 +7995,13 @@
       <c r="J7" s="30">
         <v>1</v>
       </c>
-      <c r="K7" s="533">
+      <c r="K7" s="534">
         <v>1</v>
       </c>
       <c r="L7" s="220">
         <v>0</v>
       </c>
-      <c r="M7" s="582"/>
+      <c r="M7" s="604"/>
       <c r="O7" s="608"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
@@ -8015,7 +8016,7 @@
       <c r="X7" s="465" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="616"/>
+      <c r="Y7" s="617"/>
       <c r="Z7" s="441">
         <v>1</v>
       </c>
@@ -8025,18 +8026,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="266"/>
       <c r="AF7" s="266"/>
-      <c r="AG7" s="591" t="s">
+      <c r="AG7" s="619" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="266"/>
-      <c r="AI7" s="590"/>
+      <c r="AI7" s="613"/>
       <c r="AJ7" s="266"/>
-      <c r="AK7" s="590"/>
+      <c r="AK7" s="613"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="462"/>
-      <c r="AN7" s="601"/>
+      <c r="AN7" s="599"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8053,23 +8054,23 @@
         <f>SUM(G7:N9)</f>
         <v>22</v>
       </c>
-      <c r="F8" s="582"/>
-      <c r="G8" s="633">
+      <c r="F8" s="604"/>
+      <c r="G8" s="589">
         <v>2</v>
       </c>
-      <c r="H8" s="630" t="s">
+      <c r="H8" s="586" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="533">
-        <v>0</v>
-      </c>
-      <c r="J8" s="630" t="s">
+      <c r="I8" s="534">
+        <v>0</v>
+      </c>
+      <c r="J8" s="586" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="636"/>
-      <c r="L8" s="592"/>
+      <c r="K8" s="592"/>
+      <c r="L8" s="622"/>
       <c r="M8" s="605"/>
-      <c r="N8" s="597">
+      <c r="N8" s="625">
         <f>N5+N11</f>
         <v>15</v>
       </c>
@@ -8083,7 +8084,7 @@
       <c r="X8" s="465" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="616"/>
+      <c r="Y8" s="617"/>
       <c r="Z8" s="443"/>
       <c r="AA8" s="318"/>
       <c r="AB8" s="217"/>
@@ -8091,14 +8092,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="266"/>
       <c r="AF8" s="266"/>
-      <c r="AG8" s="591"/>
+      <c r="AG8" s="619"/>
       <c r="AH8" s="266"/>
-      <c r="AI8" s="590"/>
+      <c r="AI8" s="613"/>
       <c r="AJ8" s="266"/>
       <c r="AK8" s="266"/>
       <c r="AL8" s="266"/>
       <c r="AM8" s="462"/>
-      <c r="AN8" s="601"/>
+      <c r="AN8" s="599"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="241" t="s">
@@ -8113,17 +8114,17 @@
       <c r="D9" s="369" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="582"/>
-      <c r="G9" s="635"/>
-      <c r="H9" s="631"/>
-      <c r="I9" s="535"/>
-      <c r="J9" s="631"/>
-      <c r="K9" s="637"/>
-      <c r="L9" s="593"/>
+      <c r="F9" s="604"/>
+      <c r="G9" s="591"/>
+      <c r="H9" s="587"/>
+      <c r="I9" s="536"/>
+      <c r="J9" s="587"/>
+      <c r="K9" s="593"/>
+      <c r="L9" s="623"/>
       <c r="M9" s="606"/>
-      <c r="N9" s="598"/>
+      <c r="N9" s="626"/>
       <c r="O9" s="609"/>
-      <c r="S9" s="594" t="s">
+      <c r="S9" s="620" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8135,7 +8136,7 @@
       <c r="X9" s="465" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="616"/>
+      <c r="Y9" s="617"/>
       <c r="Z9" s="444"/>
       <c r="AA9" s="318"/>
       <c r="AB9" s="217"/>
@@ -8145,16 +8146,16 @@
       </c>
       <c r="AE9" s="266"/>
       <c r="AF9" s="266"/>
-      <c r="AG9" s="591"/>
+      <c r="AG9" s="619"/>
       <c r="AH9" s="266"/>
-      <c r="AI9" s="590"/>
+      <c r="AI9" s="613"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="590" t="s">
+      <c r="AK9" s="613" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="266"/>
       <c r="AM9" s="462"/>
-      <c r="AN9" s="601"/>
+      <c r="AN9" s="599"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8169,13 +8170,13 @@
       <c r="D10" s="142"/>
       <c r="E10" s="246">
         <f>Boat!U8</f>
-        <v>39</v>
-      </c>
-      <c r="F10" s="582"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="604"/>
       <c r="N10" s="452" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="584" t="s">
+      <c r="O10" s="637" t="s">
         <v>103</v>
       </c>
       <c r="P10" s="610" t="s">
@@ -8184,7 +8185,7 @@
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="595"/>
+      <c r="S10" s="624"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8196,7 +8197,7 @@
       <c r="X10" s="465" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="616"/>
+      <c r="Y10" s="617"/>
       <c r="Z10" s="443">
         <v>0</v>
       </c>
@@ -8214,16 +8215,16 @@
       <c r="AF10" s="247" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="591"/>
+      <c r="AG10" s="619"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="590"/>
+      <c r="AI10" s="613"/>
       <c r="AJ10" s="266"/>
-      <c r="AK10" s="590"/>
+      <c r="AK10" s="613"/>
       <c r="AL10" s="266"/>
       <c r="AM10" s="476" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="601"/>
+      <c r="AN10" s="599"/>
       <c r="AO10" s="212" t="s">
         <v>95</v>
       </c>
@@ -8232,7 +8233,7 @@
       <c r="A11" s="232" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="533" t="s">
+      <c r="B11" s="534" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="491" t="s">
@@ -8241,18 +8242,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="582"/>
+      <c r="F11" s="604"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="585"/>
+      <c r="O11" s="638"/>
       <c r="P11" s="611"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="595"/>
+      <c r="S11" s="624"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8262,7 +8263,7 @@
       <c r="X11" s="465" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="616"/>
+      <c r="Y11" s="617"/>
       <c r="Z11" s="443"/>
       <c r="AA11" s="318">
         <v>1</v>
@@ -8276,14 +8277,14 @@
       <c r="AF11" s="266" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="591"/>
+      <c r="AG11" s="619"/>
       <c r="AH11" s="266"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="266"/>
       <c r="AK11" s="266"/>
       <c r="AL11" s="266"/>
       <c r="AM11" s="462"/>
-      <c r="AN11" s="601"/>
+      <c r="AN11" s="599"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8292,7 +8293,7 @@
       <c r="A12" s="236" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="535"/>
+      <c r="B12" s="536"/>
       <c r="C12" s="492" t="s">
         <v>394</v>
       </c>
@@ -8302,25 +8303,25 @@
       <c r="E12" s="233">
         <v>2</v>
       </c>
-      <c r="F12" s="582"/>
+      <c r="F12" s="604"/>
       <c r="G12" s="358" t="s">
         <v>411</v>
       </c>
-      <c r="H12" s="538" t="s">
+      <c r="H12" s="539" t="s">
         <v>447</v>
       </c>
-      <c r="I12" s="540"/>
-      <c r="J12" s="540"/>
-      <c r="K12" s="589"/>
+      <c r="I12" s="541"/>
+      <c r="J12" s="541"/>
+      <c r="K12" s="642"/>
       <c r="L12" s="211"/>
       <c r="M12" s="211"/>
       <c r="N12" s="211"/>
-      <c r="O12" s="585"/>
+      <c r="O12" s="638"/>
       <c r="P12" s="611"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="596"/>
+      <c r="S12" s="621"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8330,7 +8331,7 @@
       <c r="X12" s="465" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="616"/>
+      <c r="Y12" s="617"/>
       <c r="Z12" s="441">
         <v>1</v>
       </c>
@@ -8341,16 +8342,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="599" t="s">
+      <c r="AD12" s="627" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="475" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="591" t="s">
+      <c r="AF12" s="619" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="591"/>
+      <c r="AG12" s="619"/>
       <c r="AH12" s="247" t="s">
         <v>264</v>
       </c>
@@ -8360,10 +8361,10 @@
       <c r="AJ12" s="266"/>
       <c r="AK12" s="266"/>
       <c r="AL12" s="266"/>
-      <c r="AM12" s="613" t="s">
+      <c r="AM12" s="614" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="601"/>
+      <c r="AN12" s="599"/>
       <c r="AO12" s="359" t="s">
         <v>97</v>
       </c>
@@ -8375,16 +8376,16 @@
       <c r="E13" s="482">
         <v>-3</v>
       </c>
-      <c r="F13" s="582"/>
-      <c r="G13" s="540" t="s">
+      <c r="F13" s="604"/>
+      <c r="G13" s="541" t="s">
         <v>448</v>
       </c>
-      <c r="H13" s="540"/>
-      <c r="I13" s="540"/>
-      <c r="J13" s="589"/>
+      <c r="H13" s="541"/>
+      <c r="I13" s="541"/>
+      <c r="J13" s="642"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="585"/>
+      <c r="O13" s="638"/>
       <c r="P13" s="612"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
@@ -8395,7 +8396,7 @@
       <c r="X13" s="465" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="616"/>
+      <c r="Y13" s="617"/>
       <c r="Z13" s="441">
         <v>1</v>
       </c>
@@ -8406,8 +8407,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="599"/>
-      <c r="AF13" s="591"/>
+      <c r="AD13" s="627"/>
+      <c r="AF13" s="619"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="247" t="s">
         <v>314</v>
@@ -8418,8 +8419,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="266"/>
       <c r="AL13" s="266"/>
-      <c r="AM13" s="613"/>
-      <c r="AN13" s="601"/>
+      <c r="AM13" s="614"/>
+      <c r="AN13" s="599"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="484"/>
@@ -8427,18 +8428,18 @@
       <c r="C14" s="493"/>
       <c r="D14" s="486"/>
       <c r="E14" s="487"/>
-      <c r="F14" s="582"/>
-      <c r="G14" s="540" t="s">
+      <c r="F14" s="604"/>
+      <c r="G14" s="541" t="s">
         <v>447</v>
       </c>
-      <c r="H14" s="540"/>
-      <c r="I14" s="540"/>
-      <c r="J14" s="589"/>
+      <c r="H14" s="541"/>
+      <c r="I14" s="541"/>
+      <c r="J14" s="642"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="585"/>
+      <c r="O14" s="638"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8452,34 +8453,34 @@
       <c r="X14" s="465" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="616"/>
+      <c r="Y14" s="617"/>
       <c r="Z14" s="441">
         <v>1</v>
       </c>
       <c r="AA14" s="318"/>
       <c r="AB14" s="217"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="599"/>
+      <c r="AD14" s="627"/>
       <c r="AE14" s="266"/>
-      <c r="AF14" s="591"/>
+      <c r="AF14" s="619"/>
       <c r="AG14" s="266"/>
       <c r="AH14" s="266"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="266"/>
       <c r="AK14" s="266"/>
       <c r="AL14" s="266"/>
-      <c r="AM14" s="613"/>
-      <c r="AN14" s="601"/>
+      <c r="AM14" s="614"/>
+      <c r="AN14" s="599"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="483" t="s">
         <v>525</v>
       </c>
-      <c r="C15" s="533" t="s">
+      <c r="C15" s="534" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="582"/>
-      <c r="O15" s="585"/>
+      <c r="F15" s="604"/>
+      <c r="O15" s="638"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8492,7 +8493,7 @@
       <c r="X15" s="465" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="616"/>
+      <c r="Y15" s="617"/>
       <c r="Z15" s="443">
         <v>1</v>
       </c>
@@ -8501,8 +8502,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="599"/>
-      <c r="AF15" s="591"/>
+      <c r="AD15" s="627"/>
+      <c r="AF15" s="619"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="247" t="s">
         <v>466</v>
@@ -8515,8 +8516,8 @@
       </c>
       <c r="AK15" s="266"/>
       <c r="AL15" s="266"/>
-      <c r="AM15" s="613"/>
-      <c r="AN15" s="601"/>
+      <c r="AM15" s="614"/>
+      <c r="AN15" s="599"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8531,20 +8532,20 @@
       <c r="B16" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="C16" s="535"/>
+      <c r="C16" s="536"/>
       <c r="D16" s="61" t="s">
         <v>511</v>
       </c>
       <c r="E16" s="233">
         <v>1</v>
       </c>
-      <c r="F16" s="582"/>
+      <c r="F16" s="604"/>
       <c r="G16" s="358" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="505"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="585"/>
+      <c r="O16" s="638"/>
       <c r="R16" s="469" t="s">
         <v>185</v>
       </c>
@@ -8555,7 +8556,7 @@
       <c r="X16" s="465" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="616"/>
+      <c r="Y16" s="617"/>
       <c r="Z16" s="441">
         <v>1</v>
       </c>
@@ -8576,18 +8577,18 @@
       <c r="AM16" s="462" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="601"/>
+      <c r="AN16" s="599"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="582"/>
+      <c r="F17" s="604"/>
       <c r="I17" s="506"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="585"/>
+      <c r="O17" s="638"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8607,7 +8608,7 @@
       <c r="X17" s="465" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="616"/>
+      <c r="Y17" s="617"/>
       <c r="Z17" s="443"/>
       <c r="AA17" s="318"/>
       <c r="AB17" s="217"/>
@@ -8632,7 +8633,7 @@
       <c r="AK17" s="266"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="462"/>
-      <c r="AN17" s="601"/>
+      <c r="AN17" s="599"/>
       <c r="AO17" s="212" t="s">
         <v>516</v>
       </c>
@@ -8656,21 +8657,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="582"/>
+      <c r="F18" s="604"/>
       <c r="G18" s="358" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="585"/>
+      <c r="O18" s="638"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="577" t="s">
+      <c r="R18" s="632" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="621" t="s">
+      <c r="U18" s="577" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8680,7 +8681,7 @@
       <c r="X18" s="465" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="616"/>
+      <c r="Y18" s="617"/>
       <c r="Z18" s="443">
         <v>1</v>
       </c>
@@ -8691,38 +8692,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="266"/>
-      <c r="AF18" s="590" t="s">
+      <c r="AF18" s="613" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="266"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="614" t="s">
+      <c r="AJ18" s="615" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="266"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="462"/>
-      <c r="AN18" s="601"/>
+      <c r="AN18" s="599"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="582"/>
+      <c r="F19" s="604"/>
       <c r="I19" s="228"/>
-      <c r="O19" s="585"/>
-      <c r="R19" s="578"/>
+      <c r="O19" s="638"/>
+      <c r="R19" s="633"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="622"/>
+      <c r="U19" s="578"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="465" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="616"/>
+      <c r="Y19" s="617"/>
       <c r="Z19" s="441">
         <v>1</v>
       </c>
@@ -8731,17 +8732,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="266"/>
-      <c r="AF19" s="590"/>
+      <c r="AF19" s="613"/>
       <c r="AG19" s="266"/>
       <c r="AH19" s="266"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="614"/>
+      <c r="AJ19" s="615"/>
       <c r="AK19" s="494" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="462"/>
-      <c r="AN19" s="601"/>
+      <c r="AN19" s="599"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8762,24 +8763,24 @@
       <c r="E20" s="471">
         <v>-1</v>
       </c>
-      <c r="F20" s="582"/>
+      <c r="F20" s="604"/>
       <c r="G20" s="358" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="228"/>
-      <c r="O20" s="585"/>
-      <c r="Q20" s="587" t="s">
+      <c r="O20" s="638"/>
+      <c r="Q20" s="640" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="438" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="623"/>
+      <c r="U20" s="579"/>
       <c r="W20" s="439"/>
       <c r="X20" s="466" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="616"/>
+      <c r="Y20" s="617"/>
       <c r="Z20" s="445">
         <v>1</v>
       </c>
@@ -8804,7 +8805,7 @@
       <c r="AM20" s="409" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="601"/>
+      <c r="AN20" s="599"/>
       <c r="AO20" s="359" t="s">
         <v>478</v>
       </c>
@@ -8825,20 +8826,20 @@
       <c r="E21" s="275">
         <v>0</v>
       </c>
-      <c r="F21" s="582"/>
+      <c r="F21" s="604"/>
       <c r="I21" s="228"/>
-      <c r="O21" s="585"/>
-      <c r="Q21" s="588"/>
+      <c r="O21" s="638"/>
+      <c r="Q21" s="641"/>
       <c r="T21" s="456"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="618"/>
+      <c r="V21" s="574"/>
       <c r="W21" s="460" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="463" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="616"/>
+      <c r="Y21" s="617"/>
       <c r="Z21" s="479">
         <v>3</v>
       </c>
@@ -8869,15 +8870,15 @@
       <c r="AM21" s="462" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="601"/>
+      <c r="AN21" s="599"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="582"/>
+      <c r="F22" s="604"/>
       <c r="G22" s="358" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="228"/>
-      <c r="O22" s="585"/>
+      <c r="O22" s="638"/>
       <c r="R22" s="468" t="s">
         <v>44</v>
       </c>
@@ -8885,14 +8886,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="619"/>
+      <c r="V22" s="575"/>
       <c r="W22" s="460" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="463" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="616"/>
+      <c r="Y22" s="617"/>
       <c r="Z22" s="449"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="449"/>
@@ -8903,7 +8904,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="590" t="s">
+      <c r="AJ22" s="613" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="266"/>
@@ -8911,7 +8912,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="311"/>
-      <c r="AN22" s="601"/>
+      <c r="AN22" s="599"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="240" t="s">
@@ -8929,22 +8930,22 @@
       <c r="E23" s="234">
         <v>1</v>
       </c>
-      <c r="F23" s="582"/>
+      <c r="F23" s="604"/>
       <c r="I23" s="228"/>
-      <c r="O23" s="585"/>
-      <c r="Q23" s="587" t="s">
+      <c r="O23" s="638"/>
+      <c r="Q23" s="640" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="454" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="619"/>
+      <c r="V23" s="575"/>
       <c r="W23" s="148"/>
       <c r="X23" s="463" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="616"/>
+      <c r="Y23" s="617"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="449"/>
@@ -8955,13 +8956,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="590"/>
+      <c r="AJ23" s="613"/>
       <c r="AK23" s="266"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="311"/>
-      <c r="AN23" s="601"/>
+      <c r="AN23" s="599"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="474" t="s">
@@ -8979,23 +8980,23 @@
       <c r="E24" s="470">
         <v>1</v>
       </c>
-      <c r="F24" s="582"/>
+      <c r="F24" s="604"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="228"/>
-      <c r="O24" s="585"/>
-      <c r="Q24" s="588"/>
+      <c r="O24" s="638"/>
+      <c r="Q24" s="641"/>
       <c r="T24" s="17"/>
       <c r="U24" s="236" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="619"/>
+      <c r="V24" s="575"/>
       <c r="W24" s="148"/>
       <c r="X24" s="463" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="616"/>
+      <c r="Y24" s="617"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="449"/>
@@ -9014,12 +9015,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="311"/>
-      <c r="AN24" s="601"/>
+      <c r="AN24" s="599"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="582"/>
+      <c r="F25" s="604"/>
       <c r="I25" s="228"/>
-      <c r="O25" s="585"/>
+      <c r="O25" s="638"/>
       <c r="P25" s="212" t="s">
         <v>285</v>
       </c>
@@ -9032,12 +9033,12 @@
       <c r="U25" s="434" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="620"/>
+      <c r="V25" s="576"/>
       <c r="W25" s="148"/>
       <c r="X25" s="463" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="616"/>
+      <c r="Y25" s="617"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="449"/>
@@ -9054,7 +9055,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="311"/>
-      <c r="AN25" s="601"/>
+      <c r="AN25" s="599"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="240" t="s">
@@ -9072,17 +9073,17 @@
       <c r="E26" s="407">
         <v>1</v>
       </c>
-      <c r="F26" s="582"/>
+      <c r="F26" s="604"/>
       <c r="G26" s="358" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="228"/>
-      <c r="O26" s="585"/>
-      <c r="P26" s="603" t="s">
+      <c r="O26" s="638"/>
+      <c r="P26" s="601" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="604"/>
-      <c r="R26" s="579" t="s">
+      <c r="Q26" s="602"/>
+      <c r="R26" s="634" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="183"/>
@@ -9094,7 +9095,7 @@
       <c r="X26" s="463" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="616"/>
+      <c r="Y26" s="617"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="449"/>
@@ -9121,7 +9122,7 @@
       <c r="AM26" s="476" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="601"/>
+      <c r="AN26" s="599"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9133,13 +9134,13 @@
       <c r="E27" s="275" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="583"/>
+      <c r="F27" s="636"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="229"/>
-      <c r="O27" s="586"/>
-      <c r="R27" s="580"/>
+      <c r="O27" s="639"/>
+      <c r="R27" s="635"/>
       <c r="S27" s="455" t="s">
         <v>54</v>
       </c>
@@ -9152,7 +9153,7 @@
       <c r="X27" s="463" t="s">
         <v>552</v>
       </c>
-      <c r="Y27" s="617"/>
+      <c r="Y27" s="618"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="450"/>
@@ -9169,10 +9170,48 @@
       <c r="AM27" s="409" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="602"/>
+      <c r="AN27" s="600"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9189,44 +9228,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9236,8 +9237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9330,10 +9331,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="645" t="s">
+      <c r="V1" s="649" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="646"/>
+      <c r="W1" s="650"/>
       <c r="X1" s="317">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9349,21 +9350,21 @@
       <c r="AB1" s="313" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="647" t="s">
+      <c r="AC1" s="651" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="648"/>
-      <c r="AE1" s="649"/>
-      <c r="AF1" s="650" t="s">
+      <c r="AD1" s="652"/>
+      <c r="AE1" s="653"/>
+      <c r="AF1" s="654" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="651"/>
-      <c r="AH1" s="652"/>
-      <c r="AI1" s="642" t="s">
+      <c r="AG1" s="655"/>
+      <c r="AH1" s="656"/>
+      <c r="AI1" s="646" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="643"/>
-      <c r="AK1" s="644"/>
+      <c r="AJ1" s="647"/>
+      <c r="AK1" s="648"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9380,21 +9381,21 @@
       <c r="K2" s="336">
         <v>-3</v>
       </c>
-      <c r="L2" s="653">
+      <c r="L2" s="657">
         <f>SUM(L5:L30)</f>
-        <v>3</v>
-      </c>
-      <c r="M2" s="655">
+        <v>1</v>
+      </c>
+      <c r="M2" s="659">
         <f>SUM(M4:M29)</f>
-        <v>9</v>
-      </c>
-      <c r="N2" s="657">
+        <v>8</v>
+      </c>
+      <c r="N2" s="661">
         <f>SUM(N4:N29)</f>
         <v>6</v>
       </c>
-      <c r="O2" s="597">
+      <c r="O2" s="625">
         <f>SUM(M30:M37)* (-1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P2" s="279" t="s">
         <v>243</v>
@@ -9411,7 +9412,7 @@
       <c r="T2" s="66" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="659" t="s">
+      <c r="U2" s="663" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="61" t="s">
@@ -9480,10 +9481,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="654"/>
-      <c r="M3" s="656"/>
-      <c r="N3" s="658"/>
-      <c r="O3" s="598"/>
+      <c r="L3" s="658"/>
+      <c r="M3" s="660"/>
+      <c r="N3" s="662"/>
+      <c r="O3" s="626"/>
       <c r="P3" s="177">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9497,16 +9498,16 @@
       </c>
       <c r="T3" s="301">
         <f>SUM(T4:T29)</f>
-        <v>39</v>
-      </c>
-      <c r="U3" s="660"/>
+        <v>40</v>
+      </c>
+      <c r="U3" s="664"/>
       <c r="V3" s="159">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9518,7 +9519,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9546,7 +9547,7 @@
       </c>
       <c r="AG3" s="395">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
@@ -9554,7 +9555,7 @@
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AJ3" s="322">
         <f t="shared" si="1"/>
@@ -9598,7 +9599,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="661" t="s">
+      <c r="O4" s="643" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9677,7 +9678,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="662"/>
+      <c r="O5" s="644"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9756,16 +9757,16 @@
         <v>312</v>
       </c>
       <c r="L6" s="345">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M6" s="107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="304">
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="662"/>
+      <c r="O6" s="644"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9776,17 +9777,17 @@
         <v>2</v>
       </c>
       <c r="T6" s="334">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" s="327">
         <v>-2</v>
       </c>
       <c r="V6" s="332">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W6" s="190">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X6" s="307"/>
       <c r="Y6" s="117">
@@ -9795,7 +9796,7 @@
       </c>
       <c r="Z6" s="301">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="301">
         <v>0</v>
@@ -9857,7 +9858,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="662"/>
+      <c r="O7" s="644"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -9961,7 +9962,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="662"/>
+      <c r="O8" s="644"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9979,7 +9980,7 @@
       </c>
       <c r="U8" s="527">
         <f>T3</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V8" s="332">
         <v>0</v>
@@ -10045,7 +10046,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="662"/>
+      <c r="O9" s="644"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10141,7 +10142,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="662"/>
+      <c r="O10" s="644"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10222,7 +10223,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="662"/>
+      <c r="O11" s="644"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10282,7 +10283,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="633" t="s">
+      <c r="A12" s="589" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10291,7 +10292,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="587" t="s">
+      <c r="E12" s="640" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="271">
@@ -10315,7 +10316,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O12" s="662"/>
+      <c r="O12" s="644"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10387,14 +10388,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="635"/>
+      <c r="A13" s="591"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="588"/>
+      <c r="E13" s="641"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10417,7 +10418,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="662"/>
+      <c r="O13" s="644"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10490,7 +10491,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="662"/>
+      <c r="O14" s="644"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="208" t="s">
         <v>346</v>
@@ -10573,7 +10574,7 @@
       <c r="G15" s="270" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="716">
+      <c r="H15" s="528">
         <v>-1</v>
       </c>
       <c r="I15" s="282"/>
@@ -10589,7 +10590,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O15" s="662"/>
+      <c r="O15" s="644"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="208" t="s">
         <v>346</v>
@@ -10674,7 +10675,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="662"/>
+      <c r="O16" s="644"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10722,14 +10723,14 @@
         <v>1</v>
       </c>
       <c r="AG16" s="357">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH16" s="158">
         <v>1</v>
       </c>
       <c r="AI16" s="319">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ16" s="320">
         <f t="shared" si="8"/>
@@ -10770,7 +10771,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="662"/>
+      <c r="O17" s="644"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10853,7 +10854,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="662"/>
+      <c r="O18" s="644"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10935,7 +10936,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O19" s="662"/>
+      <c r="O19" s="644"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11031,11 +11032,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="663"/>
-      <c r="P20" s="538" t="s">
+      <c r="O20" s="645"/>
+      <c r="P20" s="539" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="589"/>
+      <c r="Q20" s="642"/>
       <c r="R20" s="327" t="s">
         <v>86</v>
       </c>
@@ -11269,7 +11270,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="640" t="s">
+      <c r="E23" s="596" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -11361,7 +11362,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="641"/>
+      <c r="E24" s="597"/>
       <c r="F24" s="177"/>
       <c r="K24" s="412" t="s">
         <v>301</v>
@@ -11376,10 +11377,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P24" s="538" t="s">
+      <c r="P24" s="539" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="589"/>
+      <c r="Q24" s="642"/>
       <c r="R24" s="327" t="s">
         <v>254</v>
       </c>
@@ -11843,9 +11844,7 @@
       </c>
       <c r="K30" s="415"/>
       <c r="L30" s="353"/>
-      <c r="M30" s="254">
-        <v>-1</v>
-      </c>
+      <c r="M30" s="254"/>
       <c r="N30" s="304">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -11858,7 +11857,7 @@
       <c r="V30" s="188"/>
       <c r="W30" s="190">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X30" s="65"/>
       <c r="Y30" s="117">
@@ -11867,12 +11866,12 @@
       </c>
       <c r="Z30" s="64">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA30" s="64"/>
       <c r="AB30" s="312">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC30" s="371"/>
       <c r="AD30" s="373"/>
@@ -11885,7 +11884,7 @@
       <c r="AH30" s="337"/>
       <c r="AI30" s="356">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ30" s="320">
         <f t="shared" si="8"/>
@@ -11912,9 +11911,7 @@
       </c>
       <c r="K31" s="412"/>
       <c r="L31" s="354"/>
-      <c r="M31" s="255">
-        <v>-1</v>
-      </c>
+      <c r="M31" s="255"/>
       <c r="N31" s="304">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -11927,7 +11924,7 @@
       <c r="V31" s="189"/>
       <c r="W31" s="190">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X31" s="65"/>
       <c r="Y31" s="117">
@@ -11936,12 +11933,12 @@
       </c>
       <c r="Z31" s="64">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA31" s="64"/>
       <c r="AB31" s="312">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="371"/>
       <c r="AD31" s="375"/>
@@ -11954,7 +11951,7 @@
       <c r="AH31" s="335"/>
       <c r="AI31" s="356">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ31" s="320">
         <f t="shared" si="8"/>
@@ -11972,9 +11969,7 @@
       </c>
       <c r="K32" s="415"/>
       <c r="L32" s="354"/>
-      <c r="M32" s="259">
-        <v>0</v>
-      </c>
+      <c r="M32" s="259"/>
       <c r="N32" s="304">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -12059,9 +12054,7 @@
       </c>
       <c r="K33" s="415"/>
       <c r="L33" s="354"/>
-      <c r="M33" s="256">
-        <v>-1</v>
-      </c>
+      <c r="M33" s="256"/>
       <c r="N33" s="304">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -12074,7 +12067,7 @@
       <c r="V33" s="173"/>
       <c r="W33" s="190">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X33" s="65"/>
       <c r="Y33" s="117">
@@ -12083,12 +12076,12 @@
       </c>
       <c r="Z33" s="64">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA33" s="64"/>
       <c r="AB33" s="312">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC33" s="371"/>
       <c r="AD33" s="375"/>
@@ -12101,7 +12094,7 @@
       <c r="AH33" s="335"/>
       <c r="AI33" s="356">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ33" s="320">
         <f t="shared" si="8"/>
@@ -12256,7 +12249,7 @@
         <v>0</v>
       </c>
       <c r="AG35" s="357"/>
-      <c r="AH35" s="404">
+      <c r="AH35" s="717">
         <v>0</v>
       </c>
       <c r="AI35" s="356">
@@ -12291,7 +12284,7 @@
       </c>
       <c r="L36" s="354"/>
       <c r="M36" s="259">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" s="304">
         <f t="shared" si="10"/>
@@ -12305,7 +12298,7 @@
         <v>1</v>
       </c>
       <c r="T36" s="262">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36" s="18">
         <v>-1</v>
@@ -12313,7 +12306,7 @@
       <c r="V36" s="64"/>
       <c r="W36" s="190">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X36" s="65"/>
       <c r="Y36" s="117">
@@ -12322,7 +12315,7 @@
       </c>
       <c r="Z36" s="64">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="64"/>
       <c r="AB36" s="312">
@@ -12436,12 +12429,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12451,6 +12438,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12484,15 +12477,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="538" t="s">
+      <c r="B1" s="539" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="589"/>
+      <c r="C1" s="642"/>
       <c r="D1" s="212"/>
-      <c r="J1" s="538" t="s">
+      <c r="J1" s="539" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="589"/>
+      <c r="K1" s="642"/>
       <c r="L1" s="203" t="s">
         <v>337</v>
       </c>
@@ -12530,13 +12523,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="204"/>
-      <c r="M2" s="664"/>
+      <c r="M2" s="665"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="667" t="s">
+      <c r="Q2" s="668" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -12559,13 +12552,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="665"/>
+      <c r="M3" s="666"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="668"/>
+      <c r="Q3" s="669"/>
       <c r="R3" s="228"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12584,13 +12577,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="665"/>
+      <c r="M4" s="666"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="668"/>
+      <c r="Q4" s="669"/>
       <c r="R4" s="228"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12610,13 +12603,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="204"/>
-      <c r="M5" s="665"/>
+      <c r="M5" s="666"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="668"/>
+      <c r="Q5" s="669"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -12637,13 +12630,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="665"/>
+      <c r="M6" s="666"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="668"/>
+      <c r="Q6" s="669"/>
       <c r="R6" s="228"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12663,13 +12656,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="206"/>
-      <c r="M7" s="665"/>
+      <c r="M7" s="666"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="668"/>
+      <c r="Q7" s="669"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -12690,13 +12683,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="665"/>
+      <c r="M8" s="666"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="668"/>
+      <c r="Q8" s="669"/>
       <c r="R8" s="228"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12716,13 +12709,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="186"/>
-      <c r="M9" s="666"/>
+      <c r="M9" s="667"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="669"/>
+      <c r="Q9" s="670"/>
       <c r="R9" s="229"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -12880,10 +12873,10 @@
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="V1" s="538" t="s">
+      <c r="V1" s="539" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="589"/>
+      <c r="W1" s="642"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12902,7 +12895,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="677" t="s">
+      <c r="AD1" s="685" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12919,10 +12912,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="676" t="s">
+      <c r="F2" s="716" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="704" t="s">
+      <c r="G2" s="673" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12950,10 +12943,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="645" t="s">
+      <c r="V2" s="649" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="646"/>
+      <c r="W2" s="650"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12972,7 +12965,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="678"/>
+      <c r="AD2" s="686"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12991,8 +12984,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="637"/>
-      <c r="G3" s="705"/>
+      <c r="F3" s="593"/>
+      <c r="G3" s="674"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13003,13 +12996,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="714" t="s">
+      <c r="O3" s="683" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="696" t="s">
+      <c r="P3" s="704" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="697"/>
+      <c r="Q3" s="705"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13019,15 +13012,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="678"/>
+      <c r="AD3" s="686"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="705"/>
+      <c r="G4" s="674"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="667" t="s">
+      <c r="L4" s="668" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="715"/>
+      <c r="O4" s="684"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13037,12 +13030,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="538" t="s">
+      <c r="Y4" s="539" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="540"/>
-      <c r="AA4" s="589"/>
-      <c r="AD4" s="678"/>
+      <c r="Z4" s="541"/>
+      <c r="AA4" s="642"/>
+      <c r="AD4" s="686"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13057,21 +13050,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="705"/>
+      <c r="G5" s="674"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="683" t="s">
+      <c r="K5" s="691" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="698"/>
+      <c r="L5" s="706"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="715"/>
+      <c r="O5" s="684"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13087,11 +13080,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="686" t="s">
+      <c r="Y5" s="694" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="687"/>
-      <c r="AD5" s="678"/>
+      <c r="Z5" s="695"/>
+      <c r="AD5" s="686"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13101,16 +13094,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="705"/>
+      <c r="G6" s="674"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="684"/>
-      <c r="L6" s="698"/>
-      <c r="O6" s="715"/>
+      <c r="K6" s="692"/>
+      <c r="L6" s="706"/>
+      <c r="O6" s="684"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13120,23 +13113,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="678"/>
+      <c r="AD6" s="686"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="705"/>
+      <c r="G7" s="674"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="684"/>
-      <c r="L7" s="698"/>
+      <c r="K7" s="692"/>
+      <c r="L7" s="706"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="715"/>
+      <c r="O7" s="684"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="678"/>
+      <c r="AD7" s="686"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13149,7 +13142,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="705"/>
+      <c r="G8" s="674"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13159,41 +13152,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="684"/>
-      <c r="L8" s="698"/>
-      <c r="O8" s="715"/>
+      <c r="K8" s="692"/>
+      <c r="L8" s="706"/>
+      <c r="O8" s="684"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="680" t="s">
+      <c r="S8" s="688" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="681"/>
-      <c r="U8" s="681"/>
-      <c r="V8" s="681"/>
-      <c r="W8" s="681"/>
-      <c r="X8" s="681"/>
-      <c r="Y8" s="681"/>
-      <c r="Z8" s="681"/>
-      <c r="AA8" s="681"/>
-      <c r="AB8" s="681"/>
-      <c r="AC8" s="682"/>
-      <c r="AD8" s="678"/>
+      <c r="T8" s="689"/>
+      <c r="U8" s="689"/>
+      <c r="V8" s="689"/>
+      <c r="W8" s="689"/>
+      <c r="X8" s="689"/>
+      <c r="Y8" s="689"/>
+      <c r="Z8" s="689"/>
+      <c r="AA8" s="689"/>
+      <c r="AB8" s="689"/>
+      <c r="AC8" s="690"/>
+      <c r="AD8" s="686"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="670"/>
-      <c r="G9" s="705"/>
+      <c r="C9" s="710"/>
+      <c r="G9" s="674"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="684"/>
-      <c r="L9" s="708" t="s">
+      <c r="K9" s="692"/>
+      <c r="L9" s="677" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="709"/>
-      <c r="N9" s="710"/>
-      <c r="O9" s="715"/>
+      <c r="M9" s="678"/>
+      <c r="N9" s="679"/>
+      <c r="O9" s="684"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="678"/>
+      <c r="AD9" s="686"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="671"/>
+      <c r="C10" s="711"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13201,7 +13194,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="705"/>
+      <c r="G10" s="674"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13209,33 +13202,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="684"/>
-      <c r="M10" s="673" t="s">
+      <c r="K10" s="692"/>
+      <c r="M10" s="713" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="674"/>
-      <c r="O10" s="674"/>
-      <c r="P10" s="674"/>
-      <c r="Q10" s="674"/>
-      <c r="R10" s="674"/>
-      <c r="S10" s="674"/>
-      <c r="T10" s="674"/>
-      <c r="U10" s="674"/>
-      <c r="V10" s="674"/>
-      <c r="W10" s="674"/>
-      <c r="X10" s="674"/>
-      <c r="Y10" s="674"/>
-      <c r="Z10" s="674"/>
-      <c r="AA10" s="674"/>
-      <c r="AB10" s="674"/>
-      <c r="AC10" s="675"/>
-      <c r="AD10" s="678"/>
+      <c r="N10" s="714"/>
+      <c r="O10" s="714"/>
+      <c r="P10" s="714"/>
+      <c r="Q10" s="714"/>
+      <c r="R10" s="714"/>
+      <c r="S10" s="714"/>
+      <c r="T10" s="714"/>
+      <c r="U10" s="714"/>
+      <c r="V10" s="714"/>
+      <c r="W10" s="714"/>
+      <c r="X10" s="714"/>
+      <c r="Y10" s="714"/>
+      <c r="Z10" s="714"/>
+      <c r="AA10" s="714"/>
+      <c r="AB10" s="714"/>
+      <c r="AC10" s="715"/>
+      <c r="AD10" s="686"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="672"/>
-      <c r="G11" s="705"/>
+      <c r="C11" s="712"/>
+      <c r="G11" s="674"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="684"/>
+      <c r="K11" s="692"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13243,17 +13236,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="694" t="s">
+      <c r="Z11" s="702" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="695"/>
+      <c r="AA11" s="703"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="678"/>
+      <c r="AD11" s="686"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13266,7 +13259,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="705"/>
+      <c r="G12" s="674"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13274,8 +13267,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="684"/>
-      <c r="L12" s="699" t="s">
+      <c r="K12" s="692"/>
+      <c r="L12" s="707" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13290,7 +13283,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="533" t="s">
+      <c r="S12" s="534" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13306,26 +13299,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="688" t="s">
+      <c r="AA12" s="696" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="689"/>
+      <c r="AB12" s="697"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="678"/>
+      <c r="AD12" s="686"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="670"/>
-      <c r="G13" s="705"/>
-      <c r="K13" s="684"/>
-      <c r="L13" s="700"/>
+      <c r="C13" s="710"/>
+      <c r="G13" s="674"/>
+      <c r="K13" s="692"/>
+      <c r="L13" s="708"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="707" t="s">
+      <c r="Q13" s="676" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="604"/>
-      <c r="S13" s="534"/>
+      <c r="R13" s="602"/>
+      <c r="S13" s="535"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13333,17 +13326,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="690"/>
-      <c r="AB13" s="691"/>
-      <c r="AD13" s="678"/>
+      <c r="AA13" s="698"/>
+      <c r="AB13" s="699"/>
+      <c r="AD13" s="686"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="672"/>
+      <c r="C14" s="712"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="705"/>
+      <c r="G14" s="674"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13351,8 +13344,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="684"/>
-      <c r="L14" s="700"/>
+      <c r="K14" s="692"/>
+      <c r="L14" s="708"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13362,7 +13355,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="534"/>
+      <c r="S14" s="535"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13373,9 +13366,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="690"/>
-      <c r="AB14" s="691"/>
-      <c r="AD14" s="678"/>
+      <c r="AA14" s="698"/>
+      <c r="AB14" s="699"/>
+      <c r="AD14" s="686"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13390,20 +13383,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="705"/>
+      <c r="G15" s="674"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="684"/>
-      <c r="L15" s="701"/>
-      <c r="Q15" s="707" t="s">
+      <c r="K15" s="692"/>
+      <c r="L15" s="709"/>
+      <c r="Q15" s="676" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="604"/>
-      <c r="S15" s="534"/>
+      <c r="R15" s="602"/>
+      <c r="S15" s="535"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13411,14 +13404,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="690"/>
-      <c r="AB15" s="691"/>
-      <c r="AD15" s="678"/>
+      <c r="AA15" s="698"/>
+      <c r="AB15" s="699"/>
+      <c r="AD15" s="686"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="705"/>
-      <c r="K16" s="684"/>
+      <c r="G16" s="674"/>
+      <c r="K16" s="692"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13426,7 +13419,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="534"/>
+      <c r="S16" s="535"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13437,34 +13430,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="690"/>
-      <c r="AB16" s="691"/>
-      <c r="AD16" s="678"/>
+      <c r="AA16" s="698"/>
+      <c r="AB16" s="699"/>
+      <c r="AD16" s="686"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="702" t="s">
+      <c r="F17" s="671" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="705"/>
+      <c r="G17" s="674"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="684"/>
-      <c r="S17" s="534"/>
+      <c r="K17" s="692"/>
+      <c r="S17" s="535"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="690"/>
-      <c r="AB17" s="691"/>
-      <c r="AD17" s="678"/>
+      <c r="AA17" s="698"/>
+      <c r="AB17" s="699"/>
+      <c r="AD17" s="686"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13474,61 +13467,58 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="703"/>
-      <c r="G18" s="705"/>
+      <c r="F18" s="672"/>
+      <c r="G18" s="674"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="684"/>
+      <c r="K18" s="692"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="534"/>
+      <c r="S18" s="535"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="692"/>
-      <c r="AB18" s="693"/>
-      <c r="AD18" s="678"/>
+      <c r="AA18" s="700"/>
+      <c r="AB18" s="701"/>
+      <c r="AD18" s="686"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="706"/>
-      <c r="K19" s="685"/>
+      <c r="G19" s="675"/>
+      <c r="K19" s="693"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="711" t="s">
+      <c r="R19" s="680" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="712"/>
-      <c r="T19" s="713"/>
+      <c r="S19" s="681"/>
+      <c r="T19" s="682"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="679"/>
+      <c r="AD19" s="687"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13540,11 +13530,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Halted - CNA
Boat Halted - CNA
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C98C789-6700-452E-85B2-03D72C243FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15366B1-9F7F-491E-B0CF-66C747CD3D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="605">
   <si>
     <t>Zone</t>
   </si>
@@ -3427,7 +3427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="718">
+  <cellXfs count="720">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4685,6 +4685,9 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4733,6 +4736,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4790,34 +4823,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4892,140 +5030,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5036,63 +5096,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5111,46 +5114,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5228,30 +5210,50 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5597,10 +5599,10 @@
       <c r="I2" s="425" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="537" t="s">
+      <c r="J2" s="538" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="538"/>
+      <c r="K2" s="539"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5610,14 +5612,14 @@
       <c r="N2" s="370" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="539" t="s">
+      <c r="O2" s="540" t="s">
         <v>385</v>
       </c>
-      <c r="P2" s="540"/>
-      <c r="Q2" s="541"/>
-      <c r="R2" s="541"/>
-      <c r="S2" s="541"/>
-      <c r="T2" s="542" t="s">
+      <c r="P2" s="541"/>
+      <c r="Q2" s="542"/>
+      <c r="R2" s="542"/>
+      <c r="S2" s="542"/>
+      <c r="T2" s="543" t="s">
         <v>386</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5631,7 +5633,7 @@
       <c r="C3" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="534"/>
+      <c r="D3" s="535"/>
       <c r="E3" s="358"/>
       <c r="F3" s="275" t="s">
         <v>69</v>
@@ -5667,7 +5669,7 @@
       <c r="S3" s="177">
         <v>0</v>
       </c>
-      <c r="T3" s="543"/>
+      <c r="T3" s="544"/>
       <c r="U3" s="19" t="s">
         <v>591</v>
       </c>
@@ -5683,7 +5685,7 @@
       <c r="C4" s="169" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="535"/>
+      <c r="D4" s="536"/>
       <c r="E4" s="61"/>
       <c r="F4" s="380" t="s">
         <v>42</v>
@@ -5701,7 +5703,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="327"/>
       <c r="S4" s="6"/>
-      <c r="T4" s="543"/>
+      <c r="T4" s="544"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5710,7 +5712,7 @@
       <c r="C5" s="169" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="536"/>
+      <c r="D5" s="537"/>
       <c r="F5" s="384" t="s">
         <v>42</v>
       </c>
@@ -5729,7 +5731,7 @@
         <v>522</v>
       </c>
       <c r="P5" s="516"/>
-      <c r="T5" s="543"/>
+      <c r="T5" s="544"/>
       <c r="U5" s="212" t="s">
         <v>228</v>
       </c>
@@ -5768,7 +5770,7 @@
       <c r="P6" s="516"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="543"/>
+      <c r="T6" s="544"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="217" t="s">
@@ -5799,7 +5801,7 @@
       <c r="P7" s="516"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="6"/>
-      <c r="T7" s="543"/>
+      <c r="T7" s="544"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5828,7 +5830,7 @@
       <c r="P8" s="516"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="543"/>
+      <c r="T8" s="544"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -5862,7 +5864,7 @@
         <v>44</v>
       </c>
       <c r="P9" s="516"/>
-      <c r="T9" s="543"/>
+      <c r="T9" s="544"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -5892,7 +5894,7 @@
         <v>522</v>
       </c>
       <c r="P10" s="516"/>
-      <c r="T10" s="543"/>
+      <c r="T10" s="544"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -5927,7 +5929,7 @@
       <c r="P11" s="516"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="142"/>
-      <c r="T11" s="543"/>
+      <c r="T11" s="544"/>
       <c r="U11" s="212" t="s">
         <v>227</v>
       </c>
@@ -5960,7 +5962,7 @@
       <c r="P12" s="516"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="543"/>
+      <c r="T12" s="544"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="265" t="s">
@@ -5995,11 +5997,11 @@
         <v>522</v>
       </c>
       <c r="P13" s="516"/>
-      <c r="T13" s="543"/>
+      <c r="T13" s="544"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="516"/>
-      <c r="T14" s="543"/>
+      <c r="T14" s="544"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6025,10 +6027,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="531">
+      <c r="M15" s="532">
         <v>45275</v>
       </c>
-      <c r="N15" s="534" t="s">
+      <c r="N15" s="535" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="514" t="s">
@@ -6036,7 +6038,7 @@
       </c>
       <c r="P15" s="516"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="543"/>
+      <c r="T15" s="544"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="496" t="s">
@@ -6062,10 +6064,10 @@
       <c r="L16" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="532"/>
-      <c r="N16" s="535"/>
+      <c r="M16" s="533"/>
+      <c r="N16" s="536"/>
       <c r="P16" s="516"/>
-      <c r="T16" s="543"/>
+      <c r="T16" s="544"/>
     </row>
     <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6093,8 +6095,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="533"/>
-      <c r="N17" s="536"/>
+      <c r="M17" s="534"/>
+      <c r="N17" s="537"/>
       <c r="O17" s="514" t="s">
         <v>44</v>
       </c>
@@ -6110,11 +6112,11 @@
       <c r="S17" s="177">
         <v>0</v>
       </c>
-      <c r="T17" s="543"/>
+      <c r="T17" s="544"/>
     </row>
     <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="516"/>
-      <c r="T18" s="543"/>
+      <c r="T18" s="544"/>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6142,14 +6144,14 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="531">
+      <c r="M19" s="532">
         <v>45275</v>
       </c>
       <c r="N19" s="424" t="s">
         <v>522</v>
       </c>
       <c r="P19" s="516"/>
-      <c r="T19" s="543"/>
+      <c r="T19" s="544"/>
     </row>
     <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="250" t="s">
@@ -6175,12 +6177,12 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="532"/>
+      <c r="M20" s="533"/>
       <c r="N20" s="413" t="s">
         <v>26</v>
       </c>
       <c r="P20" s="516"/>
-      <c r="T20" s="543"/>
+      <c r="T20" s="544"/>
     </row>
     <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="250" t="s">
@@ -6206,16 +6208,16 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="532"/>
+      <c r="M21" s="533"/>
       <c r="N21" s="413" t="s">
         <v>18</v>
       </c>
       <c r="P21" s="516"/>
-      <c r="T21" s="543"/>
-      <c r="U21" s="529" t="s">
+      <c r="T21" s="544"/>
+      <c r="U21" s="530" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="530"/>
+      <c r="V21" s="531"/>
     </row>
     <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="281" t="s">
@@ -6241,12 +6243,12 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="532"/>
+      <c r="M22" s="533"/>
       <c r="N22" s="393" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="516"/>
-      <c r="T22" s="543"/>
+      <c r="T22" s="544"/>
     </row>
     <row r="23" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6272,12 +6274,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="532"/>
+      <c r="M23" s="533"/>
       <c r="N23" s="61" t="s">
         <v>523</v>
       </c>
       <c r="P23" s="516"/>
-      <c r="T23" s="543"/>
+      <c r="T23" s="544"/>
     </row>
     <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -6303,7 +6305,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="532"/>
+      <c r="M24" s="533"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6312,7 +6314,7 @@
       </c>
       <c r="P24" s="517"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="543"/>
+      <c r="T24" s="544"/>
     </row>
     <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6340,7 +6342,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="532"/>
+      <c r="M25" s="533"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6356,7 +6358,7 @@
       <c r="S25" s="21">
         <v>0</v>
       </c>
-      <c r="T25" s="543"/>
+      <c r="T25" s="544"/>
     </row>
     <row r="26" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
@@ -6382,12 +6384,12 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="532"/>
+      <c r="M26" s="533"/>
       <c r="N26" s="61" t="s">
         <v>524</v>
       </c>
       <c r="P26" s="516"/>
-      <c r="T26" s="543"/>
+      <c r="T26" s="544"/>
     </row>
     <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="265" t="s">
@@ -6409,7 +6411,7 @@
       <c r="J27" s="421"/>
       <c r="K27" s="422"/>
       <c r="L27" s="423"/>
-      <c r="M27" s="532"/>
+      <c r="M27" s="533"/>
       <c r="N27" s="61"/>
       <c r="P27" s="327">
         <v>1</v>
@@ -6423,7 +6425,7 @@
       <c r="S27" s="177">
         <v>0</v>
       </c>
-      <c r="T27" s="543"/>
+      <c r="T27" s="544"/>
     </row>
     <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="265" t="s">
@@ -6451,7 +6453,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="533"/>
+      <c r="M28" s="534"/>
       <c r="N28" s="61" t="s">
         <v>524</v>
       </c>
@@ -6467,7 +6469,7 @@
       <c r="S28" s="21">
         <v>0</v>
       </c>
-      <c r="T28" s="544"/>
+      <c r="T28" s="545"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6486,10 +6488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H11" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6546,7 +6548,7 @@
       <c r="P1" s="432" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="564" t="s">
+      <c r="Q1" s="546" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6566,32 +6568,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="548">
+      <c r="A2" s="559">
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="B2" s="550" t="s">
+      <c r="B2" s="561" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="562" t="s">
+      <c r="C2" s="573" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="552" t="s">
+      <c r="D2" s="563" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="554" t="s">
+      <c r="E2" s="565" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="199" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="560" t="s">
+      <c r="G2" s="571" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="571" t="s">
+      <c r="I2" s="553" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="430" t="s">
@@ -6615,10 +6617,10 @@
       <c r="P2" s="433">
         <v>40</v>
       </c>
-      <c r="Q2" s="565"/>
+      <c r="Q2" s="547"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
@@ -6641,14 +6643,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="549"/>
-      <c r="B3" s="551"/>
-      <c r="C3" s="563"/>
-      <c r="D3" s="553"/>
-      <c r="E3" s="555"/>
-      <c r="G3" s="561"/>
+      <c r="A3" s="560"/>
+      <c r="B3" s="562"/>
+      <c r="C3" s="574"/>
+      <c r="D3" s="564"/>
+      <c r="E3" s="566"/>
+      <c r="G3" s="572"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="572"/>
+      <c r="I3" s="554"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6656,8 +6658,8 @@
         <v>282</v>
       </c>
       <c r="Q3" s="508">
-        <f>SUM(X24:X30)</f>
-        <v>4</v>
+        <f>SUM(X24:X32)</f>
+        <v>5</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="506"/>
@@ -6668,10 +6670,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="252"/>
-      <c r="C4" s="556" t="s">
+      <c r="C4" s="567" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="572"/>
+      <c r="I4" s="554"/>
       <c r="R4" s="508" t="s">
         <v>580</v>
       </c>
@@ -6695,7 +6697,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="557"/>
+      <c r="C5" s="568"/>
       <c r="D5" s="231" t="s">
         <v>103</v>
       </c>
@@ -6705,13 +6707,13 @@
       <c r="F5" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="534" t="s">
+      <c r="G5" s="535" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="572"/>
+      <c r="I5" s="554"/>
       <c r="J5" s="431" t="s">
         <v>273</v>
       </c>
@@ -6742,22 +6744,22 @@
       <c r="X5" s="504"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="545" t="s">
+      <c r="A6" s="556" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="558"/>
-      <c r="D6" s="559"/>
+      <c r="C6" s="569"/>
+      <c r="D6" s="570"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="535"/>
-      <c r="I6" s="572"/>
+      <c r="G6" s="536"/>
+      <c r="I6" s="554"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="546"/>
+      <c r="A7" s="557"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6767,8 +6769,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="535"/>
-      <c r="I7" s="572"/>
+      <c r="G7" s="536"/>
+      <c r="I7" s="554"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6806,7 +6808,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="547"/>
+      <c r="A8" s="558"/>
       <c r="B8" s="220" t="s">
         <v>28</v>
       </c>
@@ -6814,8 +6816,8 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="535"/>
-      <c r="I8" s="572"/>
+      <c r="G8" s="536"/>
+      <c r="I8" s="554"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6839,9 +6841,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="535"/>
+      <c r="G9" s="536"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="572"/>
+      <c r="I9" s="554"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6867,8 +6869,8 @@
         <f>Boat!U8</f>
         <v>40</v>
       </c>
-      <c r="G10" s="535"/>
-      <c r="I10" s="572"/>
+      <c r="G10" s="536"/>
+      <c r="I10" s="554"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6894,7 +6896,7 @@
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="534" t="s">
+      <c r="B11" s="535" t="s">
         <v>392</v>
       </c>
       <c r="C11" s="176" t="s">
@@ -6903,8 +6905,8 @@
       <c r="D11" s="226" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="535"/>
-      <c r="I11" s="572"/>
+      <c r="G11" s="536"/>
+      <c r="I11" s="554"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6930,23 +6932,23 @@
       <c r="S11" s="24">
         <v>0</v>
       </c>
-      <c r="U11" s="566" t="s">
+      <c r="U11" s="548" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="567"/>
-      <c r="W11" s="567"/>
-      <c r="X11" s="568"/>
+      <c r="V11" s="549"/>
+      <c r="W11" s="549"/>
+      <c r="X11" s="550"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="236" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="536"/>
+      <c r="B12" s="537"/>
       <c r="E12" s="238">
         <v>3</v>
       </c>
-      <c r="G12" s="535"/>
-      <c r="I12" s="572"/>
+      <c r="G12" s="536"/>
+      <c r="I12" s="554"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -6974,12 +6976,12 @@
       <c r="B13" s="225" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="534" t="s">
+      <c r="C13" s="535" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="535"/>
-      <c r="I13" s="572"/>
+      <c r="G13" s="536"/>
+      <c r="I13" s="554"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7006,7 +7008,7 @@
       <c r="B14" s="178" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="536"/>
+      <c r="C14" s="537"/>
       <c r="D14" s="212" t="s">
         <v>154</v>
       </c>
@@ -7016,11 +7018,11 @@
       <c r="F14" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="536"/>
+      <c r="G14" s="537"/>
       <c r="H14" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="572"/>
+      <c r="I14" s="554"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7038,7 +7040,7 @@
       <c r="H15" s="282">
         <v>0</v>
       </c>
-      <c r="I15" s="572"/>
+      <c r="I15" s="554"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7069,7 +7071,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="572"/>
+      <c r="I16" s="554"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7103,7 +7105,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="572"/>
+      <c r="I17" s="554"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7115,19 +7117,19 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="572"/>
+      <c r="I18" s="554"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="569" t="s">
+      <c r="O18" s="551" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="570"/>
+      <c r="P18" s="552"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
       <c r="R18" s="24">
         <f>5-R26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
@@ -7147,7 +7149,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="572"/>
+      <c r="I19" s="554"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7175,7 +7177,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="572"/>
+      <c r="I20" s="554"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7191,14 +7193,12 @@
       <c r="V20" s="24">
         <v>1</v>
       </c>
-      <c r="W20" s="6" t="s">
-        <v>584</v>
-      </c>
+      <c r="W20" s="6"/>
       <c r="X20" s="506"/>
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="572"/>
+      <c r="I21" s="554"/>
       <c r="M21" s="225" t="s">
         <v>422</v>
       </c>
@@ -7208,9 +7208,7 @@
       <c r="V21" s="24">
         <v>1</v>
       </c>
-      <c r="W21" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="W21" s="6"/>
       <c r="X21" s="506"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7232,13 +7230,9 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="572"/>
-      <c r="U22" s="6" t="s">
-        <v>584</v>
-      </c>
-      <c r="V22" s="504">
-        <v>1</v>
-      </c>
+      <c r="I22" s="554"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="504"/>
       <c r="W22" s="6" t="s">
         <v>235</v>
       </c>
@@ -7256,17 +7250,13 @@
       <c r="E23" s="294" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="572"/>
-      <c r="U23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="V23" s="24">
-        <v>0</v>
-      </c>
+      <c r="I23" s="554"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="572"/>
+      <c r="I24" s="554"/>
       <c r="U24" s="363"/>
       <c r="V24" s="507">
         <v>-1</v>
@@ -7294,7 +7284,7 @@
       <c r="H25" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="572"/>
+      <c r="I25" s="554"/>
       <c r="J25" s="431" t="s">
         <v>274</v>
       </c>
@@ -7339,7 +7329,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="572"/>
+      <c r="I26" s="554"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7354,7 +7344,7 @@
         <v>44</v>
       </c>
       <c r="R26" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S26" s="24">
         <v>3</v>
@@ -7374,7 +7364,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="572"/>
+      <c r="I27" s="554"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7401,7 +7391,7 @@
       <c r="E28" s="224">
         <v>2</v>
       </c>
-      <c r="I28" s="572"/>
+      <c r="I28" s="554"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7423,7 +7413,7 @@
       <c r="H29" s="199" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="573"/>
+      <c r="I29" s="555"/>
       <c r="J29" s="342"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7465,13 +7455,32 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U31" s="363"/>
+      <c r="V31" s="344">
+        <v>0</v>
+      </c>
+      <c r="W31" s="718" t="s">
+        <v>584</v>
+      </c>
+      <c r="X31" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U32" s="719"/>
+      <c r="V32" s="512">
+        <v>-1</v>
+      </c>
+      <c r="W32" s="718" t="s">
+        <v>486</v>
+      </c>
+      <c r="X32" s="24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7483,6 +7492,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7492,8 +7506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7558,7 +7572,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="560" t="s">
+      <c r="I1" s="571" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7594,7 +7608,7 @@
       <c r="X1" s="464" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="616" t="s">
+      <c r="Y1" s="617" t="s">
         <v>551</v>
       </c>
       <c r="Z1" s="440">
@@ -7619,7 +7633,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="436"/>
-      <c r="AN1" s="598"/>
+      <c r="AN1" s="602"/>
       <c r="AO1" s="359" t="s">
         <v>487</v>
       </c>
@@ -7628,23 +7642,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="580">
+      <c r="A2" s="626">
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="B2" s="582" t="s">
+      <c r="B2" s="628" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="562" t="s">
+      <c r="C2" s="573" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="584" t="s">
+      <c r="D2" s="630" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="628" t="s">
+      <c r="E2" s="575" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="603" t="s">
+      <c r="F2" s="583" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="427" t="s">
@@ -7653,31 +7667,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="561"/>
+      <c r="I2" s="572"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="630" t="s">
+      <c r="K2" s="577" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="631"/>
-      <c r="M2" s="603" t="s">
+      <c r="L2" s="578"/>
+      <c r="M2" s="583" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="607" t="s">
+      <c r="O2" s="609" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="562" t="s">
+      <c r="Q2" s="573" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="534"/>
-      <c r="S2" s="620" t="s">
+      <c r="R2" s="535"/>
+      <c r="S2" s="596" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7687,7 +7701,7 @@
       <c r="X2" s="465" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="617"/>
+      <c r="Y2" s="618"/>
       <c r="Z2" s="441">
         <v>1</v>
       </c>
@@ -7710,15 +7724,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="462"/>
-      <c r="AN2" s="599"/>
+      <c r="AN2" s="603"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="581"/>
-      <c r="B3" s="583"/>
-      <c r="C3" s="563"/>
-      <c r="D3" s="585"/>
-      <c r="E3" s="629"/>
-      <c r="F3" s="604"/>
+      <c r="A3" s="627"/>
+      <c r="B3" s="629"/>
+      <c r="C3" s="574"/>
+      <c r="D3" s="631"/>
+      <c r="E3" s="576"/>
+      <c r="F3" s="584"/>
       <c r="G3" s="428" t="s">
         <v>28</v>
       </c>
@@ -7737,17 +7751,17 @@
       <c r="L3" s="209" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="604"/>
+      <c r="M3" s="584"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="608"/>
+      <c r="O3" s="610"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="563"/>
-      <c r="R3" s="536"/>
-      <c r="S3" s="621"/>
+      <c r="Q3" s="574"/>
+      <c r="R3" s="537"/>
+      <c r="S3" s="598"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7755,7 +7769,7 @@
       <c r="X3" s="465" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="617"/>
+      <c r="Y3" s="618"/>
       <c r="Z3" s="442">
         <v>1</v>
       </c>
@@ -7764,7 +7778,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="619" t="s">
+      <c r="AD3" s="593" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="266"/>
@@ -7776,16 +7790,16 @@
       <c r="AK3" s="266"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="462"/>
-      <c r="AN3" s="599"/>
+      <c r="AN3" s="603"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="596" t="s">
+      <c r="B4" s="642" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="562" t="s">
+      <c r="C4" s="573" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="368" t="s">
@@ -7794,7 +7808,7 @@
       <c r="E4" s="405">
         <v>2</v>
       </c>
-      <c r="F4" s="604"/>
+      <c r="F4" s="584"/>
       <c r="G4" s="409" t="s">
         <v>203</v>
       </c>
@@ -7811,11 +7825,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="212"/>
-      <c r="M4" s="604"/>
+      <c r="M4" s="584"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="608"/>
+      <c r="O4" s="610"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7837,12 +7851,12 @@
       <c r="X4" s="465" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="617"/>
+      <c r="Y4" s="618"/>
       <c r="Z4" s="443"/>
       <c r="AA4" s="318"/>
       <c r="AB4" s="217"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="619"/>
+      <c r="AD4" s="593"/>
       <c r="AE4" s="266"/>
       <c r="AF4" s="266"/>
       <c r="AG4" s="16"/>
@@ -7852,37 +7866,37 @@
       <c r="AK4" s="266"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="462"/>
-      <c r="AN4" s="599"/>
+      <c r="AN4" s="603"/>
       <c r="AO4" s="359" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="560" t="s">
+      <c r="A5" s="571" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="597"/>
-      <c r="C5" s="563"/>
+      <c r="B5" s="643"/>
+      <c r="C5" s="574"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="406">
         <v>1</v>
       </c>
-      <c r="F5" s="604"/>
-      <c r="G5" s="588" t="s">
+      <c r="F5" s="584"/>
+      <c r="G5" s="634" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="588"/>
-      <c r="I5" s="588"/>
-      <c r="J5" s="588"/>
-      <c r="K5" s="588"/>
-      <c r="L5" s="589"/>
-      <c r="M5" s="604"/>
+      <c r="H5" s="634"/>
+      <c r="I5" s="634"/>
+      <c r="J5" s="634"/>
+      <c r="K5" s="634"/>
+      <c r="L5" s="635"/>
+      <c r="M5" s="584"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="608"/>
+      <c r="O5" s="610"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7890,7 +7904,7 @@
       <c r="X5" s="465" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="617"/>
+      <c r="Y5" s="618"/>
       <c r="Z5" s="443">
         <v>1</v>
       </c>
@@ -7913,24 +7927,24 @@
       <c r="AK5" s="266"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="462"/>
-      <c r="AN5" s="599"/>
+      <c r="AN5" s="603"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="561"/>
-      <c r="B6" s="594" t="s">
+      <c r="A6" s="572"/>
+      <c r="B6" s="640" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="558"/>
-      <c r="D6" s="559"/>
-      <c r="F6" s="604"/>
-      <c r="G6" s="590"/>
-      <c r="H6" s="590"/>
-      <c r="I6" s="590"/>
-      <c r="J6" s="590"/>
-      <c r="K6" s="590"/>
-      <c r="L6" s="591"/>
-      <c r="M6" s="604"/>
-      <c r="O6" s="608"/>
+      <c r="C6" s="569"/>
+      <c r="D6" s="570"/>
+      <c r="F6" s="584"/>
+      <c r="G6" s="636"/>
+      <c r="H6" s="636"/>
+      <c r="I6" s="636"/>
+      <c r="J6" s="636"/>
+      <c r="K6" s="636"/>
+      <c r="L6" s="637"/>
+      <c r="M6" s="584"/>
+      <c r="O6" s="610"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7940,7 +7954,7 @@
       <c r="X6" s="465" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="617"/>
+      <c r="Y6" s="618"/>
       <c r="Z6" s="441">
         <v>1</v>
       </c>
@@ -7954,16 +7968,16 @@
       <c r="AF6" s="266"/>
       <c r="AG6" s="266"/>
       <c r="AH6" s="266"/>
-      <c r="AI6" s="613"/>
+      <c r="AI6" s="592"/>
       <c r="AJ6" s="475" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="613" t="s">
+      <c r="AK6" s="592" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="266"/>
       <c r="AM6" s="462"/>
-      <c r="AN6" s="599"/>
+      <c r="AN6" s="603"/>
       <c r="AO6" s="359" t="s">
         <v>488</v>
       </c>
@@ -7972,7 +7986,7 @@
       <c r="A7" s="241" t="s">
         <v>599</v>
       </c>
-      <c r="B7" s="595"/>
+      <c r="B7" s="641"/>
       <c r="C7" s="210" t="s">
         <v>383</v>
       </c>
@@ -7982,7 +7996,7 @@
       <c r="E7" s="275">
         <v>0</v>
       </c>
-      <c r="F7" s="604"/>
+      <c r="F7" s="584"/>
       <c r="G7" s="429">
         <v>3</v>
       </c>
@@ -7993,16 +8007,16 @@
         <v>0</v>
       </c>
       <c r="J7" s="30">
-        <v>1</v>
-      </c>
-      <c r="K7" s="534">
+        <v>0</v>
+      </c>
+      <c r="K7" s="535">
         <v>1</v>
       </c>
       <c r="L7" s="220">
         <v>0</v>
       </c>
-      <c r="M7" s="604"/>
-      <c r="O7" s="608"/>
+      <c r="M7" s="584"/>
+      <c r="O7" s="610"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8016,7 +8030,7 @@
       <c r="X7" s="465" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="617"/>
+      <c r="Y7" s="618"/>
       <c r="Z7" s="441">
         <v>1</v>
       </c>
@@ -8026,18 +8040,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="266"/>
       <c r="AF7" s="266"/>
-      <c r="AG7" s="619" t="s">
+      <c r="AG7" s="593" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="266"/>
-      <c r="AI7" s="613"/>
+      <c r="AI7" s="592"/>
       <c r="AJ7" s="266"/>
-      <c r="AK7" s="613"/>
+      <c r="AK7" s="592"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="462"/>
-      <c r="AN7" s="599"/>
+      <c r="AN7" s="603"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8052,29 +8066,29 @@
       <c r="D8" s="358"/>
       <c r="E8" s="253">
         <f>SUM(G7:N9)</f>
-        <v>22</v>
-      </c>
-      <c r="F8" s="604"/>
-      <c r="G8" s="589">
+        <v>21</v>
+      </c>
+      <c r="F8" s="584"/>
+      <c r="G8" s="635">
         <v>2</v>
       </c>
-      <c r="H8" s="586" t="s">
+      <c r="H8" s="632" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="534">
-        <v>0</v>
-      </c>
-      <c r="J8" s="586" t="s">
+      <c r="I8" s="535">
+        <v>0</v>
+      </c>
+      <c r="J8" s="632" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="592"/>
-      <c r="L8" s="622"/>
-      <c r="M8" s="605"/>
-      <c r="N8" s="625">
+      <c r="K8" s="638"/>
+      <c r="L8" s="594"/>
+      <c r="M8" s="607"/>
+      <c r="N8" s="599">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="608"/>
+      <c r="O8" s="610"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8084,7 +8098,7 @@
       <c r="X8" s="465" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="617"/>
+      <c r="Y8" s="618"/>
       <c r="Z8" s="443"/>
       <c r="AA8" s="318"/>
       <c r="AB8" s="217"/>
@@ -8092,14 +8106,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="266"/>
       <c r="AF8" s="266"/>
-      <c r="AG8" s="619"/>
+      <c r="AG8" s="593"/>
       <c r="AH8" s="266"/>
-      <c r="AI8" s="613"/>
+      <c r="AI8" s="592"/>
       <c r="AJ8" s="266"/>
       <c r="AK8" s="266"/>
       <c r="AL8" s="266"/>
       <c r="AM8" s="462"/>
-      <c r="AN8" s="599"/>
+      <c r="AN8" s="603"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="241" t="s">
@@ -8114,17 +8128,17 @@
       <c r="D9" s="369" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="604"/>
-      <c r="G9" s="591"/>
-      <c r="H9" s="587"/>
-      <c r="I9" s="536"/>
-      <c r="J9" s="587"/>
-      <c r="K9" s="593"/>
-      <c r="L9" s="623"/>
-      <c r="M9" s="606"/>
-      <c r="N9" s="626"/>
-      <c r="O9" s="609"/>
-      <c r="S9" s="620" t="s">
+      <c r="F9" s="584"/>
+      <c r="G9" s="637"/>
+      <c r="H9" s="633"/>
+      <c r="I9" s="537"/>
+      <c r="J9" s="633"/>
+      <c r="K9" s="639"/>
+      <c r="L9" s="595"/>
+      <c r="M9" s="608"/>
+      <c r="N9" s="600"/>
+      <c r="O9" s="611"/>
+      <c r="S9" s="596" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8136,7 +8150,7 @@
       <c r="X9" s="465" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="617"/>
+      <c r="Y9" s="618"/>
       <c r="Z9" s="444"/>
       <c r="AA9" s="318"/>
       <c r="AB9" s="217"/>
@@ -8146,16 +8160,16 @@
       </c>
       <c r="AE9" s="266"/>
       <c r="AF9" s="266"/>
-      <c r="AG9" s="619"/>
+      <c r="AG9" s="593"/>
       <c r="AH9" s="266"/>
-      <c r="AI9" s="613"/>
+      <c r="AI9" s="592"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="613" t="s">
+      <c r="AK9" s="592" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="266"/>
       <c r="AM9" s="462"/>
-      <c r="AN9" s="599"/>
+      <c r="AN9" s="603"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8172,20 +8186,20 @@
         <f>Boat!U8</f>
         <v>40</v>
       </c>
-      <c r="F10" s="604"/>
+      <c r="F10" s="584"/>
       <c r="N10" s="452" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="637" t="s">
+      <c r="O10" s="586" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="610" t="s">
+      <c r="P10" s="612" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="624"/>
+      <c r="S10" s="597"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8197,7 +8211,7 @@
       <c r="X10" s="465" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="617"/>
+      <c r="Y10" s="618"/>
       <c r="Z10" s="443">
         <v>0</v>
       </c>
@@ -8215,16 +8229,16 @@
       <c r="AF10" s="247" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="619"/>
+      <c r="AG10" s="593"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="613"/>
+      <c r="AI10" s="592"/>
       <c r="AJ10" s="266"/>
-      <c r="AK10" s="613"/>
+      <c r="AK10" s="592"/>
       <c r="AL10" s="266"/>
       <c r="AM10" s="476" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="599"/>
+      <c r="AN10" s="603"/>
       <c r="AO10" s="212" t="s">
         <v>95</v>
       </c>
@@ -8233,7 +8247,7 @@
       <c r="A11" s="232" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="534" t="s">
+      <c r="B11" s="535" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="491" t="s">
@@ -8242,18 +8256,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="604"/>
+      <c r="F11" s="584"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="638"/>
-      <c r="P11" s="611"/>
+      <c r="O11" s="587"/>
+      <c r="P11" s="613"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="624"/>
+      <c r="S11" s="597"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8263,7 +8277,7 @@
       <c r="X11" s="465" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="617"/>
+      <c r="Y11" s="618"/>
       <c r="Z11" s="443"/>
       <c r="AA11" s="318">
         <v>1</v>
@@ -8277,14 +8291,14 @@
       <c r="AF11" s="266" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="619"/>
+      <c r="AG11" s="593"/>
       <c r="AH11" s="266"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="266"/>
       <c r="AK11" s="266"/>
       <c r="AL11" s="266"/>
       <c r="AM11" s="462"/>
-      <c r="AN11" s="599"/>
+      <c r="AN11" s="603"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8293,7 +8307,7 @@
       <c r="A12" s="236" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="536"/>
+      <c r="B12" s="537"/>
       <c r="C12" s="492" t="s">
         <v>394</v>
       </c>
@@ -8301,27 +8315,27 @@
         <v>154</v>
       </c>
       <c r="E12" s="233">
-        <v>2</v>
-      </c>
-      <c r="F12" s="604"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="584"/>
       <c r="G12" s="358" t="s">
         <v>411</v>
       </c>
-      <c r="H12" s="539" t="s">
+      <c r="H12" s="540" t="s">
         <v>447</v>
       </c>
-      <c r="I12" s="541"/>
-      <c r="J12" s="541"/>
-      <c r="K12" s="642"/>
+      <c r="I12" s="542"/>
+      <c r="J12" s="542"/>
+      <c r="K12" s="591"/>
       <c r="L12" s="211"/>
       <c r="M12" s="211"/>
       <c r="N12" s="211"/>
-      <c r="O12" s="638"/>
-      <c r="P12" s="611"/>
+      <c r="O12" s="587"/>
+      <c r="P12" s="613"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="621"/>
+      <c r="S12" s="598"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8331,7 +8345,7 @@
       <c r="X12" s="465" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="617"/>
+      <c r="Y12" s="618"/>
       <c r="Z12" s="441">
         <v>1</v>
       </c>
@@ -8342,16 +8356,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="627" t="s">
+      <c r="AD12" s="601" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="475" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="619" t="s">
+      <c r="AF12" s="593" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="619"/>
+      <c r="AG12" s="593"/>
       <c r="AH12" s="247" t="s">
         <v>264</v>
       </c>
@@ -8361,10 +8375,10 @@
       <c r="AJ12" s="266"/>
       <c r="AK12" s="266"/>
       <c r="AL12" s="266"/>
-      <c r="AM12" s="614" t="s">
+      <c r="AM12" s="615" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="599"/>
+      <c r="AN12" s="603"/>
       <c r="AO12" s="359" t="s">
         <v>97</v>
       </c>
@@ -8376,17 +8390,17 @@
       <c r="E13" s="482">
         <v>-3</v>
       </c>
-      <c r="F13" s="604"/>
-      <c r="G13" s="541" t="s">
+      <c r="F13" s="584"/>
+      <c r="G13" s="542" t="s">
         <v>448</v>
       </c>
-      <c r="H13" s="541"/>
-      <c r="I13" s="541"/>
-      <c r="J13" s="642"/>
+      <c r="H13" s="542"/>
+      <c r="I13" s="542"/>
+      <c r="J13" s="591"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="638"/>
-      <c r="P13" s="612"/>
+      <c r="O13" s="587"/>
+      <c r="P13" s="614"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8396,7 +8410,7 @@
       <c r="X13" s="465" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="617"/>
+      <c r="Y13" s="618"/>
       <c r="Z13" s="441">
         <v>1</v>
       </c>
@@ -8407,8 +8421,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="627"/>
-      <c r="AF13" s="619"/>
+      <c r="AD13" s="601"/>
+      <c r="AF13" s="593"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="247" t="s">
         <v>314</v>
@@ -8419,8 +8433,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="266"/>
       <c r="AL13" s="266"/>
-      <c r="AM13" s="614"/>
-      <c r="AN13" s="599"/>
+      <c r="AM13" s="615"/>
+      <c r="AN13" s="603"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="484"/>
@@ -8428,18 +8442,18 @@
       <c r="C14" s="493"/>
       <c r="D14" s="486"/>
       <c r="E14" s="487"/>
-      <c r="F14" s="604"/>
-      <c r="G14" s="541" t="s">
+      <c r="F14" s="584"/>
+      <c r="G14" s="542" t="s">
         <v>447</v>
       </c>
-      <c r="H14" s="541"/>
-      <c r="I14" s="541"/>
-      <c r="J14" s="642"/>
+      <c r="H14" s="542"/>
+      <c r="I14" s="542"/>
+      <c r="J14" s="591"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="638"/>
+      <c r="O14" s="587"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8453,34 +8467,34 @@
       <c r="X14" s="465" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="617"/>
+      <c r="Y14" s="618"/>
       <c r="Z14" s="441">
         <v>1</v>
       </c>
       <c r="AA14" s="318"/>
       <c r="AB14" s="217"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="627"/>
+      <c r="AD14" s="601"/>
       <c r="AE14" s="266"/>
-      <c r="AF14" s="619"/>
+      <c r="AF14" s="593"/>
       <c r="AG14" s="266"/>
       <c r="AH14" s="266"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="266"/>
       <c r="AK14" s="266"/>
       <c r="AL14" s="266"/>
-      <c r="AM14" s="614"/>
-      <c r="AN14" s="599"/>
+      <c r="AM14" s="615"/>
+      <c r="AN14" s="603"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="483" t="s">
         <v>525</v>
       </c>
-      <c r="C15" s="534" t="s">
+      <c r="C15" s="535" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="604"/>
-      <c r="O15" s="638"/>
+      <c r="F15" s="584"/>
+      <c r="O15" s="587"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8493,7 +8507,7 @@
       <c r="X15" s="465" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="617"/>
+      <c r="Y15" s="618"/>
       <c r="Z15" s="443">
         <v>1</v>
       </c>
@@ -8502,8 +8516,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="627"/>
-      <c r="AF15" s="619"/>
+      <c r="AD15" s="601"/>
+      <c r="AF15" s="593"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="247" t="s">
         <v>466</v>
@@ -8516,8 +8530,8 @@
       </c>
       <c r="AK15" s="266"/>
       <c r="AL15" s="266"/>
-      <c r="AM15" s="614"/>
-      <c r="AN15" s="599"/>
+      <c r="AM15" s="615"/>
+      <c r="AN15" s="603"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8532,20 +8546,20 @@
       <c r="B16" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="C16" s="536"/>
+      <c r="C16" s="537"/>
       <c r="D16" s="61" t="s">
         <v>511</v>
       </c>
       <c r="E16" s="233">
         <v>1</v>
       </c>
-      <c r="F16" s="604"/>
+      <c r="F16" s="584"/>
       <c r="G16" s="358" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="505"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="638"/>
+      <c r="O16" s="587"/>
       <c r="R16" s="469" t="s">
         <v>185</v>
       </c>
@@ -8556,7 +8570,7 @@
       <c r="X16" s="465" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="617"/>
+      <c r="Y16" s="618"/>
       <c r="Z16" s="441">
         <v>1</v>
       </c>
@@ -8577,18 +8591,18 @@
       <c r="AM16" s="462" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="599"/>
+      <c r="AN16" s="603"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="604"/>
+      <c r="F17" s="584"/>
       <c r="I17" s="506"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="638"/>
+      <c r="O17" s="587"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8608,7 +8622,7 @@
       <c r="X17" s="465" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="617"/>
+      <c r="Y17" s="618"/>
       <c r="Z17" s="443"/>
       <c r="AA17" s="318"/>
       <c r="AB17" s="217"/>
@@ -8633,7 +8647,7 @@
       <c r="AK17" s="266"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="462"/>
-      <c r="AN17" s="599"/>
+      <c r="AN17" s="603"/>
       <c r="AO17" s="212" t="s">
         <v>516</v>
       </c>
@@ -8657,21 +8671,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="604"/>
+      <c r="F18" s="584"/>
       <c r="G18" s="358" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="638"/>
+      <c r="O18" s="587"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="632" t="s">
+      <c r="R18" s="579" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="577" t="s">
+      <c r="U18" s="623" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8681,7 +8695,7 @@
       <c r="X18" s="465" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="617"/>
+      <c r="Y18" s="618"/>
       <c r="Z18" s="443">
         <v>1</v>
       </c>
@@ -8692,38 +8706,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="266"/>
-      <c r="AF18" s="613" t="s">
+      <c r="AF18" s="592" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="266"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="615" t="s">
+      <c r="AJ18" s="616" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="266"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="462"/>
-      <c r="AN18" s="599"/>
+      <c r="AN18" s="603"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="604"/>
+      <c r="F19" s="584"/>
       <c r="I19" s="228"/>
-      <c r="O19" s="638"/>
-      <c r="R19" s="633"/>
+      <c r="O19" s="587"/>
+      <c r="R19" s="580"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="578"/>
+      <c r="U19" s="624"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="465" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="617"/>
+      <c r="Y19" s="618"/>
       <c r="Z19" s="441">
         <v>1</v>
       </c>
@@ -8732,17 +8746,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="266"/>
-      <c r="AF19" s="613"/>
+      <c r="AF19" s="592"/>
       <c r="AG19" s="266"/>
       <c r="AH19" s="266"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="615"/>
+      <c r="AJ19" s="616"/>
       <c r="AK19" s="494" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="462"/>
-      <c r="AN19" s="599"/>
+      <c r="AN19" s="603"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8763,24 +8777,24 @@
       <c r="E20" s="471">
         <v>-1</v>
       </c>
-      <c r="F20" s="604"/>
+      <c r="F20" s="584"/>
       <c r="G20" s="358" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="228"/>
-      <c r="O20" s="638"/>
-      <c r="Q20" s="640" t="s">
+      <c r="O20" s="587"/>
+      <c r="Q20" s="589" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="438" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="579"/>
+      <c r="U20" s="625"/>
       <c r="W20" s="439"/>
       <c r="X20" s="466" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="617"/>
+      <c r="Y20" s="618"/>
       <c r="Z20" s="445">
         <v>1</v>
       </c>
@@ -8805,7 +8819,7 @@
       <c r="AM20" s="409" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="599"/>
+      <c r="AN20" s="603"/>
       <c r="AO20" s="359" t="s">
         <v>478</v>
       </c>
@@ -8826,20 +8840,20 @@
       <c r="E21" s="275">
         <v>0</v>
       </c>
-      <c r="F21" s="604"/>
+      <c r="F21" s="584"/>
       <c r="I21" s="228"/>
-      <c r="O21" s="638"/>
-      <c r="Q21" s="641"/>
+      <c r="O21" s="587"/>
+      <c r="Q21" s="590"/>
       <c r="T21" s="456"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="574"/>
+      <c r="V21" s="620"/>
       <c r="W21" s="460" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="463" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="617"/>
+      <c r="Y21" s="618"/>
       <c r="Z21" s="479">
         <v>3</v>
       </c>
@@ -8870,15 +8884,15 @@
       <c r="AM21" s="462" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="599"/>
+      <c r="AN21" s="603"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="604"/>
+      <c r="F22" s="584"/>
       <c r="G22" s="358" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="228"/>
-      <c r="O22" s="638"/>
+      <c r="O22" s="587"/>
       <c r="R22" s="468" t="s">
         <v>44</v>
       </c>
@@ -8886,14 +8900,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="575"/>
+      <c r="V22" s="621"/>
       <c r="W22" s="460" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="463" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="617"/>
+      <c r="Y22" s="618"/>
       <c r="Z22" s="449"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="449"/>
@@ -8904,7 +8918,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="613" t="s">
+      <c r="AJ22" s="592" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="266"/>
@@ -8912,7 +8926,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="311"/>
-      <c r="AN22" s="599"/>
+      <c r="AN22" s="603"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="240" t="s">
@@ -8930,22 +8944,22 @@
       <c r="E23" s="234">
         <v>1</v>
       </c>
-      <c r="F23" s="604"/>
+      <c r="F23" s="584"/>
       <c r="I23" s="228"/>
-      <c r="O23" s="638"/>
-      <c r="Q23" s="640" t="s">
+      <c r="O23" s="587"/>
+      <c r="Q23" s="589" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="454" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="575"/>
+      <c r="V23" s="621"/>
       <c r="W23" s="148"/>
       <c r="X23" s="463" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="617"/>
+      <c r="Y23" s="618"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="449"/>
@@ -8956,13 +8970,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="613"/>
+      <c r="AJ23" s="592"/>
       <c r="AK23" s="266"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="311"/>
-      <c r="AN23" s="599"/>
+      <c r="AN23" s="603"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="474" t="s">
@@ -8980,23 +8994,23 @@
       <c r="E24" s="470">
         <v>1</v>
       </c>
-      <c r="F24" s="604"/>
+      <c r="F24" s="584"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="228"/>
-      <c r="O24" s="638"/>
-      <c r="Q24" s="641"/>
+      <c r="O24" s="587"/>
+      <c r="Q24" s="590"/>
       <c r="T24" s="17"/>
       <c r="U24" s="236" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="575"/>
+      <c r="V24" s="621"/>
       <c r="W24" s="148"/>
       <c r="X24" s="463" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="617"/>
+      <c r="Y24" s="618"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="449"/>
@@ -9015,12 +9029,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="311"/>
-      <c r="AN24" s="599"/>
+      <c r="AN24" s="603"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="604"/>
+      <c r="F25" s="584"/>
       <c r="I25" s="228"/>
-      <c r="O25" s="638"/>
+      <c r="O25" s="587"/>
       <c r="P25" s="212" t="s">
         <v>285</v>
       </c>
@@ -9033,12 +9047,12 @@
       <c r="U25" s="434" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="576"/>
+      <c r="V25" s="622"/>
       <c r="W25" s="148"/>
       <c r="X25" s="463" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="617"/>
+      <c r="Y25" s="618"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="449"/>
@@ -9055,7 +9069,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="311"/>
-      <c r="AN25" s="599"/>
+      <c r="AN25" s="603"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="240" t="s">
@@ -9073,17 +9087,17 @@
       <c r="E26" s="407">
         <v>1</v>
       </c>
-      <c r="F26" s="604"/>
+      <c r="F26" s="584"/>
       <c r="G26" s="358" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="228"/>
-      <c r="O26" s="638"/>
-      <c r="P26" s="601" t="s">
+      <c r="O26" s="587"/>
+      <c r="P26" s="605" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="602"/>
-      <c r="R26" s="634" t="s">
+      <c r="Q26" s="606"/>
+      <c r="R26" s="581" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="183"/>
@@ -9095,7 +9109,7 @@
       <c r="X26" s="463" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="617"/>
+      <c r="Y26" s="618"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="449"/>
@@ -9122,7 +9136,7 @@
       <c r="AM26" s="476" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="599"/>
+      <c r="AN26" s="603"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9134,13 +9148,13 @@
       <c r="E27" s="275" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="636"/>
+      <c r="F27" s="585"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="229"/>
-      <c r="O27" s="639"/>
-      <c r="R27" s="635"/>
+      <c r="O27" s="588"/>
+      <c r="R27" s="582"/>
       <c r="S27" s="455" t="s">
         <v>54</v>
       </c>
@@ -9153,7 +9167,7 @@
       <c r="X27" s="463" t="s">
         <v>552</v>
       </c>
-      <c r="Y27" s="618"/>
+      <c r="Y27" s="619"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="450"/>
@@ -9170,32 +9184,26 @@
       <c r="AM27" s="409" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="600"/>
+      <c r="AN27" s="604"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9212,22 +9220,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9237,8 +9251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView topLeftCell="N18" workbookViewId="0">
+      <selection activeCell="AM37" sqref="AM37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9331,10 +9345,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="649" t="s">
+      <c r="V1" s="647" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="650"/>
+      <c r="W1" s="648"/>
       <c r="X1" s="317">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9350,21 +9364,21 @@
       <c r="AB1" s="313" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="651" t="s">
+      <c r="AC1" s="649" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="652"/>
-      <c r="AE1" s="653"/>
-      <c r="AF1" s="654" t="s">
+      <c r="AD1" s="650"/>
+      <c r="AE1" s="651"/>
+      <c r="AF1" s="652" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="655"/>
-      <c r="AH1" s="656"/>
-      <c r="AI1" s="646" t="s">
+      <c r="AG1" s="653"/>
+      <c r="AH1" s="654"/>
+      <c r="AI1" s="644" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="647"/>
-      <c r="AK1" s="648"/>
+      <c r="AJ1" s="645"/>
+      <c r="AK1" s="646"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9381,19 +9395,19 @@
       <c r="K2" s="336">
         <v>-3</v>
       </c>
-      <c r="L2" s="657">
+      <c r="L2" s="655">
         <f>SUM(L5:L30)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="659">
+      <c r="M2" s="657">
         <f>SUM(M4:M29)</f>
         <v>8</v>
       </c>
-      <c r="N2" s="661">
+      <c r="N2" s="659">
         <f>SUM(N4:N29)</f>
         <v>6</v>
       </c>
-      <c r="O2" s="625">
+      <c r="O2" s="599">
         <f>SUM(M30:M37)* (-1)</f>
         <v>0</v>
       </c>
@@ -9412,7 +9426,7 @@
       <c r="T2" s="66" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="663" t="s">
+      <c r="U2" s="661" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="61" t="s">
@@ -9481,10 +9495,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="658"/>
-      <c r="M3" s="660"/>
-      <c r="N3" s="662"/>
-      <c r="O3" s="626"/>
+      <c r="L3" s="656"/>
+      <c r="M3" s="658"/>
+      <c r="N3" s="660"/>
+      <c r="O3" s="600"/>
       <c r="P3" s="177">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9500,7 +9514,7 @@
         <f>SUM(T4:T29)</f>
         <v>40</v>
       </c>
-      <c r="U3" s="664"/>
+      <c r="U3" s="662"/>
       <c r="V3" s="159">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>8</v>
@@ -9551,7 +9565,7 @@
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
@@ -9599,7 +9613,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="643" t="s">
+      <c r="O4" s="663" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9678,7 +9692,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="644"/>
+      <c r="O5" s="664"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9766,7 +9780,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="644"/>
+      <c r="O6" s="664"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9858,7 +9872,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="644"/>
+      <c r="O7" s="664"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -9962,7 +9976,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="644"/>
+      <c r="O8" s="664"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10046,7 +10060,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="644"/>
+      <c r="O9" s="664"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10142,7 +10156,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="644"/>
+      <c r="O10" s="664"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10223,7 +10237,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="644"/>
+      <c r="O11" s="664"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10283,7 +10297,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="589" t="s">
+      <c r="A12" s="635" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10292,7 +10306,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="640" t="s">
+      <c r="E12" s="589" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="271">
@@ -10316,7 +10330,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O12" s="644"/>
+      <c r="O12" s="664"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10363,7 +10377,7 @@
       </c>
       <c r="AG12" s="357"/>
       <c r="AH12" s="158">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AI12" s="319">
         <f t="shared" si="7"/>
@@ -10388,14 +10402,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="591"/>
+      <c r="A13" s="637"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="641"/>
+      <c r="E13" s="590"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10418,7 +10432,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="644"/>
+      <c r="O13" s="664"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10491,7 +10505,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="644"/>
+      <c r="O14" s="664"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="208" t="s">
         <v>346</v>
@@ -10499,9 +10513,7 @@
       <c r="R14" s="327" t="s">
         <v>246</v>
       </c>
-      <c r="S14" s="164">
-        <v>0</v>
-      </c>
+      <c r="S14" s="164"/>
       <c r="T14" s="525">
         <v>0</v>
       </c>
@@ -10590,7 +10602,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O15" s="644"/>
+      <c r="O15" s="664"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="208" t="s">
         <v>346</v>
@@ -10675,7 +10687,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="644"/>
+      <c r="O16" s="664"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10771,7 +10783,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="644"/>
+      <c r="O17" s="664"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10854,7 +10866,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="644"/>
+      <c r="O18" s="664"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10936,7 +10948,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O19" s="644"/>
+      <c r="O19" s="664"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11032,11 +11044,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="645"/>
-      <c r="P20" s="539" t="s">
+      <c r="O20" s="665"/>
+      <c r="P20" s="540" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="642"/>
+      <c r="Q20" s="591"/>
       <c r="R20" s="327" t="s">
         <v>86</v>
       </c>
@@ -11270,7 +11282,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="596" t="s">
+      <c r="E23" s="642" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -11362,7 +11374,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="597"/>
+      <c r="E24" s="643"/>
       <c r="F24" s="177"/>
       <c r="K24" s="412" t="s">
         <v>301</v>
@@ -11377,10 +11389,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P24" s="539" t="s">
+      <c r="P24" s="540" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="642"/>
+      <c r="Q24" s="591"/>
       <c r="R24" s="327" t="s">
         <v>254</v>
       </c>
@@ -12249,7 +12261,7 @@
         <v>0</v>
       </c>
       <c r="AG35" s="357"/>
-      <c r="AH35" s="717">
+      <c r="AH35" s="529">
         <v>0</v>
       </c>
       <c r="AI35" s="356">
@@ -12423,12 +12435,21 @@
       <c r="AL37" s="6" t="s">
         <v>486</v>
       </c>
+      <c r="AM37" s="24" t="s">
+        <v>589</v>
+      </c>
       <c r="AN37" s="64" t="s">
         <v>588</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12438,12 +12459,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12477,15 +12492,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="539" t="s">
+      <c r="B1" s="540" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="642"/>
+      <c r="C1" s="591"/>
       <c r="D1" s="212"/>
-      <c r="J1" s="539" t="s">
+      <c r="J1" s="540" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="642"/>
+      <c r="K1" s="591"/>
       <c r="L1" s="203" t="s">
         <v>337</v>
       </c>
@@ -12523,13 +12538,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="204"/>
-      <c r="M2" s="665"/>
+      <c r="M2" s="666"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="668" t="s">
+      <c r="Q2" s="669" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -12552,13 +12567,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="666"/>
+      <c r="M3" s="667"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="669"/>
+      <c r="Q3" s="670"/>
       <c r="R3" s="228"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12577,13 +12592,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="666"/>
+      <c r="M4" s="667"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="669"/>
+      <c r="Q4" s="670"/>
       <c r="R4" s="228"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12603,13 +12618,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="204"/>
-      <c r="M5" s="666"/>
+      <c r="M5" s="667"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="669"/>
+      <c r="Q5" s="670"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -12630,13 +12645,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="666"/>
+      <c r="M6" s="667"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="669"/>
+      <c r="Q6" s="670"/>
       <c r="R6" s="228"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12656,13 +12671,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="206"/>
-      <c r="M7" s="666"/>
+      <c r="M7" s="667"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="669"/>
+      <c r="Q7" s="670"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -12683,13 +12698,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="666"/>
+      <c r="M8" s="667"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="669"/>
+      <c r="Q8" s="670"/>
       <c r="R8" s="228"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12709,13 +12724,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="186"/>
-      <c r="M9" s="667"/>
+      <c r="M9" s="668"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="670"/>
+      <c r="Q9" s="671"/>
       <c r="R9" s="229"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -12873,10 +12888,10 @@
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="V1" s="539" t="s">
+      <c r="V1" s="540" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="642"/>
+      <c r="W1" s="591"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12895,7 +12910,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="685" t="s">
+      <c r="AD1" s="679" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12912,10 +12927,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="716" t="s">
+      <c r="F2" s="678" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="673" t="s">
+      <c r="G2" s="706" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12943,10 +12958,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="649" t="s">
+      <c r="V2" s="647" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="650"/>
+      <c r="W2" s="648"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12965,7 +12980,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="686"/>
+      <c r="AD2" s="680"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12984,8 +12999,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="593"/>
-      <c r="G3" s="674"/>
+      <c r="F3" s="639"/>
+      <c r="G3" s="707"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -12996,13 +13011,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="683" t="s">
+      <c r="O3" s="716" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="704" t="s">
+      <c r="P3" s="698" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="705"/>
+      <c r="Q3" s="699"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13012,15 +13027,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="686"/>
+      <c r="AD3" s="680"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="674"/>
+      <c r="G4" s="707"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="668" t="s">
+      <c r="L4" s="669" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="684"/>
+      <c r="O4" s="717"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13030,12 +13045,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="539" t="s">
+      <c r="Y4" s="540" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="541"/>
-      <c r="AA4" s="642"/>
-      <c r="AD4" s="686"/>
+      <c r="Z4" s="542"/>
+      <c r="AA4" s="591"/>
+      <c r="AD4" s="680"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13050,21 +13065,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="674"/>
+      <c r="G5" s="707"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="691" t="s">
+      <c r="K5" s="685" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="706"/>
+      <c r="L5" s="700"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="684"/>
+      <c r="O5" s="717"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13080,11 +13095,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="694" t="s">
+      <c r="Y5" s="688" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="695"/>
-      <c r="AD5" s="686"/>
+      <c r="Z5" s="689"/>
+      <c r="AD5" s="680"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13094,16 +13109,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="674"/>
+      <c r="G6" s="707"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="692"/>
-      <c r="L6" s="706"/>
-      <c r="O6" s="684"/>
+      <c r="K6" s="686"/>
+      <c r="L6" s="700"/>
+      <c r="O6" s="717"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13113,23 +13128,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="686"/>
+      <c r="AD6" s="680"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="674"/>
+      <c r="G7" s="707"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="692"/>
-      <c r="L7" s="706"/>
+      <c r="K7" s="686"/>
+      <c r="L7" s="700"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="684"/>
+      <c r="O7" s="717"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="686"/>
+      <c r="AD7" s="680"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13142,7 +13157,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="674"/>
+      <c r="G8" s="707"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13152,41 +13167,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="692"/>
-      <c r="L8" s="706"/>
-      <c r="O8" s="684"/>
+      <c r="K8" s="686"/>
+      <c r="L8" s="700"/>
+      <c r="O8" s="717"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="688" t="s">
+      <c r="S8" s="682" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="689"/>
-      <c r="U8" s="689"/>
-      <c r="V8" s="689"/>
-      <c r="W8" s="689"/>
-      <c r="X8" s="689"/>
-      <c r="Y8" s="689"/>
-      <c r="Z8" s="689"/>
-      <c r="AA8" s="689"/>
-      <c r="AB8" s="689"/>
-      <c r="AC8" s="690"/>
-      <c r="AD8" s="686"/>
+      <c r="T8" s="683"/>
+      <c r="U8" s="683"/>
+      <c r="V8" s="683"/>
+      <c r="W8" s="683"/>
+      <c r="X8" s="683"/>
+      <c r="Y8" s="683"/>
+      <c r="Z8" s="683"/>
+      <c r="AA8" s="683"/>
+      <c r="AB8" s="683"/>
+      <c r="AC8" s="684"/>
+      <c r="AD8" s="680"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="710"/>
-      <c r="G9" s="674"/>
+      <c r="C9" s="672"/>
+      <c r="G9" s="707"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="692"/>
-      <c r="L9" s="677" t="s">
+      <c r="K9" s="686"/>
+      <c r="L9" s="710" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="678"/>
-      <c r="N9" s="679"/>
-      <c r="O9" s="684"/>
+      <c r="M9" s="711"/>
+      <c r="N9" s="712"/>
+      <c r="O9" s="717"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="686"/>
+      <c r="AD9" s="680"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="711"/>
+      <c r="C10" s="673"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13194,7 +13209,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="674"/>
+      <c r="G10" s="707"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13202,33 +13217,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="692"/>
-      <c r="M10" s="713" t="s">
+      <c r="K10" s="686"/>
+      <c r="M10" s="675" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="714"/>
-      <c r="O10" s="714"/>
-      <c r="P10" s="714"/>
-      <c r="Q10" s="714"/>
-      <c r="R10" s="714"/>
-      <c r="S10" s="714"/>
-      <c r="T10" s="714"/>
-      <c r="U10" s="714"/>
-      <c r="V10" s="714"/>
-      <c r="W10" s="714"/>
-      <c r="X10" s="714"/>
-      <c r="Y10" s="714"/>
-      <c r="Z10" s="714"/>
-      <c r="AA10" s="714"/>
-      <c r="AB10" s="714"/>
-      <c r="AC10" s="715"/>
-      <c r="AD10" s="686"/>
+      <c r="N10" s="676"/>
+      <c r="O10" s="676"/>
+      <c r="P10" s="676"/>
+      <c r="Q10" s="676"/>
+      <c r="R10" s="676"/>
+      <c r="S10" s="676"/>
+      <c r="T10" s="676"/>
+      <c r="U10" s="676"/>
+      <c r="V10" s="676"/>
+      <c r="W10" s="676"/>
+      <c r="X10" s="676"/>
+      <c r="Y10" s="676"/>
+      <c r="Z10" s="676"/>
+      <c r="AA10" s="676"/>
+      <c r="AB10" s="676"/>
+      <c r="AC10" s="677"/>
+      <c r="AD10" s="680"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="712"/>
-      <c r="G11" s="674"/>
+      <c r="C11" s="674"/>
+      <c r="G11" s="707"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="692"/>
+      <c r="K11" s="686"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13236,17 +13251,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="702" t="s">
+      <c r="Z11" s="696" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="703"/>
+      <c r="AA11" s="697"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="686"/>
+      <c r="AD11" s="680"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13259,7 +13274,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="674"/>
+      <c r="G12" s="707"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13267,8 +13282,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="692"/>
-      <c r="L12" s="707" t="s">
+      <c r="K12" s="686"/>
+      <c r="L12" s="701" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13283,7 +13298,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="534" t="s">
+      <c r="S12" s="535" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13299,26 +13314,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="696" t="s">
+      <c r="AA12" s="690" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="697"/>
+      <c r="AB12" s="691"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="686"/>
+      <c r="AD12" s="680"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="710"/>
-      <c r="G13" s="674"/>
-      <c r="K13" s="692"/>
-      <c r="L13" s="708"/>
+      <c r="C13" s="672"/>
+      <c r="G13" s="707"/>
+      <c r="K13" s="686"/>
+      <c r="L13" s="702"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="676" t="s">
+      <c r="Q13" s="709" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="602"/>
-      <c r="S13" s="535"/>
+      <c r="R13" s="606"/>
+      <c r="S13" s="536"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13326,17 +13341,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="698"/>
-      <c r="AB13" s="699"/>
-      <c r="AD13" s="686"/>
+      <c r="AA13" s="692"/>
+      <c r="AB13" s="693"/>
+      <c r="AD13" s="680"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="712"/>
+      <c r="C14" s="674"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="674"/>
+      <c r="G14" s="707"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13344,8 +13359,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="692"/>
-      <c r="L14" s="708"/>
+      <c r="K14" s="686"/>
+      <c r="L14" s="702"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13355,7 +13370,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="535"/>
+      <c r="S14" s="536"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13366,9 +13381,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="698"/>
-      <c r="AB14" s="699"/>
-      <c r="AD14" s="686"/>
+      <c r="AA14" s="692"/>
+      <c r="AB14" s="693"/>
+      <c r="AD14" s="680"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13383,20 +13398,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="674"/>
+      <c r="G15" s="707"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="692"/>
-      <c r="L15" s="709"/>
-      <c r="Q15" s="676" t="s">
+      <c r="K15" s="686"/>
+      <c r="L15" s="703"/>
+      <c r="Q15" s="709" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="602"/>
-      <c r="S15" s="535"/>
+      <c r="R15" s="606"/>
+      <c r="S15" s="536"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13404,14 +13419,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="698"/>
-      <c r="AB15" s="699"/>
-      <c r="AD15" s="686"/>
+      <c r="AA15" s="692"/>
+      <c r="AB15" s="693"/>
+      <c r="AD15" s="680"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="674"/>
-      <c r="K16" s="692"/>
+      <c r="G16" s="707"/>
+      <c r="K16" s="686"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13419,7 +13434,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="535"/>
+      <c r="S16" s="536"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13430,34 +13445,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="698"/>
-      <c r="AB16" s="699"/>
-      <c r="AD16" s="686"/>
+      <c r="AA16" s="692"/>
+      <c r="AB16" s="693"/>
+      <c r="AD16" s="680"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="671" t="s">
+      <c r="F17" s="704" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="674"/>
+      <c r="G17" s="707"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="692"/>
-      <c r="S17" s="535"/>
+      <c r="K17" s="686"/>
+      <c r="S17" s="536"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="698"/>
-      <c r="AB17" s="699"/>
-      <c r="AD17" s="686"/>
+      <c r="AA17" s="692"/>
+      <c r="AB17" s="693"/>
+      <c r="AD17" s="680"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13467,58 +13482,61 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="672"/>
-      <c r="G18" s="674"/>
+      <c r="F18" s="705"/>
+      <c r="G18" s="707"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="692"/>
+      <c r="K18" s="686"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="535"/>
+      <c r="S18" s="536"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="700"/>
-      <c r="AB18" s="701"/>
-      <c r="AD18" s="686"/>
+      <c r="AA18" s="694"/>
+      <c r="AB18" s="695"/>
+      <c r="AD18" s="680"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="675"/>
-      <c r="K19" s="693"/>
+      <c r="G19" s="708"/>
+      <c r="K19" s="687"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="680" t="s">
+      <c r="R19" s="713" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="681"/>
-      <c r="T19" s="682"/>
+      <c r="S19" s="714"/>
+      <c r="T19" s="715"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="687"/>
+      <c r="AD19" s="681"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13530,14 +13548,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw - NewDelhi Updates_11:13PM
Rw - NewDelhi Updates

ShieldW Enabled for ND TV India

Alliance Partner :- Times Now
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF5D69E-6F41-407C-8D51-DC334E223587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EEA27C-658E-41C6-A91D-554941E9CD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="606">
   <si>
     <t>Zone</t>
   </si>
@@ -4793,6 +4793,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4823,62 +4880,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4904,12 +5066,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4931,161 +5087,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5144,15 +5153,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5171,25 +5171,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5267,46 +5288,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6538,7 +6538,7 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6595,7 +6595,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="565" t="s">
+      <c r="Q1" s="584" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6615,32 +6615,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="578">
+      <c r="A2" s="568">
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="B2" s="580" t="s">
+      <c r="B2" s="570" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="582" t="s">
+      <c r="D2" s="572" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="584" t="s">
+      <c r="E2" s="574" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="590" t="s">
+      <c r="G2" s="580" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="572" t="s">
+      <c r="I2" s="591" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6664,10 +6664,10 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="566"/>
+      <c r="Q2" s="585"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
@@ -6690,14 +6690,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="579"/>
-      <c r="B3" s="581"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="583"/>
-      <c r="E3" s="585"/>
-      <c r="G3" s="591"/>
+      <c r="A3" s="569"/>
+      <c r="B3" s="571"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="573"/>
+      <c r="E3" s="575"/>
+      <c r="G3" s="581"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="573"/>
+      <c r="I3" s="592"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6717,10 +6717,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="586" t="s">
+      <c r="C4" s="576" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="573"/>
+      <c r="I4" s="592"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
@@ -6728,8 +6728,12 @@
         <f>IF((R7-SUM(V2:V10)&lt;0),R7-SUM(V2:V10),0)</f>
         <v>0</v>
       </c>
-      <c r="U4" s="6"/>
-      <c r="V4" s="497"/>
+      <c r="U4" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="V4" s="497">
+        <v>1</v>
+      </c>
       <c r="W4" s="6" t="s">
         <v>252</v>
       </c>
@@ -6744,7 +6748,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="587"/>
+      <c r="C5" s="577"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6760,7 +6764,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="573"/>
+      <c r="I5" s="592"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6791,22 +6795,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="575" t="s">
+      <c r="A6" s="565" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="555"/>
-      <c r="I6" s="573"/>
+      <c r="I6" s="592"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="576"/>
+      <c r="A7" s="566"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6817,7 +6821,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="555"/>
-      <c r="I7" s="573"/>
+      <c r="I7" s="592"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6835,7 +6839,7 @@
       </c>
       <c r="R7" s="24">
         <f>3-R11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
@@ -6855,7 +6859,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="577"/>
+      <c r="A8" s="567"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6864,7 +6868,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="555"/>
-      <c r="I8" s="573"/>
+      <c r="I8" s="592"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6888,7 +6892,7 @@
       </c>
       <c r="G9" s="555"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="573"/>
+      <c r="I9" s="592"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6915,7 +6919,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="555"/>
-      <c r="I10" s="573"/>
+      <c r="I10" s="592"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6949,7 +6953,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="555"/>
-      <c r="I11" s="573"/>
+      <c r="I11" s="592"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6970,17 +6974,17 @@
         <v>44</v>
       </c>
       <c r="R11" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="567" t="s">
+      <c r="U11" s="586" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="568"/>
-      <c r="W11" s="568"/>
-      <c r="X11" s="569"/>
+      <c r="V11" s="587"/>
+      <c r="W11" s="587"/>
+      <c r="X11" s="588"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -6991,7 +6995,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="555"/>
-      <c r="I12" s="573"/>
+      <c r="I12" s="592"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7024,7 +7028,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="555"/>
-      <c r="I13" s="573"/>
+      <c r="I13" s="592"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7065,7 +7069,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="573"/>
+      <c r="I14" s="592"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7083,7 +7087,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="573"/>
+      <c r="I15" s="592"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7114,7 +7118,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="573"/>
+      <c r="I16" s="592"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7148,7 +7152,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="573"/>
+      <c r="I17" s="592"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7160,13 +7164,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="573"/>
+      <c r="I18" s="592"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="570" t="s">
+      <c r="O18" s="589" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="571"/>
+      <c r="P18" s="590"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7192,7 +7196,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="573"/>
+      <c r="I19" s="592"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7220,7 +7224,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="573"/>
+      <c r="I20" s="592"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7241,7 +7245,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="573"/>
+      <c r="I21" s="592"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7273,7 +7277,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="573"/>
+      <c r="I22" s="592"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7293,13 +7297,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="573"/>
+      <c r="I23" s="592"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="573"/>
+      <c r="I24" s="592"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7327,7 +7331,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="573"/>
+      <c r="I25" s="592"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7372,7 +7376,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="573"/>
+      <c r="I26" s="592"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7407,7 +7411,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="573"/>
+      <c r="I27" s="592"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7434,7 +7438,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="573"/>
+      <c r="I28" s="592"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7456,7 +7460,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="574"/>
+      <c r="I29" s="593"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7524,6 +7528,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7535,11 +7544,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7549,7 +7553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7:K9"/>
     </sheetView>
   </sheetViews>
@@ -7615,7 +7619,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="590" t="s">
+      <c r="I1" s="580" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7676,7 +7680,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="621"/>
+      <c r="AN1" s="618"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7685,23 +7689,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="645">
+      <c r="A2" s="600">
         <f ca="1">TODAY()</f>
         <v>45278</v>
       </c>
-      <c r="B2" s="647" t="s">
+      <c r="B2" s="602" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="649" t="s">
+      <c r="D2" s="604" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="594" t="s">
+      <c r="E2" s="648" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="602" t="s">
+      <c r="F2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7710,31 +7714,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="591"/>
+      <c r="I2" s="581"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="596" t="s">
+      <c r="K2" s="650" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="597"/>
-      <c r="M2" s="602" t="s">
+      <c r="L2" s="651"/>
+      <c r="M2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="628" t="s">
+      <c r="O2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="592" t="s">
+      <c r="Q2" s="582" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="554"/>
-      <c r="S2" s="615" t="s">
+      <c r="S2" s="640" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7767,15 +7771,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="622"/>
+      <c r="AN2" s="619"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="646"/>
-      <c r="B3" s="648"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="650"/>
-      <c r="E3" s="595"/>
-      <c r="F3" s="603"/>
+      <c r="A3" s="601"/>
+      <c r="B3" s="603"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="605"/>
+      <c r="E3" s="649"/>
+      <c r="F3" s="624"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7794,17 +7798,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="603"/>
+      <c r="M3" s="624"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="629"/>
+      <c r="O3" s="628"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="593"/>
+      <c r="Q3" s="583"/>
       <c r="R3" s="556"/>
-      <c r="S3" s="617"/>
+      <c r="S3" s="641"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7821,7 +7825,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="612" t="s">
+      <c r="AD3" s="639" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7833,16 +7837,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="622"/>
+      <c r="AN3" s="619"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="661" t="s">
+      <c r="B4" s="616" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="592" t="s">
+      <c r="C4" s="582" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7851,7 +7855,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="603"/>
+      <c r="F4" s="624"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7868,11 +7872,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="603"/>
+      <c r="M4" s="624"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="629"/>
+      <c r="O4" s="628"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7899,7 +7903,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="612"/>
+      <c r="AD4" s="639"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7909,37 +7913,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="622"/>
+      <c r="AN4" s="619"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="580" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="662"/>
-      <c r="C5" s="593"/>
+      <c r="B5" s="617"/>
+      <c r="C5" s="583"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="603"/>
-      <c r="G5" s="653" t="s">
+      <c r="F5" s="624"/>
+      <c r="G5" s="608" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="653"/>
-      <c r="I5" s="653"/>
-      <c r="J5" s="653"/>
-      <c r="K5" s="653"/>
-      <c r="L5" s="654"/>
-      <c r="M5" s="603"/>
+      <c r="H5" s="608"/>
+      <c r="I5" s="608"/>
+      <c r="J5" s="608"/>
+      <c r="K5" s="608"/>
+      <c r="L5" s="609"/>
+      <c r="M5" s="624"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="629"/>
+      <c r="O5" s="628"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7970,24 +7974,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="622"/>
+      <c r="AN5" s="619"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="591"/>
-      <c r="B6" s="659" t="s">
+      <c r="A6" s="581"/>
+      <c r="B6" s="614" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
-      <c r="F6" s="603"/>
-      <c r="G6" s="655"/>
-      <c r="H6" s="655"/>
-      <c r="I6" s="655"/>
-      <c r="J6" s="655"/>
-      <c r="K6" s="655"/>
-      <c r="L6" s="656"/>
-      <c r="M6" s="603"/>
-      <c r="O6" s="629"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
+      <c r="F6" s="624"/>
+      <c r="G6" s="610"/>
+      <c r="H6" s="610"/>
+      <c r="I6" s="610"/>
+      <c r="J6" s="610"/>
+      <c r="K6" s="610"/>
+      <c r="L6" s="611"/>
+      <c r="M6" s="624"/>
+      <c r="O6" s="628"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8011,16 +8015,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="611"/>
+      <c r="AI6" s="633"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="611" t="s">
+      <c r="AK6" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="622"/>
+      <c r="AN6" s="619"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8029,7 +8033,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="660"/>
+      <c r="B7" s="615"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8039,7 +8043,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="603"/>
+      <c r="F7" s="624"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8058,8 +8062,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="603"/>
-      <c r="O7" s="629"/>
+      <c r="M7" s="624"/>
+      <c r="O7" s="628"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8083,18 +8087,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="612" t="s">
+      <c r="AG7" s="639" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="611"/>
+      <c r="AI7" s="633"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="611"/>
+      <c r="AK7" s="633"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="622"/>
+      <c r="AN7" s="619"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8111,27 +8115,27 @@
         <f>SUM(G7:N9)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="603"/>
-      <c r="G8" s="654">
-        <v>0</v>
-      </c>
-      <c r="H8" s="651" t="s">
+      <c r="F8" s="624"/>
+      <c r="G8" s="609">
+        <v>0</v>
+      </c>
+      <c r="H8" s="606" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="554">
         <v>0</v>
       </c>
-      <c r="J8" s="651" t="s">
+      <c r="J8" s="606" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="657"/>
-      <c r="L8" s="613"/>
-      <c r="M8" s="626"/>
-      <c r="N8" s="618">
+      <c r="K8" s="612"/>
+      <c r="L8" s="642"/>
+      <c r="M8" s="625"/>
+      <c r="N8" s="645">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="629"/>
+      <c r="O8" s="628"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8149,14 +8153,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="612"/>
+      <c r="AG8" s="639"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="611"/>
+      <c r="AI8" s="633"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="622"/>
+      <c r="AN8" s="619"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8171,17 +8175,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="603"/>
-      <c r="G9" s="656"/>
-      <c r="H9" s="652"/>
+      <c r="F9" s="624"/>
+      <c r="G9" s="611"/>
+      <c r="H9" s="607"/>
       <c r="I9" s="556"/>
-      <c r="J9" s="652"/>
-      <c r="K9" s="658"/>
-      <c r="L9" s="614"/>
-      <c r="M9" s="627"/>
-      <c r="N9" s="619"/>
-      <c r="O9" s="630"/>
-      <c r="S9" s="615" t="s">
+      <c r="J9" s="607"/>
+      <c r="K9" s="613"/>
+      <c r="L9" s="643"/>
+      <c r="M9" s="626"/>
+      <c r="N9" s="646"/>
+      <c r="O9" s="629"/>
+      <c r="S9" s="640" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8203,16 +8207,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="612"/>
+      <c r="AG9" s="639"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="611"/>
+      <c r="AI9" s="633"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="611" t="s">
+      <c r="AK9" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="622"/>
+      <c r="AN9" s="619"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8229,20 +8233,20 @@
         <f>Boat!U8</f>
         <v>42</v>
       </c>
-      <c r="F10" s="603"/>
+      <c r="F10" s="624"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="605" t="s">
+      <c r="O10" s="657" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="631" t="s">
+      <c r="P10" s="630" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="616"/>
+      <c r="S10" s="644"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8272,16 +8276,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="612"/>
+      <c r="AG10" s="639"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="611"/>
+      <c r="AI10" s="633"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="611"/>
+      <c r="AK10" s="633"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="622"/>
+      <c r="AN10" s="619"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8299,18 +8303,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="603"/>
+      <c r="F11" s="624"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="606"/>
-      <c r="P11" s="632"/>
+      <c r="O11" s="658"/>
+      <c r="P11" s="631"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="616"/>
+      <c r="S11" s="644"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8334,14 +8338,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="612"/>
+      <c r="AG11" s="639"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="622"/>
+      <c r="AN11" s="619"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8360,7 +8364,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="603"/>
+      <c r="F12" s="624"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8369,16 +8373,16 @@
       </c>
       <c r="I12" s="561"/>
       <c r="J12" s="561"/>
-      <c r="K12" s="610"/>
+      <c r="K12" s="662"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="606"/>
-      <c r="P12" s="632"/>
+      <c r="O12" s="658"/>
+      <c r="P12" s="631"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="617"/>
+      <c r="S12" s="641"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8399,16 +8403,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="620" t="s">
+      <c r="AD12" s="647" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="612" t="s">
+      <c r="AF12" s="639" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="612"/>
+      <c r="AG12" s="639"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8421,7 +8425,7 @@
       <c r="AM12" s="634" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="622"/>
+      <c r="AN12" s="619"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8433,17 +8437,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="603"/>
+      <c r="F13" s="624"/>
       <c r="G13" s="561" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="561"/>
       <c r="I13" s="561"/>
-      <c r="J13" s="610"/>
+      <c r="J13" s="662"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="606"/>
-      <c r="P13" s="633"/>
+      <c r="O13" s="658"/>
+      <c r="P13" s="632"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8464,8 +8468,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="620"/>
-      <c r="AF13" s="612"/>
+      <c r="AD13" s="647"/>
+      <c r="AF13" s="639"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8477,7 +8481,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="634"/>
-      <c r="AN13" s="622"/>
+      <c r="AN13" s="619"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8485,18 +8489,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="603"/>
+      <c r="F14" s="624"/>
       <c r="G14" s="561" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="561"/>
       <c r="I14" s="561"/>
-      <c r="J14" s="610"/>
+      <c r="J14" s="662"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="606"/>
+      <c r="O14" s="658"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8517,9 +8521,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="620"/>
+      <c r="AD14" s="647"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="612"/>
+      <c r="AF14" s="639"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8527,7 +8531,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="634"/>
-      <c r="AN14" s="622"/>
+      <c r="AN14" s="619"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8536,8 +8540,8 @@
       <c r="C15" s="554" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="603"/>
-      <c r="O15" s="606"/>
+      <c r="F15" s="624"/>
+      <c r="O15" s="658"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8559,8 +8563,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="620"/>
-      <c r="AF15" s="612"/>
+      <c r="AD15" s="647"/>
+      <c r="AF15" s="639"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8574,7 +8578,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="634"/>
-      <c r="AN15" s="622"/>
+      <c r="AN15" s="619"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8596,13 +8600,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="603"/>
+      <c r="F16" s="624"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="606"/>
+      <c r="O16" s="658"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8634,18 +8638,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="622"/>
+      <c r="AN16" s="619"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="603"/>
+      <c r="F17" s="624"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="606"/>
+      <c r="O17" s="658"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8690,7 +8694,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="622"/>
+      <c r="AN17" s="619"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8714,21 +8718,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="603"/>
+      <c r="F18" s="624"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="606"/>
+      <c r="O18" s="658"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="598" t="s">
+      <c r="R18" s="652" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="642" t="s">
+      <c r="U18" s="597" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8749,7 +8753,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="611" t="s">
+      <c r="AF18" s="633" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8761,20 +8765,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="622"/>
+      <c r="AN18" s="619"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="603"/>
+      <c r="F19" s="624"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="606"/>
-      <c r="R19" s="599"/>
+      <c r="O19" s="658"/>
+      <c r="R19" s="653"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="643"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8789,7 +8793,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="611"/>
+      <c r="AF19" s="633"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8799,7 +8803,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="622"/>
+      <c r="AN19" s="619"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8820,19 +8824,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="603"/>
+      <c r="F20" s="624"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="606"/>
-      <c r="Q20" s="608" t="s">
+      <c r="O20" s="658"/>
+      <c r="Q20" s="660" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="644"/>
+      <c r="U20" s="599"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8862,7 +8866,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="622"/>
+      <c r="AN20" s="619"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8883,13 +8887,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="603"/>
+      <c r="F21" s="624"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="606"/>
-      <c r="Q21" s="609"/>
+      <c r="O21" s="658"/>
+      <c r="Q21" s="661"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="639"/>
+      <c r="V21" s="594"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8927,15 +8931,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="622"/>
+      <c r="AN21" s="619"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="603"/>
+      <c r="F22" s="624"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="606"/>
+      <c r="O22" s="658"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8943,7 +8947,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="640"/>
+      <c r="V22" s="595"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -8961,7 +8965,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="611" t="s">
+      <c r="AJ22" s="633" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -8969,7 +8973,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="622"/>
+      <c r="AN22" s="619"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -8987,17 +8991,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="603"/>
+      <c r="F23" s="624"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="606"/>
-      <c r="Q23" s="608" t="s">
+      <c r="O23" s="658"/>
+      <c r="Q23" s="660" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="640"/>
+      <c r="V23" s="595"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9013,13 +9017,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="611"/>
+      <c r="AJ23" s="633"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="622"/>
+      <c r="AN23" s="619"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9037,18 +9041,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="603"/>
+      <c r="F24" s="624"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="606"/>
-      <c r="Q24" s="609"/>
+      <c r="O24" s="658"/>
+      <c r="Q24" s="661"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="640"/>
+      <c r="V24" s="595"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9072,12 +9076,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="622"/>
+      <c r="AN24" s="619"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="603"/>
+      <c r="F25" s="624"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="606"/>
+      <c r="O25" s="658"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9090,7 +9094,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="641"/>
+      <c r="V25" s="596"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9112,7 +9116,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="622"/>
+      <c r="AN25" s="619"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9130,17 +9134,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="603"/>
+      <c r="F26" s="624"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="606"/>
-      <c r="P26" s="624" t="s">
+      <c r="O26" s="658"/>
+      <c r="P26" s="621" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="625"/>
-      <c r="R26" s="600" t="s">
+      <c r="Q26" s="622"/>
+      <c r="R26" s="654" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9179,7 +9183,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="622"/>
+      <c r="AN26" s="619"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9191,13 +9195,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="604"/>
+      <c r="F27" s="656"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="607"/>
-      <c r="R27" s="601"/>
+      <c r="O27" s="659"/>
+      <c r="R27" s="655"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9227,10 +9231,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="623"/>
+      <c r="AN27" s="620"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9247,44 +9289,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9294,8 +9298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AH30" sqref="AH30"/>
+    <sheetView tabSelected="1" topLeftCell="N18" workbookViewId="0">
+      <selection activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9390,10 +9394,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="666" t="s">
+      <c r="V1" s="669" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="667"/>
+      <c r="W1" s="670"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9409,21 +9413,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="668" t="s">
+      <c r="AC1" s="671" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="669"/>
-      <c r="AE1" s="670"/>
-      <c r="AF1" s="671" t="s">
+      <c r="AD1" s="672"/>
+      <c r="AE1" s="673"/>
+      <c r="AF1" s="674" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="672"/>
-      <c r="AH1" s="673"/>
-      <c r="AI1" s="663" t="s">
+      <c r="AG1" s="675"/>
+      <c r="AH1" s="676"/>
+      <c r="AI1" s="666" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="664"/>
-      <c r="AK1" s="665"/>
+      <c r="AJ1" s="667"/>
+      <c r="AK1" s="668"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9440,19 +9444,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="674">
+      <c r="L2" s="677">
         <f>SUM(L5:L30)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="676">
+      <c r="M2" s="679">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="678">
+      <c r="N2" s="681">
         <f>SUM(N4:N29)</f>
         <v>4</v>
       </c>
-      <c r="O2" s="618">
+      <c r="O2" s="645">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-1</v>
       </c>
@@ -9471,7 +9475,7 @@
       <c r="T2" s="518" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="680" t="s">
+      <c r="U2" s="683" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="519" t="s">
@@ -9540,10 +9544,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="675"/>
-      <c r="M3" s="677"/>
-      <c r="N3" s="679"/>
-      <c r="O3" s="619"/>
+      <c r="L3" s="678"/>
+      <c r="M3" s="680"/>
+      <c r="N3" s="682"/>
+      <c r="O3" s="646"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9559,7 +9563,7 @@
         <f>SUM(T4:T29)</f>
         <v>42</v>
       </c>
-      <c r="U3" s="681"/>
+      <c r="U3" s="684"/>
       <c r="V3" s="522">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>8</v>
@@ -9658,7 +9662,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="682" t="s">
+      <c r="O4" s="663" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9737,7 +9741,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="683"/>
+      <c r="O5" s="664"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9825,7 +9829,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="683"/>
+      <c r="O6" s="664"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9917,7 +9921,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="683"/>
+      <c r="O7" s="664"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10023,7 +10027,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="683"/>
+      <c r="O8" s="664"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10107,7 +10111,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="683"/>
+      <c r="O9" s="664"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10203,7 +10207,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="683"/>
+      <c r="O10" s="664"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10284,7 +10288,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="683"/>
+      <c r="O11" s="664"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10344,7 +10348,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="654" t="s">
+      <c r="A12" s="609" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10353,7 +10357,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="608" t="s">
+      <c r="E12" s="660" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10372,7 +10376,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="683"/>
+      <c r="O12" s="664"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10440,14 +10444,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="656"/>
+      <c r="A13" s="611"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="609"/>
+      <c r="E13" s="661"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10470,7 +10474,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="683"/>
+      <c r="O13" s="664"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10543,7 +10547,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="683"/>
+      <c r="O14" s="664"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10640,7 +10644,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O15" s="683"/>
+      <c r="O15" s="664"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10725,7 +10729,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="683"/>
+      <c r="O16" s="664"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10821,7 +10825,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="683"/>
+      <c r="O17" s="664"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10905,7 +10909,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="683"/>
+      <c r="O18" s="664"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10986,7 +10990,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O19" s="683"/>
+      <c r="O19" s="664"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11082,11 +11086,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="684"/>
+      <c r="O20" s="665"/>
       <c r="P20" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="610"/>
+      <c r="Q20" s="662"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11321,7 +11325,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="661" t="s">
+      <c r="E23" s="616" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184">
@@ -11413,7 +11417,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="662"/>
+      <c r="E24" s="617"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11431,7 +11435,7 @@
       <c r="P24" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="610"/>
+      <c r="Q24" s="662"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12177,7 +12181,7 @@
       </c>
       <c r="N34" s="299">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" s="21" t="s">
         <v>342</v>
@@ -12202,44 +12206,48 @@
       <c r="X34" s="65"/>
       <c r="Y34" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z34" s="64">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AA34" s="64"/>
+        <v>2</v>
+      </c>
+      <c r="AA34" s="64">
+        <v>1</v>
+      </c>
       <c r="AB34" s="307">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC34" s="362"/>
+      <c r="AC34" s="362">
+        <v>1</v>
+      </c>
       <c r="AD34" s="366"/>
       <c r="AE34" s="367"/>
       <c r="AF34" s="325">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG34" s="348"/>
       <c r="AH34" s="326"/>
       <c r="AI34" s="347">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ34" s="315">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK34" s="316">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL34" s="6"/>
       <c r="AM34" s="321" t="s">
         <v>590</v>
       </c>
-      <c r="AN34" s="262" t="s">
-        <v>191</v>
+      <c r="AN34" s="142" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="35" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12486,12 +12494,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12501,6 +12503,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12537,12 +12545,12 @@
       <c r="B1" s="559" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="610"/>
+      <c r="C1" s="662"/>
       <c r="D1" s="209"/>
       <c r="J1" s="559" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="610"/>
+      <c r="K1" s="662"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12933,7 +12941,7 @@
       <c r="V1" s="559" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="610"/>
+      <c r="W1" s="662"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12952,7 +12960,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="698" t="s">
+      <c r="AD1" s="705" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12969,10 +12977,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="697" t="s">
+      <c r="F2" s="736" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="725" t="s">
+      <c r="G2" s="693" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13000,10 +13008,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="666" t="s">
+      <c r="V2" s="669" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="667"/>
+      <c r="W2" s="670"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13022,7 +13030,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="699"/>
+      <c r="AD2" s="706"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13041,8 +13049,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="658"/>
-      <c r="G3" s="726"/>
+      <c r="F3" s="613"/>
+      <c r="G3" s="694"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13053,13 +13061,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="735" t="s">
+      <c r="O3" s="703" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="717" t="s">
+      <c r="P3" s="724" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="718"/>
+      <c r="Q3" s="725"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13069,15 +13077,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="699"/>
+      <c r="AD3" s="706"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="726"/>
+      <c r="G4" s="694"/>
       <c r="H4" s="6"/>
       <c r="L4" s="688" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="736"/>
+      <c r="O4" s="704"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13091,8 +13099,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="561"/>
-      <c r="AA4" s="610"/>
-      <c r="AD4" s="699"/>
+      <c r="AA4" s="662"/>
+      <c r="AD4" s="706"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13107,21 +13115,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="726"/>
+      <c r="G5" s="694"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="704" t="s">
+      <c r="K5" s="711" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="719"/>
+      <c r="L5" s="726"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="736"/>
+      <c r="O5" s="704"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13137,11 +13145,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="707" t="s">
+      <c r="Y5" s="714" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="708"/>
-      <c r="AD5" s="699"/>
+      <c r="Z5" s="715"/>
+      <c r="AD5" s="706"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13151,16 +13159,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="726"/>
+      <c r="G6" s="694"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="705"/>
-      <c r="L6" s="719"/>
-      <c r="O6" s="736"/>
+      <c r="K6" s="712"/>
+      <c r="L6" s="726"/>
+      <c r="O6" s="704"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13170,23 +13178,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="699"/>
+      <c r="AD6" s="706"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="726"/>
+      <c r="G7" s="694"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="705"/>
-      <c r="L7" s="719"/>
+      <c r="K7" s="712"/>
+      <c r="L7" s="726"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="736"/>
+      <c r="O7" s="704"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="699"/>
+      <c r="AD7" s="706"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13199,7 +13207,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="726"/>
+      <c r="G8" s="694"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13209,41 +13217,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="705"/>
-      <c r="L8" s="719"/>
-      <c r="O8" s="736"/>
+      <c r="K8" s="712"/>
+      <c r="L8" s="726"/>
+      <c r="O8" s="704"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="701" t="s">
+      <c r="S8" s="708" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="702"/>
-      <c r="U8" s="702"/>
-      <c r="V8" s="702"/>
-      <c r="W8" s="702"/>
-      <c r="X8" s="702"/>
-      <c r="Y8" s="702"/>
-      <c r="Z8" s="702"/>
-      <c r="AA8" s="702"/>
-      <c r="AB8" s="702"/>
-      <c r="AC8" s="703"/>
-      <c r="AD8" s="699"/>
+      <c r="T8" s="709"/>
+      <c r="U8" s="709"/>
+      <c r="V8" s="709"/>
+      <c r="W8" s="709"/>
+      <c r="X8" s="709"/>
+      <c r="Y8" s="709"/>
+      <c r="Z8" s="709"/>
+      <c r="AA8" s="709"/>
+      <c r="AB8" s="709"/>
+      <c r="AC8" s="710"/>
+      <c r="AD8" s="706"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="691"/>
-      <c r="G9" s="726"/>
+      <c r="C9" s="730"/>
+      <c r="G9" s="694"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="705"/>
-      <c r="L9" s="729" t="s">
+      <c r="K9" s="712"/>
+      <c r="L9" s="697" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="730"/>
-      <c r="N9" s="731"/>
-      <c r="O9" s="736"/>
+      <c r="M9" s="698"/>
+      <c r="N9" s="699"/>
+      <c r="O9" s="704"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="699"/>
+      <c r="AD9" s="706"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="692"/>
+      <c r="C10" s="731"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13251,7 +13259,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="726"/>
+      <c r="G10" s="694"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13259,33 +13267,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="705"/>
-      <c r="M10" s="694" t="s">
+      <c r="K10" s="712"/>
+      <c r="M10" s="733" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="695"/>
-      <c r="O10" s="695"/>
-      <c r="P10" s="695"/>
-      <c r="Q10" s="695"/>
-      <c r="R10" s="695"/>
-      <c r="S10" s="695"/>
-      <c r="T10" s="695"/>
-      <c r="U10" s="695"/>
-      <c r="V10" s="695"/>
-      <c r="W10" s="695"/>
-      <c r="X10" s="695"/>
-      <c r="Y10" s="695"/>
-      <c r="Z10" s="695"/>
-      <c r="AA10" s="695"/>
-      <c r="AB10" s="695"/>
-      <c r="AC10" s="696"/>
-      <c r="AD10" s="699"/>
+      <c r="N10" s="734"/>
+      <c r="O10" s="734"/>
+      <c r="P10" s="734"/>
+      <c r="Q10" s="734"/>
+      <c r="R10" s="734"/>
+      <c r="S10" s="734"/>
+      <c r="T10" s="734"/>
+      <c r="U10" s="734"/>
+      <c r="V10" s="734"/>
+      <c r="W10" s="734"/>
+      <c r="X10" s="734"/>
+      <c r="Y10" s="734"/>
+      <c r="Z10" s="734"/>
+      <c r="AA10" s="734"/>
+      <c r="AB10" s="734"/>
+      <c r="AC10" s="735"/>
+      <c r="AD10" s="706"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="693"/>
-      <c r="G11" s="726"/>
+      <c r="C11" s="732"/>
+      <c r="G11" s="694"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="705"/>
+      <c r="K11" s="712"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13293,17 +13301,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="715" t="s">
+      <c r="Z11" s="722" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="716"/>
+      <c r="AA11" s="723"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="699"/>
+      <c r="AD11" s="706"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13316,7 +13324,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="726"/>
+      <c r="G12" s="694"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13324,8 +13332,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="705"/>
-      <c r="L12" s="720" t="s">
+      <c r="K12" s="712"/>
+      <c r="L12" s="727" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13356,25 +13364,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="709" t="s">
+      <c r="AA12" s="716" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="710"/>
+      <c r="AB12" s="717"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="699"/>
+      <c r="AD12" s="706"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="691"/>
-      <c r="G13" s="726"/>
-      <c r="K13" s="705"/>
-      <c r="L13" s="721"/>
+      <c r="C13" s="730"/>
+      <c r="G13" s="694"/>
+      <c r="K13" s="712"/>
+      <c r="L13" s="728"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="728" t="s">
+      <c r="Q13" s="696" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="625"/>
+      <c r="R13" s="622"/>
       <c r="S13" s="555"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13383,17 +13391,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="711"/>
-      <c r="AB13" s="712"/>
-      <c r="AD13" s="699"/>
+      <c r="AA13" s="718"/>
+      <c r="AB13" s="719"/>
+      <c r="AD13" s="706"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="693"/>
+      <c r="C14" s="732"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="726"/>
+      <c r="G14" s="694"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13401,8 +13409,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="705"/>
-      <c r="L14" s="721"/>
+      <c r="K14" s="712"/>
+      <c r="L14" s="728"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13423,9 +13431,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="711"/>
-      <c r="AB14" s="712"/>
-      <c r="AD14" s="699"/>
+      <c r="AA14" s="718"/>
+      <c r="AB14" s="719"/>
+      <c r="AD14" s="706"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13440,19 +13448,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="726"/>
+      <c r="G15" s="694"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="705"/>
-      <c r="L15" s="722"/>
-      <c r="Q15" s="728" t="s">
+      <c r="K15" s="712"/>
+      <c r="L15" s="729"/>
+      <c r="Q15" s="696" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="625"/>
+      <c r="R15" s="622"/>
       <c r="S15" s="555"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13461,14 +13469,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="711"/>
-      <c r="AB15" s="712"/>
-      <c r="AD15" s="699"/>
+      <c r="AA15" s="718"/>
+      <c r="AB15" s="719"/>
+      <c r="AD15" s="706"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="726"/>
-      <c r="K16" s="705"/>
+      <c r="G16" s="694"/>
+      <c r="K16" s="712"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13487,24 +13495,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="711"/>
-      <c r="AB16" s="712"/>
-      <c r="AD16" s="699"/>
+      <c r="AA16" s="718"/>
+      <c r="AB16" s="719"/>
+      <c r="AD16" s="706"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="723" t="s">
+      <c r="F17" s="691" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="726"/>
+      <c r="G17" s="694"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="705"/>
+      <c r="K17" s="712"/>
       <c r="S17" s="555"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13512,9 +13520,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="711"/>
-      <c r="AB17" s="712"/>
-      <c r="AD17" s="699"/>
+      <c r="AA17" s="718"/>
+      <c r="AB17" s="719"/>
+      <c r="AD17" s="706"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13524,15 +13532,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="724"/>
-      <c r="G18" s="726"/>
+      <c r="F18" s="692"/>
+      <c r="G18" s="694"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="705"/>
+      <c r="K18" s="712"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13543,42 +13551,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="713"/>
-      <c r="AB18" s="714"/>
-      <c r="AD18" s="699"/>
+      <c r="AA18" s="720"/>
+      <c r="AB18" s="721"/>
+      <c r="AD18" s="706"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="727"/>
-      <c r="K19" s="706"/>
+      <c r="G19" s="695"/>
+      <c r="K19" s="713"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="732" t="s">
+      <c r="R19" s="700" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="733"/>
-      <c r="T19" s="734"/>
+      <c r="S19" s="701"/>
+      <c r="T19" s="702"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="700"/>
+      <c r="AD19" s="707"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13590,11 +13595,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - NBC
Boat Enabled - NBC
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EEA27C-658E-41C6-A91D-554941E9CD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DACF1A7-62C1-4192-B284-7F614459AB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4793,6 +4793,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4850,34 +4880,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4952,140 +5087,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5096,63 +5153,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5171,46 +5171,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5288,25 +5267,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5601,7 +5601,7 @@
   <dimension ref="B1:V28"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,7 +5791,7 @@
         <v>228</v>
       </c>
       <c r="V5" s="19">
-        <v>5640</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5989,7 +5989,7 @@
         <v>227</v>
       </c>
       <c r="V11" s="64">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6537,8 +6537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6595,7 +6595,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="584" t="s">
+      <c r="Q1" s="565" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6615,32 +6615,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="568">
+      <c r="A2" s="578">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
-      </c>
-      <c r="B2" s="570" t="s">
+        <v>45279</v>
+      </c>
+      <c r="B2" s="580" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="582" t="s">
+      <c r="C2" s="592" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="572" t="s">
+      <c r="D2" s="582" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="574" t="s">
+      <c r="E2" s="584" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="580" t="s">
+      <c r="G2" s="590" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="591" t="s">
+      <c r="I2" s="572" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6664,7 +6664,7 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="585"/>
+      <c r="Q2" s="566"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6690,14 +6690,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="569"/>
-      <c r="B3" s="571"/>
-      <c r="C3" s="583"/>
-      <c r="D3" s="573"/>
-      <c r="E3" s="575"/>
-      <c r="G3" s="581"/>
+      <c r="A3" s="579"/>
+      <c r="B3" s="581"/>
+      <c r="C3" s="593"/>
+      <c r="D3" s="583"/>
+      <c r="E3" s="585"/>
+      <c r="G3" s="591"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="592"/>
+      <c r="I3" s="573"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6717,10 +6717,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="576" t="s">
+      <c r="C4" s="586" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="592"/>
+      <c r="I4" s="573"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
@@ -6748,7 +6748,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="577"/>
+      <c r="C5" s="587"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6764,7 +6764,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="592"/>
+      <c r="I5" s="573"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6795,22 +6795,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="565" t="s">
+      <c r="A6" s="575" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="578"/>
-      <c r="D6" s="579"/>
+      <c r="C6" s="588"/>
+      <c r="D6" s="589"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="555"/>
-      <c r="I6" s="592"/>
+      <c r="I6" s="573"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="566"/>
+      <c r="A7" s="576"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="555"/>
-      <c r="I7" s="592"/>
+      <c r="I7" s="573"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6859,7 +6859,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="567"/>
+      <c r="A8" s="577"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="555"/>
-      <c r="I8" s="592"/>
+      <c r="I8" s="573"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6892,7 +6892,7 @@
       </c>
       <c r="G9" s="555"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="592"/>
+      <c r="I9" s="573"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="555"/>
-      <c r="I10" s="592"/>
+      <c r="I10" s="573"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="555"/>
-      <c r="I11" s="592"/>
+      <c r="I11" s="573"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6979,12 +6979,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="586" t="s">
+      <c r="U11" s="567" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="587"/>
-      <c r="W11" s="587"/>
-      <c r="X11" s="588"/>
+      <c r="V11" s="568"/>
+      <c r="W11" s="568"/>
+      <c r="X11" s="569"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -6995,7 +6995,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="555"/>
-      <c r="I12" s="592"/>
+      <c r="I12" s="573"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="555"/>
-      <c r="I13" s="592"/>
+      <c r="I13" s="573"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7069,7 +7069,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="592"/>
+      <c r="I14" s="573"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7087,7 +7087,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="592"/>
+      <c r="I15" s="573"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7118,7 +7118,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="592"/>
+      <c r="I16" s="573"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7152,7 +7152,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="592"/>
+      <c r="I17" s="573"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7164,13 +7164,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="592"/>
+      <c r="I18" s="573"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="589" t="s">
+      <c r="O18" s="570" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="590"/>
+      <c r="P18" s="571"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7196,7 +7196,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="592"/>
+      <c r="I19" s="573"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7224,7 +7224,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="592"/>
+      <c r="I20" s="573"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7245,7 +7245,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="592"/>
+      <c r="I21" s="573"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7277,7 +7277,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="592"/>
+      <c r="I22" s="573"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7297,13 +7297,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="592"/>
+      <c r="I23" s="573"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="592"/>
+      <c r="I24" s="573"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7331,7 +7331,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="592"/>
+      <c r="I25" s="573"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7376,7 +7376,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="592"/>
+      <c r="I26" s="573"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7411,7 +7411,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="592"/>
+      <c r="I27" s="573"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7438,7 +7438,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="592"/>
+      <c r="I28" s="573"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7460,7 +7460,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="593"/>
+      <c r="I29" s="574"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7528,11 +7528,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7544,6 +7539,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7553,8 +7553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7619,7 +7619,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="580" t="s">
+      <c r="I1" s="590" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7680,7 +7680,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="618"/>
+      <c r="AN1" s="621"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7689,23 +7689,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="600">
+      <c r="A2" s="645">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
-      </c>
-      <c r="B2" s="602" t="s">
+        <v>45279</v>
+      </c>
+      <c r="B2" s="647" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="582" t="s">
+      <c r="C2" s="592" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="604" t="s">
+      <c r="D2" s="649" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="648" t="s">
+      <c r="E2" s="594" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="623" t="s">
+      <c r="F2" s="602" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7714,31 +7714,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="581"/>
+      <c r="I2" s="591"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="650" t="s">
+      <c r="K2" s="596" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="651"/>
-      <c r="M2" s="623" t="s">
+      <c r="L2" s="597"/>
+      <c r="M2" s="602" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="627" t="s">
+      <c r="O2" s="628" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="582" t="s">
+      <c r="Q2" s="592" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="554"/>
-      <c r="S2" s="640" t="s">
+      <c r="S2" s="615" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7771,15 +7771,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="619"/>
+      <c r="AN2" s="622"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="601"/>
-      <c r="B3" s="603"/>
-      <c r="C3" s="583"/>
-      <c r="D3" s="605"/>
-      <c r="E3" s="649"/>
-      <c r="F3" s="624"/>
+      <c r="A3" s="646"/>
+      <c r="B3" s="648"/>
+      <c r="C3" s="593"/>
+      <c r="D3" s="650"/>
+      <c r="E3" s="595"/>
+      <c r="F3" s="603"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7798,17 +7798,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="624"/>
+      <c r="M3" s="603"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="628"/>
+      <c r="O3" s="629"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="583"/>
+      <c r="Q3" s="593"/>
       <c r="R3" s="556"/>
-      <c r="S3" s="641"/>
+      <c r="S3" s="617"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7825,7 +7825,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="639" t="s">
+      <c r="AD3" s="612" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7837,16 +7837,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="619"/>
+      <c r="AN3" s="622"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="616" t="s">
+      <c r="B4" s="661" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="582" t="s">
+      <c r="C4" s="592" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7855,7 +7855,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="624"/>
+      <c r="F4" s="603"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7872,11 +7872,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="624"/>
+      <c r="M4" s="603"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="628"/>
+      <c r="O4" s="629"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7903,7 +7903,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="639"/>
+      <c r="AD4" s="612"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7913,37 +7913,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="619"/>
+      <c r="AN4" s="622"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="580" t="s">
+      <c r="A5" s="590" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="617"/>
-      <c r="C5" s="583"/>
+      <c r="B5" s="662"/>
+      <c r="C5" s="593"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="624"/>
-      <c r="G5" s="608" t="s">
+      <c r="F5" s="603"/>
+      <c r="G5" s="653" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="608"/>
-      <c r="I5" s="608"/>
-      <c r="J5" s="608"/>
-      <c r="K5" s="608"/>
-      <c r="L5" s="609"/>
-      <c r="M5" s="624"/>
+      <c r="H5" s="653"/>
+      <c r="I5" s="653"/>
+      <c r="J5" s="653"/>
+      <c r="K5" s="653"/>
+      <c r="L5" s="654"/>
+      <c r="M5" s="603"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="628"/>
+      <c r="O5" s="629"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7974,24 +7974,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="619"/>
+      <c r="AN5" s="622"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="581"/>
-      <c r="B6" s="614" t="s">
+      <c r="A6" s="591"/>
+      <c r="B6" s="659" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="578"/>
-      <c r="D6" s="579"/>
-      <c r="F6" s="624"/>
-      <c r="G6" s="610"/>
-      <c r="H6" s="610"/>
-      <c r="I6" s="610"/>
-      <c r="J6" s="610"/>
-      <c r="K6" s="610"/>
-      <c r="L6" s="611"/>
-      <c r="M6" s="624"/>
-      <c r="O6" s="628"/>
+      <c r="C6" s="588"/>
+      <c r="D6" s="589"/>
+      <c r="F6" s="603"/>
+      <c r="G6" s="655"/>
+      <c r="H6" s="655"/>
+      <c r="I6" s="655"/>
+      <c r="J6" s="655"/>
+      <c r="K6" s="655"/>
+      <c r="L6" s="656"/>
+      <c r="M6" s="603"/>
+      <c r="O6" s="629"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8015,16 +8015,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="633"/>
+      <c r="AI6" s="611"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="633" t="s">
+      <c r="AK6" s="611" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="619"/>
+      <c r="AN6" s="622"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8033,7 +8033,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="615"/>
+      <c r="B7" s="660"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8043,7 +8043,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="624"/>
+      <c r="F7" s="603"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8057,13 +8057,13 @@
         <v>0</v>
       </c>
       <c r="K7" s="554">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="624"/>
-      <c r="O7" s="628"/>
+      <c r="M7" s="603"/>
+      <c r="O7" s="629"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8087,18 +8087,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="639" t="s">
+      <c r="AG7" s="612" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="633"/>
+      <c r="AI7" s="611"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="633"/>
+      <c r="AK7" s="611"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="619"/>
+      <c r="AN7" s="622"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8113,29 +8113,29 @@
       <c r="D8" s="349"/>
       <c r="E8" s="249">
         <f>SUM(G7:N9)</f>
-        <v>16</v>
-      </c>
-      <c r="F8" s="624"/>
-      <c r="G8" s="609">
-        <v>0</v>
-      </c>
-      <c r="H8" s="606" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="603"/>
+      <c r="G8" s="654">
+        <v>0</v>
+      </c>
+      <c r="H8" s="651" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="554">
         <v>0</v>
       </c>
-      <c r="J8" s="606" t="s">
+      <c r="J8" s="651" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="612"/>
-      <c r="L8" s="642"/>
-      <c r="M8" s="625"/>
-      <c r="N8" s="645">
+      <c r="K8" s="657"/>
+      <c r="L8" s="613"/>
+      <c r="M8" s="626"/>
+      <c r="N8" s="618">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="628"/>
+      <c r="O8" s="629"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8153,14 +8153,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="639"/>
+      <c r="AG8" s="612"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="633"/>
+      <c r="AI8" s="611"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="619"/>
+      <c r="AN8" s="622"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8175,17 +8175,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="624"/>
-      <c r="G9" s="611"/>
-      <c r="H9" s="607"/>
+      <c r="F9" s="603"/>
+      <c r="G9" s="656"/>
+      <c r="H9" s="652"/>
       <c r="I9" s="556"/>
-      <c r="J9" s="607"/>
-      <c r="K9" s="613"/>
-      <c r="L9" s="643"/>
-      <c r="M9" s="626"/>
-      <c r="N9" s="646"/>
-      <c r="O9" s="629"/>
-      <c r="S9" s="640" t="s">
+      <c r="J9" s="652"/>
+      <c r="K9" s="658"/>
+      <c r="L9" s="614"/>
+      <c r="M9" s="627"/>
+      <c r="N9" s="619"/>
+      <c r="O9" s="630"/>
+      <c r="S9" s="615" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8207,16 +8207,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="639"/>
+      <c r="AG9" s="612"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="633"/>
+      <c r="AI9" s="611"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="633" t="s">
+      <c r="AK9" s="611" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="619"/>
+      <c r="AN9" s="622"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8233,20 +8233,20 @@
         <f>Boat!U8</f>
         <v>42</v>
       </c>
-      <c r="F10" s="624"/>
+      <c r="F10" s="603"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="657" t="s">
+      <c r="O10" s="605" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="630" t="s">
+      <c r="P10" s="631" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="644"/>
+      <c r="S10" s="616"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8276,16 +8276,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="639"/>
+      <c r="AG10" s="612"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="633"/>
+      <c r="AI10" s="611"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="633"/>
+      <c r="AK10" s="611"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="619"/>
+      <c r="AN10" s="622"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8303,18 +8303,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="624"/>
+      <c r="F11" s="603"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="658"/>
-      <c r="P11" s="631"/>
+      <c r="O11" s="606"/>
+      <c r="P11" s="632"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="644"/>
+      <c r="S11" s="616"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8338,14 +8338,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="639"/>
+      <c r="AG11" s="612"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="619"/>
+      <c r="AN11" s="622"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8364,7 +8364,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="624"/>
+      <c r="F12" s="603"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8373,16 +8373,16 @@
       </c>
       <c r="I12" s="561"/>
       <c r="J12" s="561"/>
-      <c r="K12" s="662"/>
+      <c r="K12" s="610"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="658"/>
-      <c r="P12" s="631"/>
+      <c r="O12" s="606"/>
+      <c r="P12" s="632"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="641"/>
+      <c r="S12" s="617"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8403,16 +8403,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="647" t="s">
+      <c r="AD12" s="620" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="639" t="s">
+      <c r="AF12" s="612" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="639"/>
+      <c r="AG12" s="612"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8425,7 +8425,7 @@
       <c r="AM12" s="634" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="619"/>
+      <c r="AN12" s="622"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8437,17 +8437,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="624"/>
+      <c r="F13" s="603"/>
       <c r="G13" s="561" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="561"/>
       <c r="I13" s="561"/>
-      <c r="J13" s="662"/>
+      <c r="J13" s="610"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="658"/>
-      <c r="P13" s="632"/>
+      <c r="O13" s="606"/>
+      <c r="P13" s="633"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8468,8 +8468,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="647"/>
-      <c r="AF13" s="639"/>
+      <c r="AD13" s="620"/>
+      <c r="AF13" s="612"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8481,7 +8481,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="634"/>
-      <c r="AN13" s="619"/>
+      <c r="AN13" s="622"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8489,18 +8489,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="624"/>
+      <c r="F14" s="603"/>
       <c r="G14" s="561" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="561"/>
       <c r="I14" s="561"/>
-      <c r="J14" s="662"/>
+      <c r="J14" s="610"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="658"/>
+      <c r="O14" s="606"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8521,9 +8521,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="647"/>
+      <c r="AD14" s="620"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="639"/>
+      <c r="AF14" s="612"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8531,7 +8531,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="634"/>
-      <c r="AN14" s="619"/>
+      <c r="AN14" s="622"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8540,8 +8540,8 @@
       <c r="C15" s="554" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="624"/>
-      <c r="O15" s="658"/>
+      <c r="F15" s="603"/>
+      <c r="O15" s="606"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8563,8 +8563,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="647"/>
-      <c r="AF15" s="639"/>
+      <c r="AD15" s="620"/>
+      <c r="AF15" s="612"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8578,7 +8578,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="634"/>
-      <c r="AN15" s="619"/>
+      <c r="AN15" s="622"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8600,13 +8600,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="624"/>
+      <c r="F16" s="603"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="658"/>
+      <c r="O16" s="606"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8638,18 +8638,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="619"/>
+      <c r="AN16" s="622"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="624"/>
+      <c r="F17" s="603"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="658"/>
+      <c r="O17" s="606"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8694,7 +8694,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="619"/>
+      <c r="AN17" s="622"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8718,21 +8718,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="624"/>
+      <c r="F18" s="603"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="658"/>
+      <c r="O18" s="606"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="652" t="s">
+      <c r="R18" s="598" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="597" t="s">
+      <c r="U18" s="642" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8753,7 +8753,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="633" t="s">
+      <c r="AF18" s="611" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8765,20 +8765,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="619"/>
+      <c r="AN18" s="622"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="624"/>
+      <c r="F19" s="603"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="658"/>
-      <c r="R19" s="653"/>
+      <c r="O19" s="606"/>
+      <c r="R19" s="599"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="598"/>
+      <c r="U19" s="643"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8793,7 +8793,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="633"/>
+      <c r="AF19" s="611"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8803,7 +8803,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="619"/>
+      <c r="AN19" s="622"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8824,19 +8824,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="624"/>
+      <c r="F20" s="603"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="658"/>
-      <c r="Q20" s="660" t="s">
+      <c r="O20" s="606"/>
+      <c r="Q20" s="608" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="599"/>
+      <c r="U20" s="644"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8866,7 +8866,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="619"/>
+      <c r="AN20" s="622"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8887,13 +8887,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="624"/>
+      <c r="F21" s="603"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="658"/>
-      <c r="Q21" s="661"/>
+      <c r="O21" s="606"/>
+      <c r="Q21" s="609"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="594"/>
+      <c r="V21" s="639"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8931,15 +8931,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="619"/>
+      <c r="AN21" s="622"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="624"/>
+      <c r="F22" s="603"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="658"/>
+      <c r="O22" s="606"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="595"/>
+      <c r="V22" s="640"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -8965,7 +8965,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="633" t="s">
+      <c r="AJ22" s="611" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -8973,7 +8973,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="619"/>
+      <c r="AN22" s="622"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -8991,17 +8991,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="624"/>
+      <c r="F23" s="603"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="658"/>
-      <c r="Q23" s="660" t="s">
+      <c r="O23" s="606"/>
+      <c r="Q23" s="608" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="595"/>
+      <c r="V23" s="640"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9017,13 +9017,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="633"/>
+      <c r="AJ23" s="611"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="619"/>
+      <c r="AN23" s="622"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9041,18 +9041,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="624"/>
+      <c r="F24" s="603"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="658"/>
-      <c r="Q24" s="661"/>
+      <c r="O24" s="606"/>
+      <c r="Q24" s="609"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="595"/>
+      <c r="V24" s="640"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9076,12 +9076,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="619"/>
+      <c r="AN24" s="622"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="624"/>
+      <c r="F25" s="603"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="658"/>
+      <c r="O25" s="606"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9094,7 +9094,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="596"/>
+      <c r="V25" s="641"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9116,7 +9116,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="619"/>
+      <c r="AN25" s="622"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9134,17 +9134,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="624"/>
+      <c r="F26" s="603"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="658"/>
-      <c r="P26" s="621" t="s">
+      <c r="O26" s="606"/>
+      <c r="P26" s="624" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="622"/>
-      <c r="R26" s="654" t="s">
+      <c r="Q26" s="625"/>
+      <c r="R26" s="600" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9183,7 +9183,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="619"/>
+      <c r="AN26" s="622"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9195,13 +9195,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="656"/>
+      <c r="F27" s="604"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="659"/>
-      <c r="R27" s="655"/>
+      <c r="O27" s="607"/>
+      <c r="R27" s="601"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9231,32 +9231,26 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="620"/>
+      <c r="AN27" s="623"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9273,22 +9267,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9299,7 +9299,7 @@
   <dimension ref="A1:AN37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N18" workbookViewId="0">
-      <selection activeCell="AD34" sqref="AD34"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9389,15 +9389,15 @@
       </c>
       <c r="R1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="669" t="s">
+      <c r="V1" s="666" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="670"/>
+      <c r="W1" s="667"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9413,21 +9413,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="671" t="s">
+      <c r="AC1" s="668" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="672"/>
-      <c r="AE1" s="673"/>
-      <c r="AF1" s="674" t="s">
+      <c r="AD1" s="669"/>
+      <c r="AE1" s="670"/>
+      <c r="AF1" s="671" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="675"/>
-      <c r="AH1" s="676"/>
-      <c r="AI1" s="666" t="s">
+      <c r="AG1" s="672"/>
+      <c r="AH1" s="673"/>
+      <c r="AI1" s="663" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="667"/>
-      <c r="AK1" s="668"/>
+      <c r="AJ1" s="664"/>
+      <c r="AK1" s="665"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9444,21 +9444,21 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="677">
+      <c r="L2" s="674">
         <f>SUM(L5:L30)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="679">
+      <c r="M2" s="676">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="681">
+      <c r="N2" s="678">
         <f>SUM(N4:N29)</f>
         <v>4</v>
       </c>
-      <c r="O2" s="645">
+      <c r="O2" s="618">
         <f>SUM(M30:M37)* (-1)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="P2" s="275" t="s">
         <v>243</v>
@@ -9475,7 +9475,7 @@
       <c r="T2" s="518" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="683" t="s">
+      <c r="U2" s="680" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="519" t="s">
@@ -9544,10 +9544,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="678"/>
-      <c r="M3" s="680"/>
-      <c r="N3" s="682"/>
-      <c r="O3" s="646"/>
+      <c r="L3" s="675"/>
+      <c r="M3" s="677"/>
+      <c r="N3" s="679"/>
+      <c r="O3" s="619"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9563,7 +9563,7 @@
         <f>SUM(T4:T29)</f>
         <v>42</v>
       </c>
-      <c r="U3" s="684"/>
+      <c r="U3" s="681"/>
       <c r="V3" s="522">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>8</v>
@@ -9662,7 +9662,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="663" t="s">
+      <c r="O4" s="682" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9741,7 +9741,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="664"/>
+      <c r="O5" s="683"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9829,7 +9829,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="664"/>
+      <c r="O6" s="683"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9921,7 +9921,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="664"/>
+      <c r="O7" s="683"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10027,7 +10027,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="664"/>
+      <c r="O8" s="683"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10111,7 +10111,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="664"/>
+      <c r="O9" s="683"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10207,7 +10207,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="664"/>
+      <c r="O10" s="683"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10288,7 +10288,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="664"/>
+      <c r="O11" s="683"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10348,7 +10348,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="609" t="s">
+      <c r="A12" s="654" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10357,7 +10357,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="660" t="s">
+      <c r="E12" s="608" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10376,7 +10376,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="664"/>
+      <c r="O12" s="683"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10444,14 +10444,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="611"/>
+      <c r="A13" s="656"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="661"/>
+      <c r="E13" s="609"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10474,7 +10474,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="664"/>
+      <c r="O13" s="683"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10547,7 +10547,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="664"/>
+      <c r="O14" s="683"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10644,7 +10644,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O15" s="664"/>
+      <c r="O15" s="683"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10729,7 +10729,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="664"/>
+      <c r="O16" s="683"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10825,7 +10825,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="664"/>
+      <c r="O17" s="683"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10909,7 +10909,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="664"/>
+      <c r="O18" s="683"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10990,7 +10990,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O19" s="664"/>
+      <c r="O19" s="683"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11086,11 +11086,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="665"/>
+      <c r="O20" s="684"/>
       <c r="P20" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="662"/>
+      <c r="Q20" s="610"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11325,7 +11325,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="616" t="s">
+      <c r="E23" s="661" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184">
@@ -11417,7 +11417,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="617"/>
+      <c r="E24" s="662"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11435,7 +11435,7 @@
       <c r="P24" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="662"/>
+      <c r="Q24" s="610"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12027,10 +12027,12 @@
       </c>
       <c r="K32" s="406"/>
       <c r="L32" s="345"/>
-      <c r="M32" s="255"/>
+      <c r="M32" s="255">
+        <v>1</v>
+      </c>
       <c r="N32" s="299">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="20"/>
       <c r="R32" s="17" t="s">
@@ -12040,7 +12042,7 @@
         <v>2</v>
       </c>
       <c r="T32" s="157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U32" s="15">
         <v>-2</v>
@@ -12050,48 +12052,48 @@
       </c>
       <c r="W32" s="188">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X32" s="65"/>
       <c r="Y32" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32" s="64">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA32" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB32" s="307">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC32" s="362">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32" s="366"/>
       <c r="AE32" s="367"/>
       <c r="AF32" s="325">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG32" s="348">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH32" s="326"/>
       <c r="AI32" s="347">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ32" s="315">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK32" s="316">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL32" s="6" t="s">
         <v>467</v>
@@ -12105,7 +12107,9 @@
     </row>
     <row r="33" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G33" s="513"/>
-      <c r="H33" s="42"/>
+      <c r="H33" s="42">
+        <v>-1</v>
+      </c>
       <c r="I33" s="21" t="s">
         <v>512</v>
       </c>
@@ -12410,7 +12414,7 @@
     </row>
     <row r="37" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H37" s="544">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="K37" s="407"/>
       <c r="L37" s="346"/>
@@ -12494,6 +12498,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12503,12 +12513,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12545,12 +12549,12 @@
       <c r="B1" s="559" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="662"/>
+      <c r="C1" s="610"/>
       <c r="D1" s="209"/>
       <c r="J1" s="559" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="662"/>
+      <c r="K1" s="610"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12936,12 +12940,12 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
       <c r="V1" s="559" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="662"/>
+      <c r="W1" s="610"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12960,7 +12964,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="705" t="s">
+      <c r="AD1" s="698" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12977,10 +12981,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="736" t="s">
+      <c r="F2" s="697" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="693" t="s">
+      <c r="G2" s="725" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13008,10 +13012,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="669" t="s">
+      <c r="V2" s="666" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="670"/>
+      <c r="W2" s="667"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13030,7 +13034,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="706"/>
+      <c r="AD2" s="699"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13049,8 +13053,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="613"/>
-      <c r="G3" s="694"/>
+      <c r="F3" s="658"/>
+      <c r="G3" s="726"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13061,13 +13065,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="703" t="s">
+      <c r="O3" s="735" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="724" t="s">
+      <c r="P3" s="717" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="725"/>
+      <c r="Q3" s="718"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13077,15 +13081,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="706"/>
+      <c r="AD3" s="699"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="694"/>
+      <c r="G4" s="726"/>
       <c r="H4" s="6"/>
       <c r="L4" s="688" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="704"/>
+      <c r="O4" s="736"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13099,8 +13103,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="561"/>
-      <c r="AA4" s="662"/>
-      <c r="AD4" s="706"/>
+      <c r="AA4" s="610"/>
+      <c r="AD4" s="699"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13115,21 +13119,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="694"/>
+      <c r="G5" s="726"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="711" t="s">
+      <c r="K5" s="704" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="726"/>
+      <c r="L5" s="719"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="704"/>
+      <c r="O5" s="736"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13145,11 +13149,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="714" t="s">
+      <c r="Y5" s="707" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="715"/>
-      <c r="AD5" s="706"/>
+      <c r="Z5" s="708"/>
+      <c r="AD5" s="699"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13159,16 +13163,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="694"/>
+      <c r="G6" s="726"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="712"/>
-      <c r="L6" s="726"/>
-      <c r="O6" s="704"/>
+      <c r="K6" s="705"/>
+      <c r="L6" s="719"/>
+      <c r="O6" s="736"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13178,23 +13182,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="706"/>
+      <c r="AD6" s="699"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="694"/>
+      <c r="G7" s="726"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="712"/>
-      <c r="L7" s="726"/>
+      <c r="K7" s="705"/>
+      <c r="L7" s="719"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="704"/>
+      <c r="O7" s="736"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="706"/>
+      <c r="AD7" s="699"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13207,7 +13211,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="694"/>
+      <c r="G8" s="726"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13217,41 +13221,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="712"/>
-      <c r="L8" s="726"/>
-      <c r="O8" s="704"/>
+      <c r="K8" s="705"/>
+      <c r="L8" s="719"/>
+      <c r="O8" s="736"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="708" t="s">
+      <c r="S8" s="701" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="709"/>
-      <c r="U8" s="709"/>
-      <c r="V8" s="709"/>
-      <c r="W8" s="709"/>
-      <c r="X8" s="709"/>
-      <c r="Y8" s="709"/>
-      <c r="Z8" s="709"/>
-      <c r="AA8" s="709"/>
-      <c r="AB8" s="709"/>
-      <c r="AC8" s="710"/>
-      <c r="AD8" s="706"/>
+      <c r="T8" s="702"/>
+      <c r="U8" s="702"/>
+      <c r="V8" s="702"/>
+      <c r="W8" s="702"/>
+      <c r="X8" s="702"/>
+      <c r="Y8" s="702"/>
+      <c r="Z8" s="702"/>
+      <c r="AA8" s="702"/>
+      <c r="AB8" s="702"/>
+      <c r="AC8" s="703"/>
+      <c r="AD8" s="699"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="730"/>
-      <c r="G9" s="694"/>
+      <c r="C9" s="691"/>
+      <c r="G9" s="726"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="712"/>
-      <c r="L9" s="697" t="s">
+      <c r="K9" s="705"/>
+      <c r="L9" s="729" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="698"/>
-      <c r="N9" s="699"/>
-      <c r="O9" s="704"/>
+      <c r="M9" s="730"/>
+      <c r="N9" s="731"/>
+      <c r="O9" s="736"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="706"/>
+      <c r="AD9" s="699"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="731"/>
+      <c r="C10" s="692"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13259,7 +13263,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="694"/>
+      <c r="G10" s="726"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13267,33 +13271,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="712"/>
-      <c r="M10" s="733" t="s">
+      <c r="K10" s="705"/>
+      <c r="M10" s="694" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="734"/>
-      <c r="O10" s="734"/>
-      <c r="P10" s="734"/>
-      <c r="Q10" s="734"/>
-      <c r="R10" s="734"/>
-      <c r="S10" s="734"/>
-      <c r="T10" s="734"/>
-      <c r="U10" s="734"/>
-      <c r="V10" s="734"/>
-      <c r="W10" s="734"/>
-      <c r="X10" s="734"/>
-      <c r="Y10" s="734"/>
-      <c r="Z10" s="734"/>
-      <c r="AA10" s="734"/>
-      <c r="AB10" s="734"/>
-      <c r="AC10" s="735"/>
-      <c r="AD10" s="706"/>
+      <c r="N10" s="695"/>
+      <c r="O10" s="695"/>
+      <c r="P10" s="695"/>
+      <c r="Q10" s="695"/>
+      <c r="R10" s="695"/>
+      <c r="S10" s="695"/>
+      <c r="T10" s="695"/>
+      <c r="U10" s="695"/>
+      <c r="V10" s="695"/>
+      <c r="W10" s="695"/>
+      <c r="X10" s="695"/>
+      <c r="Y10" s="695"/>
+      <c r="Z10" s="695"/>
+      <c r="AA10" s="695"/>
+      <c r="AB10" s="695"/>
+      <c r="AC10" s="696"/>
+      <c r="AD10" s="699"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="732"/>
-      <c r="G11" s="694"/>
+      <c r="C11" s="693"/>
+      <c r="G11" s="726"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="712"/>
+      <c r="K11" s="705"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13301,17 +13305,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="722" t="s">
+      <c r="Z11" s="715" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="723"/>
+      <c r="AA11" s="716"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="706"/>
+      <c r="AD11" s="699"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13324,7 +13328,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="694"/>
+      <c r="G12" s="726"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13332,8 +13336,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="712"/>
-      <c r="L12" s="727" t="s">
+      <c r="K12" s="705"/>
+      <c r="L12" s="720" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13364,25 +13368,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="716" t="s">
+      <c r="AA12" s="709" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="717"/>
+      <c r="AB12" s="710"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="706"/>
+      <c r="AD12" s="699"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="730"/>
-      <c r="G13" s="694"/>
-      <c r="K13" s="712"/>
-      <c r="L13" s="728"/>
+      <c r="C13" s="691"/>
+      <c r="G13" s="726"/>
+      <c r="K13" s="705"/>
+      <c r="L13" s="721"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="696" t="s">
+      <c r="Q13" s="728" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="622"/>
+      <c r="R13" s="625"/>
       <c r="S13" s="555"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13391,17 +13395,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="718"/>
-      <c r="AB13" s="719"/>
-      <c r="AD13" s="706"/>
+      <c r="AA13" s="711"/>
+      <c r="AB13" s="712"/>
+      <c r="AD13" s="699"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="732"/>
+      <c r="C14" s="693"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="694"/>
+      <c r="G14" s="726"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13409,8 +13413,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="712"/>
-      <c r="L14" s="728"/>
+      <c r="K14" s="705"/>
+      <c r="L14" s="721"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13431,9 +13435,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="718"/>
-      <c r="AB14" s="719"/>
-      <c r="AD14" s="706"/>
+      <c r="AA14" s="711"/>
+      <c r="AB14" s="712"/>
+      <c r="AD14" s="699"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13448,19 +13452,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="694"/>
+      <c r="G15" s="726"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="712"/>
-      <c r="L15" s="729"/>
-      <c r="Q15" s="696" t="s">
+      <c r="K15" s="705"/>
+      <c r="L15" s="722"/>
+      <c r="Q15" s="728" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="622"/>
+      <c r="R15" s="625"/>
       <c r="S15" s="555"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13469,14 +13473,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="718"/>
-      <c r="AB15" s="719"/>
-      <c r="AD15" s="706"/>
+      <c r="AA15" s="711"/>
+      <c r="AB15" s="712"/>
+      <c r="AD15" s="699"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="694"/>
-      <c r="K16" s="712"/>
+      <c r="G16" s="726"/>
+      <c r="K16" s="705"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13495,24 +13499,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="718"/>
-      <c r="AB16" s="719"/>
-      <c r="AD16" s="706"/>
+      <c r="AA16" s="711"/>
+      <c r="AB16" s="712"/>
+      <c r="AD16" s="699"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="691" t="s">
+      <c r="F17" s="723" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="694"/>
+      <c r="G17" s="726"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="712"/>
+      <c r="K17" s="705"/>
       <c r="S17" s="555"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13520,9 +13524,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="718"/>
-      <c r="AB17" s="719"/>
-      <c r="AD17" s="706"/>
+      <c r="AA17" s="711"/>
+      <c r="AB17" s="712"/>
+      <c r="AD17" s="699"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13532,15 +13536,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="692"/>
-      <c r="G18" s="694"/>
+      <c r="F18" s="724"/>
+      <c r="G18" s="726"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="712"/>
+      <c r="K18" s="705"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13551,39 +13555,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="720"/>
-      <c r="AB18" s="721"/>
-      <c r="AD18" s="706"/>
+      <c r="AA18" s="713"/>
+      <c r="AB18" s="714"/>
+      <c r="AD18" s="699"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="695"/>
-      <c r="K19" s="713"/>
+      <c r="G19" s="727"/>
+      <c r="K19" s="706"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="700" t="s">
+      <c r="R19" s="732" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="701"/>
-      <c r="T19" s="702"/>
+      <c r="S19" s="733"/>
+      <c r="T19" s="734"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="707"/>
+      <c r="AD19" s="700"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13595,14 +13602,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw - Local Wbt Updates
Total = 12
BoardRw_Wbt :- [3M - 4F]
Boat_Reserved :-[5F]
Validity = 1 Day
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA897228-D79E-45EE-AED9-825511ADEF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256DD147-3B6C-4737-AD6D-6FBDB8753317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="608">
   <si>
     <t>Zone</t>
   </si>
@@ -1857,6 +1857,12 @@
   </si>
   <si>
     <t>Reserved</t>
+  </si>
+  <si>
+    <t>3M4F</t>
+  </si>
+  <si>
+    <t>1day WBt</t>
   </si>
 </sst>
 </file>
@@ -4793,6 +4799,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4823,62 +4886,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4904,12 +5072,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4931,161 +5093,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5144,15 +5159,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5171,25 +5177,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5267,46 +5294,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5598,10 +5604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:V28"/>
+  <dimension ref="B1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5625,7 +5631,7 @@
     <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.140625" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5712,7 +5718,7 @@
         <v>12</v>
       </c>
       <c r="O3" s="6"/>
-      <c r="P3" s="320">
+      <c r="P3" s="188">
         <v>1</v>
       </c>
       <c r="Q3" s="19" t="s">
@@ -5730,7 +5736,7 @@
       </c>
       <c r="V3" s="19">
         <f>SUM(P3:P28)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6124,7 +6130,7 @@
       <c r="P16" s="506"/>
       <c r="T16" s="563"/>
     </row>
-    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>224</v>
       </c>
@@ -6155,7 +6161,9 @@
       <c r="O17" s="504" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="321"/>
+      <c r="P17" s="321">
+        <v>1</v>
+      </c>
       <c r="Q17" s="19" t="s">
         <v>208</v>
       </c>
@@ -6167,11 +6175,11 @@
       </c>
       <c r="T17" s="563"/>
     </row>
-    <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="506"/>
       <c r="T18" s="563"/>
     </row>
-    <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>405</v>
       </c>
@@ -6206,7 +6214,7 @@
       <c r="P19" s="506"/>
       <c r="T19" s="563"/>
     </row>
-    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="246" t="s">
         <v>533</v>
       </c>
@@ -6237,7 +6245,7 @@
       <c r="P20" s="506"/>
       <c r="T20" s="563"/>
     </row>
-    <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="246" t="s">
         <v>27</v>
       </c>
@@ -6272,7 +6280,7 @@
       </c>
       <c r="V21" s="550"/>
     </row>
-    <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="276" t="s">
         <v>401</v>
       </c>
@@ -6303,7 +6311,7 @@
       <c r="P22" s="506"/>
       <c r="T22" s="563"/>
     </row>
-    <row r="23" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>434</v>
       </c>
@@ -6334,7 +6342,7 @@
       <c r="P23" s="506"/>
       <c r="T23" s="563"/>
     </row>
-    <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>534</v>
       </c>
@@ -6369,7 +6377,7 @@
       <c r="S24" s="16"/>
       <c r="T24" s="563"/>
     </row>
-    <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
@@ -6399,7 +6407,9 @@
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="P25" s="506"/>
+      <c r="P25" s="506">
+        <v>1</v>
+      </c>
       <c r="Q25" s="2" t="s">
         <v>594</v>
       </c>
@@ -6410,8 +6420,11 @@
         <v>1</v>
       </c>
       <c r="T25" s="563"/>
-    </row>
-    <row r="26" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V25" s="23" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>429</v>
       </c>
@@ -6441,8 +6454,11 @@
       </c>
       <c r="P26" s="506"/>
       <c r="T26" s="563"/>
-    </row>
-    <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W26" s="19" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="261" t="s">
         <v>406</v>
       </c>
@@ -6464,7 +6480,9 @@
       <c r="L27" s="414"/>
       <c r="M27" s="552"/>
       <c r="N27" s="61"/>
-      <c r="P27" s="321"/>
+      <c r="P27" s="321">
+        <v>1</v>
+      </c>
       <c r="Q27" s="2" t="s">
         <v>592</v>
       </c>
@@ -6476,7 +6494,7 @@
       </c>
       <c r="T27" s="563"/>
     </row>
-    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="261" t="s">
         <v>406</v>
       </c>
@@ -6506,7 +6524,9 @@
       <c r="N28" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="P28" s="508"/>
+      <c r="P28" s="508">
+        <v>1</v>
+      </c>
       <c r="Q28" s="2" t="s">
         <v>208</v>
       </c>
@@ -6595,7 +6615,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="565" t="s">
+      <c r="Q1" s="584" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6615,32 +6635,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="578">
+      <c r="A2" s="568">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="580" t="s">
+      <c r="B2" s="570" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="582" t="s">
+      <c r="D2" s="572" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="584" t="s">
+      <c r="E2" s="574" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="590" t="s">
+      <c r="G2" s="580" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="572" t="s">
+      <c r="I2" s="591" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6664,7 +6684,7 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="566"/>
+      <c r="Q2" s="585"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6682,22 +6702,22 @@
       <c r="X2" s="496"/>
       <c r="Z2" s="24">
         <f>BoardRW!V3</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AA2" s="68">
         <f>Z2+T2</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="579"/>
-      <c r="B3" s="581"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="583"/>
-      <c r="E3" s="585"/>
-      <c r="G3" s="591"/>
+      <c r="A3" s="569"/>
+      <c r="B3" s="571"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="573"/>
+      <c r="E3" s="575"/>
+      <c r="G3" s="581"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="573"/>
+      <c r="I3" s="592"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6717,10 +6737,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="586" t="s">
+      <c r="C4" s="576" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="573"/>
+      <c r="I4" s="592"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
@@ -6748,7 +6768,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="587"/>
+      <c r="C5" s="577"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6764,7 +6784,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="573"/>
+      <c r="I5" s="592"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6795,22 +6815,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="575" t="s">
+      <c r="A6" s="565" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="555"/>
-      <c r="I6" s="573"/>
+      <c r="I6" s="592"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="576"/>
+      <c r="A7" s="566"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6821,7 +6841,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="555"/>
-      <c r="I7" s="573"/>
+      <c r="I7" s="592"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6859,7 +6879,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="577"/>
+      <c r="A8" s="567"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6868,7 +6888,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="555"/>
-      <c r="I8" s="573"/>
+      <c r="I8" s="592"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6892,7 +6912,7 @@
       </c>
       <c r="G9" s="555"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="573"/>
+      <c r="I9" s="592"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6919,7 +6939,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="555"/>
-      <c r="I10" s="573"/>
+      <c r="I10" s="592"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6953,7 +6973,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="555"/>
-      <c r="I11" s="573"/>
+      <c r="I11" s="592"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6979,12 +6999,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="567" t="s">
+      <c r="U11" s="586" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="568"/>
-      <c r="W11" s="568"/>
-      <c r="X11" s="569"/>
+      <c r="V11" s="587"/>
+      <c r="W11" s="587"/>
+      <c r="X11" s="588"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -6995,7 +7015,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="555"/>
-      <c r="I12" s="573"/>
+      <c r="I12" s="592"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7028,7 +7048,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="555"/>
-      <c r="I13" s="573"/>
+      <c r="I13" s="592"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7069,7 +7089,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="573"/>
+      <c r="I14" s="592"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7087,7 +7107,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="573"/>
+      <c r="I15" s="592"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7118,7 +7138,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="573"/>
+      <c r="I16" s="592"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7152,7 +7172,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="573"/>
+      <c r="I17" s="592"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7164,13 +7184,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="573"/>
+      <c r="I18" s="592"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="570" t="s">
+      <c r="O18" s="589" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="571"/>
+      <c r="P18" s="590"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7196,7 +7216,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="573"/>
+      <c r="I19" s="592"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7224,7 +7244,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="573"/>
+      <c r="I20" s="592"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7245,7 +7265,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="573"/>
+      <c r="I21" s="592"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7277,7 +7297,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="573"/>
+      <c r="I22" s="592"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7297,13 +7317,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="573"/>
+      <c r="I23" s="592"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="573"/>
+      <c r="I24" s="592"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7331,7 +7351,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="573"/>
+      <c r="I25" s="592"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7376,7 +7396,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="573"/>
+      <c r="I26" s="592"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7411,7 +7431,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="573"/>
+      <c r="I27" s="592"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7438,7 +7458,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="573"/>
+      <c r="I28" s="592"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7460,7 +7480,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="574"/>
+      <c r="I29" s="593"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7528,6 +7548,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7539,11 +7564,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7619,7 +7639,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="590" t="s">
+      <c r="I1" s="580" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7680,7 +7700,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="621"/>
+      <c r="AN1" s="618"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7689,23 +7709,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="645">
+      <c r="A2" s="600">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="647" t="s">
+      <c r="B2" s="602" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="649" t="s">
+      <c r="D2" s="604" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="594" t="s">
+      <c r="E2" s="648" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="602" t="s">
+      <c r="F2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7714,31 +7734,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="591"/>
+      <c r="I2" s="581"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="596" t="s">
+      <c r="K2" s="650" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="597"/>
-      <c r="M2" s="602" t="s">
+      <c r="L2" s="651"/>
+      <c r="M2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="628" t="s">
+      <c r="O2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="592" t="s">
+      <c r="Q2" s="582" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="554"/>
-      <c r="S2" s="615" t="s">
+      <c r="S2" s="640" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7771,15 +7791,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="622"/>
+      <c r="AN2" s="619"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="646"/>
-      <c r="B3" s="648"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="650"/>
-      <c r="E3" s="595"/>
-      <c r="F3" s="603"/>
+      <c r="A3" s="601"/>
+      <c r="B3" s="603"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="605"/>
+      <c r="E3" s="649"/>
+      <c r="F3" s="624"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7798,17 +7818,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="603"/>
+      <c r="M3" s="624"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="629"/>
+      <c r="O3" s="628"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="593"/>
+      <c r="Q3" s="583"/>
       <c r="R3" s="556"/>
-      <c r="S3" s="617"/>
+      <c r="S3" s="641"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7825,7 +7845,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="612" t="s">
+      <c r="AD3" s="639" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7837,16 +7857,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="622"/>
+      <c r="AN3" s="619"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="661" t="s">
+      <c r="B4" s="616" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="592" t="s">
+      <c r="C4" s="582" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7855,7 +7875,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="603"/>
+      <c r="F4" s="624"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7872,11 +7892,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="603"/>
+      <c r="M4" s="624"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="629"/>
+      <c r="O4" s="628"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7903,7 +7923,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="612"/>
+      <c r="AD4" s="639"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7913,37 +7933,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="622"/>
+      <c r="AN4" s="619"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="580" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="662"/>
-      <c r="C5" s="593"/>
+      <c r="B5" s="617"/>
+      <c r="C5" s="583"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="603"/>
-      <c r="G5" s="653" t="s">
+      <c r="F5" s="624"/>
+      <c r="G5" s="608" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="653"/>
-      <c r="I5" s="653"/>
-      <c r="J5" s="653"/>
-      <c r="K5" s="653"/>
-      <c r="L5" s="654"/>
-      <c r="M5" s="603"/>
+      <c r="H5" s="608"/>
+      <c r="I5" s="608"/>
+      <c r="J5" s="608"/>
+      <c r="K5" s="608"/>
+      <c r="L5" s="609"/>
+      <c r="M5" s="624"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="629"/>
+      <c r="O5" s="628"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7974,24 +7994,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="622"/>
+      <c r="AN5" s="619"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="591"/>
-      <c r="B6" s="659" t="s">
+      <c r="A6" s="581"/>
+      <c r="B6" s="614" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
-      <c r="F6" s="603"/>
-      <c r="G6" s="655"/>
-      <c r="H6" s="655"/>
-      <c r="I6" s="655"/>
-      <c r="J6" s="655"/>
-      <c r="K6" s="655"/>
-      <c r="L6" s="656"/>
-      <c r="M6" s="603"/>
-      <c r="O6" s="629"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
+      <c r="F6" s="624"/>
+      <c r="G6" s="610"/>
+      <c r="H6" s="610"/>
+      <c r="I6" s="610"/>
+      <c r="J6" s="610"/>
+      <c r="K6" s="610"/>
+      <c r="L6" s="611"/>
+      <c r="M6" s="624"/>
+      <c r="O6" s="628"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8015,16 +8035,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="611"/>
+      <c r="AI6" s="633"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="611" t="s">
+      <c r="AK6" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="622"/>
+      <c r="AN6" s="619"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8033,7 +8053,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="660"/>
+      <c r="B7" s="615"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8043,7 +8063,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="603"/>
+      <c r="F7" s="624"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8062,8 +8082,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="603"/>
-      <c r="O7" s="629"/>
+      <c r="M7" s="624"/>
+      <c r="O7" s="628"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8087,18 +8107,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="612" t="s">
+      <c r="AG7" s="639" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="611"/>
+      <c r="AI7" s="633"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="611"/>
+      <c r="AK7" s="633"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="622"/>
+      <c r="AN7" s="619"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8115,27 +8135,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="603"/>
-      <c r="G8" s="654">
-        <v>0</v>
-      </c>
-      <c r="H8" s="651" t="s">
+      <c r="F8" s="624"/>
+      <c r="G8" s="609">
+        <v>0</v>
+      </c>
+      <c r="H8" s="606" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="554">
         <v>0</v>
       </c>
-      <c r="J8" s="651" t="s">
+      <c r="J8" s="606" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="657"/>
-      <c r="L8" s="613"/>
-      <c r="M8" s="626"/>
-      <c r="N8" s="618">
+      <c r="K8" s="612"/>
+      <c r="L8" s="642"/>
+      <c r="M8" s="625"/>
+      <c r="N8" s="645">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="629"/>
+      <c r="O8" s="628"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8153,14 +8173,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="612"/>
+      <c r="AG8" s="639"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="611"/>
+      <c r="AI8" s="633"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="622"/>
+      <c r="AN8" s="619"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8175,17 +8195,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="603"/>
-      <c r="G9" s="656"/>
-      <c r="H9" s="652"/>
+      <c r="F9" s="624"/>
+      <c r="G9" s="611"/>
+      <c r="H9" s="607"/>
       <c r="I9" s="556"/>
-      <c r="J9" s="652"/>
-      <c r="K9" s="658"/>
-      <c r="L9" s="614"/>
-      <c r="M9" s="627"/>
-      <c r="N9" s="619"/>
-      <c r="O9" s="630"/>
-      <c r="S9" s="615" t="s">
+      <c r="J9" s="607"/>
+      <c r="K9" s="613"/>
+      <c r="L9" s="643"/>
+      <c r="M9" s="626"/>
+      <c r="N9" s="646"/>
+      <c r="O9" s="629"/>
+      <c r="S9" s="640" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8207,16 +8227,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="612"/>
+      <c r="AG9" s="639"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="611"/>
+      <c r="AI9" s="633"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="611" t="s">
+      <c r="AK9" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="622"/>
+      <c r="AN9" s="619"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8233,20 +8253,20 @@
         <f>Boat!U8</f>
         <v>42</v>
       </c>
-      <c r="F10" s="603"/>
+      <c r="F10" s="624"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="605" t="s">
+      <c r="O10" s="657" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="631" t="s">
+      <c r="P10" s="630" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="616"/>
+      <c r="S10" s="644"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8276,16 +8296,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="612"/>
+      <c r="AG10" s="639"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="611"/>
+      <c r="AI10" s="633"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="611"/>
+      <c r="AK10" s="633"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="622"/>
+      <c r="AN10" s="619"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8303,18 +8323,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="603"/>
+      <c r="F11" s="624"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="606"/>
-      <c r="P11" s="632"/>
+      <c r="O11" s="658"/>
+      <c r="P11" s="631"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="616"/>
+      <c r="S11" s="644"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8338,14 +8358,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="612"/>
+      <c r="AG11" s="639"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="622"/>
+      <c r="AN11" s="619"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8364,7 +8384,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="603"/>
+      <c r="F12" s="624"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8373,16 +8393,16 @@
       </c>
       <c r="I12" s="561"/>
       <c r="J12" s="561"/>
-      <c r="K12" s="610"/>
+      <c r="K12" s="662"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="606"/>
-      <c r="P12" s="632"/>
+      <c r="O12" s="658"/>
+      <c r="P12" s="631"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="617"/>
+      <c r="S12" s="641"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8403,16 +8423,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="620" t="s">
+      <c r="AD12" s="647" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="612" t="s">
+      <c r="AF12" s="639" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="612"/>
+      <c r="AG12" s="639"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8425,7 +8445,7 @@
       <c r="AM12" s="634" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="622"/>
+      <c r="AN12" s="619"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8437,17 +8457,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="603"/>
+      <c r="F13" s="624"/>
       <c r="G13" s="561" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="561"/>
       <c r="I13" s="561"/>
-      <c r="J13" s="610"/>
+      <c r="J13" s="662"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="606"/>
-      <c r="P13" s="633"/>
+      <c r="O13" s="658"/>
+      <c r="P13" s="632"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8468,8 +8488,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="620"/>
-      <c r="AF13" s="612"/>
+      <c r="AD13" s="647"/>
+      <c r="AF13" s="639"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8481,7 +8501,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="634"/>
-      <c r="AN13" s="622"/>
+      <c r="AN13" s="619"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8489,18 +8509,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="603"/>
+      <c r="F14" s="624"/>
       <c r="G14" s="561" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="561"/>
       <c r="I14" s="561"/>
-      <c r="J14" s="610"/>
+      <c r="J14" s="662"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="606"/>
+      <c r="O14" s="658"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8521,9 +8541,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="620"/>
+      <c r="AD14" s="647"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="612"/>
+      <c r="AF14" s="639"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8531,7 +8551,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="634"/>
-      <c r="AN14" s="622"/>
+      <c r="AN14" s="619"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8540,8 +8560,8 @@
       <c r="C15" s="554" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="603"/>
-      <c r="O15" s="606"/>
+      <c r="F15" s="624"/>
+      <c r="O15" s="658"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8563,8 +8583,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="620"/>
-      <c r="AF15" s="612"/>
+      <c r="AD15" s="647"/>
+      <c r="AF15" s="639"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8578,7 +8598,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="634"/>
-      <c r="AN15" s="622"/>
+      <c r="AN15" s="619"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8600,13 +8620,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="603"/>
+      <c r="F16" s="624"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="606"/>
+      <c r="O16" s="658"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8638,18 +8658,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="622"/>
+      <c r="AN16" s="619"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="603"/>
+      <c r="F17" s="624"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="606"/>
+      <c r="O17" s="658"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8694,7 +8714,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="622"/>
+      <c r="AN17" s="619"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8718,21 +8738,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="603"/>
+      <c r="F18" s="624"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="606"/>
+      <c r="O18" s="658"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="598" t="s">
+      <c r="R18" s="652" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="642" t="s">
+      <c r="U18" s="597" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8753,7 +8773,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="611" t="s">
+      <c r="AF18" s="633" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8765,20 +8785,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="622"/>
+      <c r="AN18" s="619"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="603"/>
+      <c r="F19" s="624"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="606"/>
-      <c r="R19" s="599"/>
+      <c r="O19" s="658"/>
+      <c r="R19" s="653"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="643"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8793,7 +8813,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="611"/>
+      <c r="AF19" s="633"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8803,7 +8823,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="622"/>
+      <c r="AN19" s="619"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8824,19 +8844,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="603"/>
+      <c r="F20" s="624"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="606"/>
-      <c r="Q20" s="608" t="s">
+      <c r="O20" s="658"/>
+      <c r="Q20" s="660" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="644"/>
+      <c r="U20" s="599"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8866,7 +8886,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="622"/>
+      <c r="AN20" s="619"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8887,13 +8907,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="603"/>
+      <c r="F21" s="624"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="606"/>
-      <c r="Q21" s="609"/>
+      <c r="O21" s="658"/>
+      <c r="Q21" s="661"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="639"/>
+      <c r="V21" s="594"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8931,15 +8951,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="622"/>
+      <c r="AN21" s="619"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="603"/>
+      <c r="F22" s="624"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="606"/>
+      <c r="O22" s="658"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8947,7 +8967,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="640"/>
+      <c r="V22" s="595"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -8965,7 +8985,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="611" t="s">
+      <c r="AJ22" s="633" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -8973,7 +8993,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="622"/>
+      <c r="AN22" s="619"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -8991,17 +9011,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="603"/>
+      <c r="F23" s="624"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="606"/>
-      <c r="Q23" s="608" t="s">
+      <c r="O23" s="658"/>
+      <c r="Q23" s="660" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="640"/>
+      <c r="V23" s="595"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9017,13 +9037,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="611"/>
+      <c r="AJ23" s="633"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="622"/>
+      <c r="AN23" s="619"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9041,18 +9061,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="603"/>
+      <c r="F24" s="624"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="606"/>
-      <c r="Q24" s="609"/>
+      <c r="O24" s="658"/>
+      <c r="Q24" s="661"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="640"/>
+      <c r="V24" s="595"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9076,12 +9096,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="622"/>
+      <c r="AN24" s="619"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="603"/>
+      <c r="F25" s="624"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="606"/>
+      <c r="O25" s="658"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9094,7 +9114,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="641"/>
+      <c r="V25" s="596"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9116,7 +9136,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="622"/>
+      <c r="AN25" s="619"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9134,17 +9154,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="603"/>
+      <c r="F26" s="624"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="606"/>
-      <c r="P26" s="624" t="s">
+      <c r="O26" s="658"/>
+      <c r="P26" s="621" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="625"/>
-      <c r="R26" s="600" t="s">
+      <c r="Q26" s="622"/>
+      <c r="R26" s="654" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9183,7 +9203,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="622"/>
+      <c r="AN26" s="619"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9195,13 +9215,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="604"/>
+      <c r="F27" s="656"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="607"/>
-      <c r="R27" s="601"/>
+      <c r="O27" s="659"/>
+      <c r="R27" s="655"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9231,10 +9251,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="623"/>
+      <c r="AN27" s="620"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9251,44 +9309,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9298,8 +9318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AE17" sqref="AE17"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9394,10 +9414,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="666" t="s">
+      <c r="V1" s="669" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="667"/>
+      <c r="W1" s="670"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9413,21 +9433,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="668" t="s">
+      <c r="AC1" s="671" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="669"/>
-      <c r="AE1" s="670"/>
-      <c r="AF1" s="671" t="s">
+      <c r="AD1" s="672"/>
+      <c r="AE1" s="673"/>
+      <c r="AF1" s="674" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="672"/>
-      <c r="AH1" s="673"/>
-      <c r="AI1" s="663" t="s">
+      <c r="AG1" s="675"/>
+      <c r="AH1" s="676"/>
+      <c r="AI1" s="666" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="664"/>
-      <c r="AK1" s="665"/>
+      <c r="AJ1" s="667"/>
+      <c r="AK1" s="668"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9436,7 +9456,7 @@
       </c>
       <c r="H2" s="544">
         <f>SUM(H4:H37)</f>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>236</v>
@@ -9444,19 +9464,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="674">
+      <c r="L2" s="677">
         <f>SUM(L5:L30)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="676">
+      <c r="M2" s="679">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="678">
+      <c r="N2" s="681">
         <f>SUM(N4:N29)</f>
         <v>5</v>
       </c>
-      <c r="O2" s="618">
+      <c r="O2" s="645">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-2</v>
       </c>
@@ -9475,7 +9495,7 @@
       <c r="T2" s="518" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="680" t="s">
+      <c r="U2" s="683" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="519" t="s">
@@ -9544,10 +9564,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="675"/>
-      <c r="M3" s="677"/>
-      <c r="N3" s="679"/>
-      <c r="O3" s="619"/>
+      <c r="L3" s="678"/>
+      <c r="M3" s="680"/>
+      <c r="N3" s="682"/>
+      <c r="O3" s="646"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9563,7 +9583,7 @@
         <f>SUM(T4:T29)</f>
         <v>42</v>
       </c>
-      <c r="U3" s="681"/>
+      <c r="U3" s="684"/>
       <c r="V3" s="522">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>8</v>
@@ -9662,7 +9682,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="682" t="s">
+      <c r="O4" s="663" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9741,7 +9761,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="683"/>
+      <c r="O5" s="664"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9829,7 +9849,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="683"/>
+      <c r="O6" s="664"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9921,7 +9941,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="683"/>
+      <c r="O7" s="664"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10027,7 +10047,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="683"/>
+      <c r="O8" s="664"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10111,7 +10131,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="683"/>
+      <c r="O9" s="664"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10207,7 +10227,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="683"/>
+      <c r="O10" s="664"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10288,7 +10308,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="683"/>
+      <c r="O11" s="664"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10348,7 +10368,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="654" t="s">
+      <c r="A12" s="609" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10357,7 +10377,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="608" t="s">
+      <c r="E12" s="660" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10376,7 +10396,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="683"/>
+      <c r="O12" s="664"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10444,14 +10464,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="656"/>
+      <c r="A13" s="611"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="609"/>
+      <c r="E13" s="661"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10474,7 +10494,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="683"/>
+      <c r="O13" s="664"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10547,7 +10567,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="683"/>
+      <c r="O14" s="664"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10644,7 +10664,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="683"/>
+      <c r="O15" s="664"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10731,7 +10751,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="683"/>
+      <c r="O16" s="664"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10827,7 +10847,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="683"/>
+      <c r="O17" s="664"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10911,7 +10931,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="683"/>
+      <c r="O18" s="664"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10992,7 +11012,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O19" s="683"/>
+      <c r="O19" s="664"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11088,11 +11108,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="684"/>
+      <c r="O20" s="665"/>
       <c r="P20" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="610"/>
+      <c r="Q20" s="662"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11327,12 +11347,10 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="661" t="s">
+      <c r="E23" s="616" t="s">
         <v>294</v>
       </c>
-      <c r="F23" s="184">
-        <v>2</v>
-      </c>
+      <c r="F23" s="184"/>
       <c r="K23" s="403" t="s">
         <v>263</v>
       </c>
@@ -11419,7 +11437,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="662"/>
+      <c r="E24" s="617"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11437,7 +11455,7 @@
       <c r="P24" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="610"/>
+      <c r="Q24" s="662"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -11896,7 +11914,6 @@
     </row>
     <row r="30" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="274"/>
-      <c r="H30" s="274"/>
       <c r="I30" s="61" t="s">
         <v>511</v>
       </c>
@@ -11965,6 +11982,9 @@
       <c r="F31" s="100">
         <v>-1</v>
       </c>
+      <c r="H31" s="42">
+        <v>-5</v>
+      </c>
       <c r="I31" s="21" t="s">
         <v>436</v>
       </c>
@@ -12500,12 +12520,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12515,6 +12529,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12551,12 +12571,12 @@
       <c r="B1" s="559" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="610"/>
+      <c r="C1" s="662"/>
       <c r="D1" s="209"/>
       <c r="J1" s="559" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="610"/>
+      <c r="K1" s="662"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12890,7 +12910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F389A6-DF8C-48FB-B1F3-A2AFD91E9805}">
   <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
@@ -12947,7 +12967,7 @@
       <c r="V1" s="559" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="610"/>
+      <c r="W1" s="662"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12966,7 +12986,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="698" t="s">
+      <c r="AD1" s="705" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12983,10 +13003,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="697" t="s">
+      <c r="F2" s="736" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="725" t="s">
+      <c r="G2" s="693" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13014,10 +13034,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="666" t="s">
+      <c r="V2" s="669" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="667"/>
+      <c r="W2" s="670"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13036,7 +13056,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="699"/>
+      <c r="AD2" s="706"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13055,8 +13075,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="658"/>
-      <c r="G3" s="726"/>
+      <c r="F3" s="613"/>
+      <c r="G3" s="694"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13067,13 +13087,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="735" t="s">
+      <c r="O3" s="703" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="717" t="s">
+      <c r="P3" s="724" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="718"/>
+      <c r="Q3" s="725"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13083,15 +13103,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="699"/>
+      <c r="AD3" s="706"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="726"/>
+      <c r="G4" s="694"/>
       <c r="H4" s="6"/>
       <c r="L4" s="688" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="736"/>
+      <c r="O4" s="704"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13105,8 +13125,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="561"/>
-      <c r="AA4" s="610"/>
-      <c r="AD4" s="699"/>
+      <c r="AA4" s="662"/>
+      <c r="AD4" s="706"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13121,21 +13141,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="726"/>
+      <c r="G5" s="694"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="704" t="s">
+      <c r="K5" s="711" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="719"/>
+      <c r="L5" s="726"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="736"/>
+      <c r="O5" s="704"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13151,11 +13171,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="707" t="s">
+      <c r="Y5" s="714" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="708"/>
-      <c r="AD5" s="699"/>
+      <c r="Z5" s="715"/>
+      <c r="AD5" s="706"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13165,16 +13185,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="726"/>
+      <c r="G6" s="694"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="705"/>
-      <c r="L6" s="719"/>
-      <c r="O6" s="736"/>
+      <c r="K6" s="712"/>
+      <c r="L6" s="726"/>
+      <c r="O6" s="704"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13184,23 +13204,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="699"/>
+      <c r="AD6" s="706"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="726"/>
+      <c r="G7" s="694"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="705"/>
-      <c r="L7" s="719"/>
+      <c r="K7" s="712"/>
+      <c r="L7" s="726"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="736"/>
+      <c r="O7" s="704"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="699"/>
+      <c r="AD7" s="706"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13213,7 +13233,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="726"/>
+      <c r="G8" s="694"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13223,41 +13243,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="705"/>
-      <c r="L8" s="719"/>
-      <c r="O8" s="736"/>
+      <c r="K8" s="712"/>
+      <c r="L8" s="726"/>
+      <c r="O8" s="704"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="701" t="s">
+      <c r="S8" s="708" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="702"/>
-      <c r="U8" s="702"/>
-      <c r="V8" s="702"/>
-      <c r="W8" s="702"/>
-      <c r="X8" s="702"/>
-      <c r="Y8" s="702"/>
-      <c r="Z8" s="702"/>
-      <c r="AA8" s="702"/>
-      <c r="AB8" s="702"/>
-      <c r="AC8" s="703"/>
-      <c r="AD8" s="699"/>
+      <c r="T8" s="709"/>
+      <c r="U8" s="709"/>
+      <c r="V8" s="709"/>
+      <c r="W8" s="709"/>
+      <c r="X8" s="709"/>
+      <c r="Y8" s="709"/>
+      <c r="Z8" s="709"/>
+      <c r="AA8" s="709"/>
+      <c r="AB8" s="709"/>
+      <c r="AC8" s="710"/>
+      <c r="AD8" s="706"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="691"/>
-      <c r="G9" s="726"/>
+      <c r="C9" s="730"/>
+      <c r="G9" s="694"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="705"/>
-      <c r="L9" s="729" t="s">
+      <c r="K9" s="712"/>
+      <c r="L9" s="697" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="730"/>
-      <c r="N9" s="731"/>
-      <c r="O9" s="736"/>
+      <c r="M9" s="698"/>
+      <c r="N9" s="699"/>
+      <c r="O9" s="704"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="699"/>
+      <c r="AD9" s="706"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="692"/>
+      <c r="C10" s="731"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13265,7 +13285,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="726"/>
+      <c r="G10" s="694"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13273,33 +13293,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="705"/>
-      <c r="M10" s="694" t="s">
+      <c r="K10" s="712"/>
+      <c r="M10" s="733" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="695"/>
-      <c r="O10" s="695"/>
-      <c r="P10" s="695"/>
-      <c r="Q10" s="695"/>
-      <c r="R10" s="695"/>
-      <c r="S10" s="695"/>
-      <c r="T10" s="695"/>
-      <c r="U10" s="695"/>
-      <c r="V10" s="695"/>
-      <c r="W10" s="695"/>
-      <c r="X10" s="695"/>
-      <c r="Y10" s="695"/>
-      <c r="Z10" s="695"/>
-      <c r="AA10" s="695"/>
-      <c r="AB10" s="695"/>
-      <c r="AC10" s="696"/>
-      <c r="AD10" s="699"/>
+      <c r="N10" s="734"/>
+      <c r="O10" s="734"/>
+      <c r="P10" s="734"/>
+      <c r="Q10" s="734"/>
+      <c r="R10" s="734"/>
+      <c r="S10" s="734"/>
+      <c r="T10" s="734"/>
+      <c r="U10" s="734"/>
+      <c r="V10" s="734"/>
+      <c r="W10" s="734"/>
+      <c r="X10" s="734"/>
+      <c r="Y10" s="734"/>
+      <c r="Z10" s="734"/>
+      <c r="AA10" s="734"/>
+      <c r="AB10" s="734"/>
+      <c r="AC10" s="735"/>
+      <c r="AD10" s="706"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="693"/>
-      <c r="G11" s="726"/>
+      <c r="C11" s="732"/>
+      <c r="G11" s="694"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="705"/>
+      <c r="K11" s="712"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13307,17 +13327,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="715" t="s">
+      <c r="Z11" s="722" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="716"/>
+      <c r="AA11" s="723"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="699"/>
+      <c r="AD11" s="706"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13330,7 +13350,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="726"/>
+      <c r="G12" s="694"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13338,8 +13358,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="705"/>
-      <c r="L12" s="720" t="s">
+      <c r="K12" s="712"/>
+      <c r="L12" s="727" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13370,25 +13390,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="709" t="s">
+      <c r="AA12" s="716" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="710"/>
+      <c r="AB12" s="717"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="699"/>
+      <c r="AD12" s="706"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="691"/>
-      <c r="G13" s="726"/>
-      <c r="K13" s="705"/>
-      <c r="L13" s="721"/>
+      <c r="C13" s="730"/>
+      <c r="G13" s="694"/>
+      <c r="K13" s="712"/>
+      <c r="L13" s="728"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="728" t="s">
+      <c r="Q13" s="696" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="625"/>
+      <c r="R13" s="622"/>
       <c r="S13" s="555"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13397,17 +13417,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="711"/>
-      <c r="AB13" s="712"/>
-      <c r="AD13" s="699"/>
+      <c r="AA13" s="718"/>
+      <c r="AB13" s="719"/>
+      <c r="AD13" s="706"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="693"/>
+      <c r="C14" s="732"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="726"/>
+      <c r="G14" s="694"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13415,8 +13435,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="705"/>
-      <c r="L14" s="721"/>
+      <c r="K14" s="712"/>
+      <c r="L14" s="728"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13437,9 +13457,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="711"/>
-      <c r="AB14" s="712"/>
-      <c r="AD14" s="699"/>
+      <c r="AA14" s="718"/>
+      <c r="AB14" s="719"/>
+      <c r="AD14" s="706"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13454,19 +13474,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="726"/>
+      <c r="G15" s="694"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="705"/>
-      <c r="L15" s="722"/>
-      <c r="Q15" s="728" t="s">
+      <c r="K15" s="712"/>
+      <c r="L15" s="729"/>
+      <c r="Q15" s="696" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="625"/>
+      <c r="R15" s="622"/>
       <c r="S15" s="555"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13475,14 +13495,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="711"/>
-      <c r="AB15" s="712"/>
-      <c r="AD15" s="699"/>
+      <c r="AA15" s="718"/>
+      <c r="AB15" s="719"/>
+      <c r="AD15" s="706"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="726"/>
-      <c r="K16" s="705"/>
+      <c r="G16" s="694"/>
+      <c r="K16" s="712"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13501,24 +13521,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="711"/>
-      <c r="AB16" s="712"/>
-      <c r="AD16" s="699"/>
+      <c r="AA16" s="718"/>
+      <c r="AB16" s="719"/>
+      <c r="AD16" s="706"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="723" t="s">
+      <c r="F17" s="691" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="726"/>
+      <c r="G17" s="694"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="705"/>
+      <c r="K17" s="712"/>
       <c r="S17" s="555"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13526,9 +13546,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="711"/>
-      <c r="AB17" s="712"/>
-      <c r="AD17" s="699"/>
+      <c r="AA17" s="718"/>
+      <c r="AB17" s="719"/>
+      <c r="AD17" s="706"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13538,15 +13558,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="724"/>
-      <c r="G18" s="726"/>
+      <c r="F18" s="692"/>
+      <c r="G18" s="694"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="705"/>
+      <c r="K18" s="712"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13557,42 +13577,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="713"/>
-      <c r="AB18" s="714"/>
-      <c r="AD18" s="699"/>
+      <c r="AA18" s="720"/>
+      <c r="AB18" s="721"/>
+      <c r="AD18" s="706"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="727"/>
-      <c r="K19" s="706"/>
+      <c r="G19" s="695"/>
+      <c r="K19" s="713"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="732" t="s">
+      <c r="R19" s="700" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="733"/>
-      <c r="T19" s="734"/>
+      <c r="S19" s="701"/>
+      <c r="T19" s="702"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="700"/>
+      <c r="AD19" s="707"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13604,11 +13621,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - Polimer
Boat Enabled - Polimer News
</commit_message>
<xml_diff>
--- a/System_2.1.4.xlsx
+++ b/System_2.1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78954FAE-A184-441E-A3C4-92AA00B02AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE484F1D-FC6F-4348-8CE5-E44B0D76A848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -4802,6 +4802,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4832,62 +4889,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4913,12 +5075,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4940,161 +5096,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5153,15 +5162,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5180,25 +5180,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5276,46 +5297,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5609,8 +5609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6563,8 +6563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6621,7 +6621,7 @@
       <c r="P1" s="423" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="565" t="s">
+      <c r="Q1" s="584" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6641,32 +6641,32 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="578">
+      <c r="A2" s="568">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="580" t="s">
+      <c r="B2" s="570" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="582" t="s">
+      <c r="D2" s="572" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="584" t="s">
+      <c r="E2" s="574" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="590" t="s">
+      <c r="G2" s="580" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="572" t="s">
+      <c r="I2" s="591" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="421" t="s">
@@ -6690,7 +6690,7 @@
       <c r="P2" s="424">
         <v>40</v>
       </c>
-      <c r="Q2" s="566"/>
+      <c r="Q2" s="585"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>6</v>
@@ -6716,14 +6716,14 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="579"/>
-      <c r="B3" s="581"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="583"/>
-      <c r="E3" s="585"/>
-      <c r="G3" s="591"/>
+      <c r="A3" s="569"/>
+      <c r="B3" s="571"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="573"/>
+      <c r="E3" s="575"/>
+      <c r="G3" s="581"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="573"/>
+      <c r="I3" s="592"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6743,10 +6743,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="586" t="s">
+      <c r="C4" s="576" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="573"/>
+      <c r="I4" s="592"/>
       <c r="R4" s="499" t="s">
         <v>580</v>
       </c>
@@ -6774,7 +6774,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="587"/>
+      <c r="C5" s="577"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -6790,7 +6790,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="573"/>
+      <c r="I5" s="592"/>
       <c r="J5" s="422" t="s">
         <v>273</v>
       </c>
@@ -6821,22 +6821,22 @@
       <c r="X5" s="495"/>
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="575" t="s">
+      <c r="A6" s="565" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="555"/>
-      <c r="I6" s="573"/>
+      <c r="I6" s="592"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="576"/>
+      <c r="A7" s="566"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="555"/>
-      <c r="I7" s="573"/>
+      <c r="I7" s="592"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6874,9 +6874,7 @@
       <c r="U7" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="V7" s="496">
-        <v>1</v>
-      </c>
+      <c r="V7" s="496"/>
       <c r="W7" s="6" t="s">
         <v>528</v>
       </c>
@@ -6885,7 +6883,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="577"/>
+      <c r="A8" s="567"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -6894,7 +6892,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="555"/>
-      <c r="I8" s="573"/>
+      <c r="I8" s="592"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6918,7 +6916,7 @@
       </c>
       <c r="G9" s="555"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="573"/>
+      <c r="I9" s="592"/>
       <c r="M9" s="19" t="s">
         <v>547</v>
       </c>
@@ -6927,7 +6925,7 @@
         <v>247</v>
       </c>
       <c r="V9" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9" s="493"/>
     </row>
@@ -6945,7 +6943,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="555"/>
-      <c r="I10" s="573"/>
+      <c r="I10" s="592"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6979,7 +6977,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="555"/>
-      <c r="I11" s="573"/>
+      <c r="I11" s="592"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7005,12 +7003,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="U11" s="567" t="s">
+      <c r="U11" s="586" t="s">
         <v>583</v>
       </c>
-      <c r="V11" s="568"/>
-      <c r="W11" s="568"/>
-      <c r="X11" s="569"/>
+      <c r="V11" s="587"/>
+      <c r="W11" s="587"/>
+      <c r="X11" s="588"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7021,7 +7019,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="555"/>
-      <c r="I12" s="573"/>
+      <c r="I12" s="592"/>
       <c r="J12" s="24" t="s">
         <v>538</v>
       </c>
@@ -7054,7 +7052,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="555"/>
-      <c r="I13" s="573"/>
+      <c r="I13" s="592"/>
       <c r="J13" s="108" t="s">
         <v>572</v>
       </c>
@@ -7095,7 +7093,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="573"/>
+      <c r="I14" s="592"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -7113,7 +7111,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="573"/>
+      <c r="I15" s="592"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7144,7 +7142,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="573"/>
+      <c r="I16" s="592"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7178,7 +7176,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="573"/>
+      <c r="I17" s="592"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -7190,13 +7188,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="573"/>
+      <c r="I18" s="592"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="570" t="s">
+      <c r="O18" s="589" t="s">
         <v>539</v>
       </c>
-      <c r="P18" s="571"/>
+      <c r="P18" s="590"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7222,7 +7220,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="573"/>
+      <c r="I19" s="592"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7250,7 +7248,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="573"/>
+      <c r="I20" s="592"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7271,7 +7269,7 @@
       <c r="Z20" s="112"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="573"/>
+      <c r="I21" s="592"/>
       <c r="M21" s="221" t="s">
         <v>422</v>
       </c>
@@ -7303,7 +7301,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="573"/>
+      <c r="I22" s="592"/>
       <c r="U22" s="6"/>
       <c r="V22" s="495"/>
       <c r="W22" s="6" t="s">
@@ -7323,13 +7321,13 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="573"/>
+      <c r="I23" s="592"/>
       <c r="U23" s="6"/>
       <c r="V23" s="24"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="573"/>
+      <c r="I24" s="592"/>
       <c r="U24" s="354"/>
       <c r="V24" s="498">
         <v>-1</v>
@@ -7357,7 +7355,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="573"/>
+      <c r="I25" s="592"/>
       <c r="J25" s="422" t="s">
         <v>274</v>
       </c>
@@ -7402,7 +7400,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="573"/>
+      <c r="I26" s="592"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7437,7 +7435,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="573"/>
+      <c r="I27" s="592"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7464,7 +7462,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="573"/>
+      <c r="I28" s="592"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7486,7 +7484,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="574"/>
+      <c r="I29" s="593"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7554,6 +7552,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7565,11 +7568,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7645,7 +7643,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="590" t="s">
+      <c r="I1" s="580" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7706,7 +7704,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="427"/>
-      <c r="AN1" s="621"/>
+      <c r="AN1" s="618"/>
       <c r="AO1" s="350" t="s">
         <v>487</v>
       </c>
@@ -7715,23 +7713,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="645">
+      <c r="A2" s="600">
         <f ca="1">TODAY()</f>
         <v>45279</v>
       </c>
-      <c r="B2" s="647" t="s">
+      <c r="B2" s="602" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="592" t="s">
+      <c r="C2" s="582" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="649" t="s">
+      <c r="D2" s="604" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="594" t="s">
+      <c r="E2" s="648" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="602" t="s">
+      <c r="F2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="418" t="s">
@@ -7740,31 +7738,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="591"/>
+      <c r="I2" s="581"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="596" t="s">
+      <c r="K2" s="650" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="597"/>
-      <c r="M2" s="602" t="s">
+      <c r="L2" s="651"/>
+      <c r="M2" s="623" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="628" t="s">
+      <c r="O2" s="627" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="592" t="s">
+      <c r="Q2" s="582" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="554"/>
-      <c r="S2" s="615" t="s">
+      <c r="S2" s="640" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7797,15 +7795,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="453"/>
-      <c r="AN2" s="622"/>
+      <c r="AN2" s="619"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="646"/>
-      <c r="B3" s="648"/>
-      <c r="C3" s="593"/>
-      <c r="D3" s="650"/>
-      <c r="E3" s="595"/>
-      <c r="F3" s="603"/>
+      <c r="A3" s="601"/>
+      <c r="B3" s="603"/>
+      <c r="C3" s="583"/>
+      <c r="D3" s="605"/>
+      <c r="E3" s="649"/>
+      <c r="F3" s="624"/>
       <c r="G3" s="419" t="s">
         <v>28</v>
       </c>
@@ -7824,17 +7822,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="603"/>
+      <c r="M3" s="624"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="629"/>
+      <c r="O3" s="628"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="593"/>
+      <c r="Q3" s="583"/>
       <c r="R3" s="556"/>
-      <c r="S3" s="617"/>
+      <c r="S3" s="641"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7851,7 +7849,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="612" t="s">
+      <c r="AD3" s="639" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="262"/>
@@ -7863,16 +7861,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="453"/>
-      <c r="AN3" s="622"/>
+      <c r="AN3" s="619"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="661" t="s">
+      <c r="B4" s="616" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="592" t="s">
+      <c r="C4" s="582" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -7881,7 +7879,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="603"/>
+      <c r="F4" s="624"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -7898,11 +7896,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="603"/>
+      <c r="M4" s="624"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="629"/>
+      <c r="O4" s="628"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7929,7 +7927,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="612"/>
+      <c r="AD4" s="639"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -7939,37 +7937,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="453"/>
-      <c r="AN4" s="622"/>
+      <c r="AN4" s="619"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="580" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="662"/>
-      <c r="C5" s="593"/>
+      <c r="B5" s="617"/>
+      <c r="C5" s="583"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="603"/>
-      <c r="G5" s="653" t="s">
+      <c r="F5" s="624"/>
+      <c r="G5" s="608" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="653"/>
-      <c r="I5" s="653"/>
-      <c r="J5" s="653"/>
-      <c r="K5" s="653"/>
-      <c r="L5" s="654"/>
-      <c r="M5" s="603"/>
+      <c r="H5" s="608"/>
+      <c r="I5" s="608"/>
+      <c r="J5" s="608"/>
+      <c r="K5" s="608"/>
+      <c r="L5" s="609"/>
+      <c r="M5" s="624"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="629"/>
+      <c r="O5" s="628"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8000,24 +7998,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="453"/>
-      <c r="AN5" s="622"/>
+      <c r="AN5" s="619"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="591"/>
-      <c r="B6" s="659" t="s">
+      <c r="A6" s="581"/>
+      <c r="B6" s="614" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
-      <c r="F6" s="603"/>
-      <c r="G6" s="655"/>
-      <c r="H6" s="655"/>
-      <c r="I6" s="655"/>
-      <c r="J6" s="655"/>
-      <c r="K6" s="655"/>
-      <c r="L6" s="656"/>
-      <c r="M6" s="603"/>
-      <c r="O6" s="629"/>
+      <c r="C6" s="578"/>
+      <c r="D6" s="579"/>
+      <c r="F6" s="624"/>
+      <c r="G6" s="610"/>
+      <c r="H6" s="610"/>
+      <c r="I6" s="610"/>
+      <c r="J6" s="610"/>
+      <c r="K6" s="610"/>
+      <c r="L6" s="611"/>
+      <c r="M6" s="624"/>
+      <c r="O6" s="628"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8041,16 +8039,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="611"/>
+      <c r="AI6" s="633"/>
       <c r="AJ6" s="466" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="611" t="s">
+      <c r="AK6" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="453"/>
-      <c r="AN6" s="622"/>
+      <c r="AN6" s="619"/>
       <c r="AO6" s="350" t="s">
         <v>488</v>
       </c>
@@ -8059,7 +8057,7 @@
       <c r="A7" s="237" t="s">
         <v>598</v>
       </c>
-      <c r="B7" s="660"/>
+      <c r="B7" s="615"/>
       <c r="C7" s="207" t="s">
         <v>383</v>
       </c>
@@ -8069,7 +8067,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="603"/>
+      <c r="F7" s="624"/>
       <c r="G7" s="420">
         <v>0</v>
       </c>
@@ -8088,8 +8086,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="603"/>
-      <c r="O7" s="629"/>
+      <c r="M7" s="624"/>
+      <c r="O7" s="628"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8113,18 +8111,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="612" t="s">
+      <c r="AG7" s="639" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="611"/>
+      <c r="AI7" s="633"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="611"/>
+      <c r="AK7" s="633"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="453"/>
-      <c r="AN7" s="622"/>
+      <c r="AN7" s="619"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -8141,27 +8139,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="603"/>
-      <c r="G8" s="654">
-        <v>0</v>
-      </c>
-      <c r="H8" s="651" t="s">
+      <c r="F8" s="624"/>
+      <c r="G8" s="609">
+        <v>0</v>
+      </c>
+      <c r="H8" s="606" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="554">
         <v>0</v>
       </c>
-      <c r="J8" s="651" t="s">
+      <c r="J8" s="606" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="657"/>
-      <c r="L8" s="613"/>
-      <c r="M8" s="626"/>
-      <c r="N8" s="618">
+      <c r="K8" s="612"/>
+      <c r="L8" s="642"/>
+      <c r="M8" s="625"/>
+      <c r="N8" s="645">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="629"/>
+      <c r="O8" s="628"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8179,14 +8177,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="612"/>
+      <c r="AG8" s="639"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="611"/>
+      <c r="AI8" s="633"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="453"/>
-      <c r="AN8" s="622"/>
+      <c r="AN8" s="619"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8201,17 +8199,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="603"/>
-      <c r="G9" s="656"/>
-      <c r="H9" s="652"/>
+      <c r="F9" s="624"/>
+      <c r="G9" s="611"/>
+      <c r="H9" s="607"/>
       <c r="I9" s="556"/>
-      <c r="J9" s="652"/>
-      <c r="K9" s="658"/>
-      <c r="L9" s="614"/>
-      <c r="M9" s="627"/>
-      <c r="N9" s="619"/>
-      <c r="O9" s="630"/>
-      <c r="S9" s="615" t="s">
+      <c r="J9" s="607"/>
+      <c r="K9" s="613"/>
+      <c r="L9" s="643"/>
+      <c r="M9" s="626"/>
+      <c r="N9" s="646"/>
+      <c r="O9" s="629"/>
+      <c r="S9" s="640" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8233,16 +8231,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="612"/>
+      <c r="AG9" s="639"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="611"/>
+      <c r="AI9" s="633"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="611" t="s">
+      <c r="AK9" s="633" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="453"/>
-      <c r="AN9" s="622"/>
+      <c r="AN9" s="619"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8259,20 +8257,20 @@
         <f>Boat!U8</f>
         <v>42</v>
       </c>
-      <c r="F10" s="603"/>
+      <c r="F10" s="624"/>
       <c r="N10" s="443" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="605" t="s">
+      <c r="O10" s="657" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="631" t="s">
+      <c r="P10" s="630" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="616"/>
+      <c r="S10" s="644"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8302,16 +8300,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="612"/>
+      <c r="AG10" s="639"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="611"/>
+      <c r="AI10" s="633"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="611"/>
+      <c r="AK10" s="633"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="622"/>
+      <c r="AN10" s="619"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8329,18 +8327,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="603"/>
+      <c r="F11" s="624"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="606"/>
-      <c r="P11" s="632"/>
+      <c r="O11" s="658"/>
+      <c r="P11" s="631"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="616"/>
+      <c r="S11" s="644"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8364,14 +8362,14 @@
       <c r="AF11" s="262" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="612"/>
+      <c r="AG11" s="639"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="453"/>
-      <c r="AN11" s="622"/>
+      <c r="AN11" s="619"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8390,7 +8388,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="603"/>
+      <c r="F12" s="624"/>
       <c r="G12" s="349" t="s">
         <v>411</v>
       </c>
@@ -8399,16 +8397,16 @@
       </c>
       <c r="I12" s="561"/>
       <c r="J12" s="561"/>
-      <c r="K12" s="610"/>
+      <c r="K12" s="662"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="606"/>
-      <c r="P12" s="632"/>
+      <c r="O12" s="658"/>
+      <c r="P12" s="631"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="617"/>
+      <c r="S12" s="641"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8429,16 +8427,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="620" t="s">
+      <c r="AD12" s="647" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="466" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="612" t="s">
+      <c r="AF12" s="639" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="612"/>
+      <c r="AG12" s="639"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8451,7 +8449,7 @@
       <c r="AM12" s="634" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="622"/>
+      <c r="AN12" s="619"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8463,17 +8461,17 @@
       <c r="E13" s="473">
         <v>-3</v>
       </c>
-      <c r="F13" s="603"/>
+      <c r="F13" s="624"/>
       <c r="G13" s="561" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="561"/>
       <c r="I13" s="561"/>
-      <c r="J13" s="610"/>
+      <c r="J13" s="662"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="606"/>
-      <c r="P13" s="633"/>
+      <c r="O13" s="658"/>
+      <c r="P13" s="632"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8494,8 +8492,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="620"/>
-      <c r="AF13" s="612"/>
+      <c r="AD13" s="647"/>
+      <c r="AF13" s="639"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8507,7 +8505,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="634"/>
-      <c r="AN13" s="622"/>
+      <c r="AN13" s="619"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="475"/>
@@ -8515,18 +8513,18 @@
       <c r="C14" s="484"/>
       <c r="D14" s="477"/>
       <c r="E14" s="478"/>
-      <c r="F14" s="603"/>
+      <c r="F14" s="624"/>
       <c r="G14" s="561" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="561"/>
       <c r="I14" s="561"/>
-      <c r="J14" s="610"/>
+      <c r="J14" s="662"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="606"/>
+      <c r="O14" s="658"/>
       <c r="Q14" s="61" t="s">
         <v>555</v>
       </c>
@@ -8547,9 +8545,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="620"/>
+      <c r="AD14" s="647"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="612"/>
+      <c r="AF14" s="639"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8557,7 +8555,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="634"/>
-      <c r="AN14" s="622"/>
+      <c r="AN14" s="619"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="474" t="s">
@@ -8566,8 +8564,8 @@
       <c r="C15" s="554" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="603"/>
-      <c r="O15" s="606"/>
+      <c r="F15" s="624"/>
+      <c r="O15" s="658"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8589,8 +8587,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="620"/>
-      <c r="AF15" s="612"/>
+      <c r="AD15" s="647"/>
+      <c r="AF15" s="639"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>466</v>
@@ -8604,7 +8602,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="634"/>
-      <c r="AN15" s="622"/>
+      <c r="AN15" s="619"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8626,13 +8624,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="603"/>
+      <c r="F16" s="624"/>
       <c r="G16" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="496"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="606"/>
+      <c r="O16" s="658"/>
       <c r="R16" s="460" t="s">
         <v>185</v>
       </c>
@@ -8664,18 +8662,18 @@
       <c r="AM16" s="453" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="622"/>
+      <c r="AN16" s="619"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="603"/>
+      <c r="F17" s="624"/>
       <c r="I17" s="497"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="606"/>
+      <c r="O17" s="658"/>
       <c r="Q17" s="21" t="s">
         <v>553</v>
       </c>
@@ -8720,7 +8718,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="453"/>
-      <c r="AN17" s="622"/>
+      <c r="AN17" s="619"/>
       <c r="AO17" s="209" t="s">
         <v>516</v>
       </c>
@@ -8744,21 +8742,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="603"/>
+      <c r="F18" s="624"/>
       <c r="G18" s="349" t="s">
         <v>550</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="606"/>
+      <c r="O18" s="658"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="598" t="s">
+      <c r="R18" s="652" t="s">
         <v>558</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="642" t="s">
+      <c r="U18" s="597" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8779,7 +8777,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="611" t="s">
+      <c r="AF18" s="633" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="262"/>
@@ -8791,20 +8789,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="453"/>
-      <c r="AN18" s="622"/>
+      <c r="AN18" s="619"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="603"/>
+      <c r="F19" s="624"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="606"/>
-      <c r="R19" s="599"/>
+      <c r="O19" s="658"/>
+      <c r="R19" s="653"/>
       <c r="S19" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="U19" s="643"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="456" t="s">
@@ -8819,7 +8817,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="611"/>
+      <c r="AF19" s="633"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -8829,7 +8827,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="453"/>
-      <c r="AN19" s="622"/>
+      <c r="AN19" s="619"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8850,19 +8848,19 @@
       <c r="E20" s="462">
         <v>-1</v>
       </c>
-      <c r="F20" s="603"/>
+      <c r="F20" s="624"/>
       <c r="G20" s="349" t="s">
         <v>509</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="606"/>
-      <c r="Q20" s="608" t="s">
+      <c r="O20" s="658"/>
+      <c r="Q20" s="660" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="429" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="644"/>
+      <c r="U20" s="599"/>
       <c r="W20" s="430"/>
       <c r="X20" s="457" t="s">
         <v>175</v>
@@ -8892,7 +8890,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="622"/>
+      <c r="AN20" s="619"/>
       <c r="AO20" s="350" t="s">
         <v>478</v>
       </c>
@@ -8913,13 +8911,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="603"/>
+      <c r="F21" s="624"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="606"/>
-      <c r="Q21" s="609"/>
+      <c r="O21" s="658"/>
+      <c r="Q21" s="661"/>
       <c r="T21" s="447"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="639"/>
+      <c r="V21" s="594"/>
       <c r="W21" s="451" t="s">
         <v>176</v>
       </c>
@@ -8957,15 +8955,15 @@
       <c r="AM21" s="453" t="s">
         <v>567</v>
       </c>
-      <c r="AN21" s="622"/>
+      <c r="AN21" s="619"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="603"/>
+      <c r="F22" s="624"/>
       <c r="G22" s="349" t="s">
         <v>507</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="606"/>
+      <c r="O22" s="658"/>
       <c r="R22" s="459" t="s">
         <v>44</v>
       </c>
@@ -8973,7 +8971,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="640"/>
+      <c r="V22" s="595"/>
       <c r="W22" s="451" t="s">
         <v>176</v>
       </c>
@@ -8991,7 +8989,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="611" t="s">
+      <c r="AJ22" s="633" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="262"/>
@@ -8999,7 +8997,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="622"/>
+      <c r="AN22" s="619"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9017,17 +9015,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="603"/>
+      <c r="F23" s="624"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="606"/>
-      <c r="Q23" s="608" t="s">
+      <c r="O23" s="658"/>
+      <c r="Q23" s="660" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="445" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="640"/>
+      <c r="V23" s="595"/>
       <c r="W23" s="148"/>
       <c r="X23" s="454" t="s">
         <v>189</v>
@@ -9043,13 +9041,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="611"/>
+      <c r="AJ23" s="633"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="622"/>
+      <c r="AN23" s="619"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="465" t="s">
@@ -9067,18 +9065,18 @@
       <c r="E24" s="461">
         <v>1</v>
       </c>
-      <c r="F24" s="603"/>
+      <c r="F24" s="624"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="606"/>
-      <c r="Q24" s="609"/>
+      <c r="O24" s="658"/>
+      <c r="Q24" s="661"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="640"/>
+      <c r="V24" s="595"/>
       <c r="W24" s="148"/>
       <c r="X24" s="454" t="s">
         <v>186</v>
@@ -9102,12 +9100,12 @@
         <v>481</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="622"/>
+      <c r="AN24" s="619"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="603"/>
+      <c r="F25" s="624"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="606"/>
+      <c r="O25" s="658"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9120,7 +9118,7 @@
       <c r="U25" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="641"/>
+      <c r="V25" s="596"/>
       <c r="W25" s="148"/>
       <c r="X25" s="454" t="s">
         <v>190</v>
@@ -9142,7 +9140,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="622"/>
+      <c r="AN25" s="619"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9160,17 +9158,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="603"/>
+      <c r="F26" s="624"/>
       <c r="G26" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="606"/>
-      <c r="P26" s="624" t="s">
+      <c r="O26" s="658"/>
+      <c r="P26" s="621" t="s">
         <v>548</v>
       </c>
-      <c r="Q26" s="625"/>
-      <c r="R26" s="600" t="s">
+      <c r="Q26" s="622"/>
+      <c r="R26" s="654" t="s">
         <v>557</v>
       </c>
       <c r="T26" s="182"/>
@@ -9209,7 +9207,7 @@
       <c r="AM26" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="622"/>
+      <c r="AN26" s="619"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9221,13 +9219,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="604"/>
+      <c r="F27" s="656"/>
       <c r="G27" s="61" t="s">
         <v>566</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="607"/>
-      <c r="R27" s="601"/>
+      <c r="O27" s="659"/>
+      <c r="R27" s="655"/>
       <c r="S27" s="446" t="s">
         <v>54</v>
       </c>
@@ -9257,10 +9255,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="623"/>
+      <c r="AN27" s="620"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9277,44 +9313,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9324,8 +9322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="N12" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9420,17 +9418,17 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="666" t="s">
+      <c r="V1" s="669" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="667"/>
+      <c r="W1" s="670"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y1" s="102">
         <f>X1+X3</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z1" s="102" t="s">
         <v>458</v>
@@ -9439,21 +9437,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="668" t="s">
+      <c r="AC1" s="671" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="669"/>
-      <c r="AE1" s="670"/>
-      <c r="AF1" s="671" t="s">
+      <c r="AD1" s="672"/>
+      <c r="AE1" s="673"/>
+      <c r="AF1" s="674" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="672"/>
-      <c r="AH1" s="673"/>
-      <c r="AI1" s="663" t="s">
+      <c r="AG1" s="675"/>
+      <c r="AH1" s="676"/>
+      <c r="AI1" s="666" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="664"/>
-      <c r="AK1" s="665"/>
+      <c r="AJ1" s="667"/>
+      <c r="AK1" s="668"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9462,7 +9460,7 @@
       </c>
       <c r="H2" s="544">
         <f>SUM(H4:H37)</f>
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>236</v>
@@ -9470,19 +9468,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="674">
+      <c r="L2" s="677">
         <f>SUM(L5:L30)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="676">
+        <v>1</v>
+      </c>
+      <c r="M2" s="679">
         <f>SUM(M4:M29)</f>
         <v>6</v>
       </c>
-      <c r="N2" s="678">
+      <c r="N2" s="681">
         <f>SUM(N4:N29)</f>
         <v>5</v>
       </c>
-      <c r="O2" s="618">
+      <c r="O2" s="645">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-2</v>
       </c>
@@ -9501,7 +9499,7 @@
       <c r="T2" s="518" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="680" t="s">
+      <c r="U2" s="683" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="519" t="s">
@@ -9568,12 +9566,12 @@
       </c>
       <c r="K3" s="319">
         <f>T3+V3+W3+S3</f>
-        <v>68</v>
-      </c>
-      <c r="L3" s="675"/>
-      <c r="M3" s="677"/>
-      <c r="N3" s="679"/>
-      <c r="O3" s="619"/>
+        <v>69</v>
+      </c>
+      <c r="L3" s="678"/>
+      <c r="M3" s="680"/>
+      <c r="N3" s="682"/>
+      <c r="O3" s="646"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9589,14 +9587,14 @@
         <f>SUM(T4:T29)</f>
         <v>42</v>
       </c>
-      <c r="U3" s="681"/>
+      <c r="U3" s="684"/>
       <c r="V3" s="522">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>8</v>
       </c>
       <c r="W3" s="522">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9608,7 +9606,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9688,7 +9686,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="682" t="s">
+      <c r="O4" s="663" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -9767,7 +9765,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="683"/>
+      <c r="O5" s="664"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -9855,7 +9853,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="683"/>
+      <c r="O6" s="664"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9947,7 +9945,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="683"/>
+      <c r="O7" s="664"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10053,7 +10051,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="683"/>
+      <c r="O8" s="664"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10137,7 +10135,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="683"/>
+      <c r="O9" s="664"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10233,7 +10231,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="683"/>
+      <c r="O10" s="664"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10314,7 +10312,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="683"/>
+      <c r="O11" s="664"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10374,7 +10372,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="654" t="s">
+      <c r="A12" s="609" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10383,7 +10381,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="608" t="s">
+      <c r="E12" s="660" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10402,7 +10400,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="683"/>
+      <c r="O12" s="664"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10470,14 +10468,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="656"/>
+      <c r="A13" s="611"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="609"/>
+      <c r="E13" s="661"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10500,7 +10498,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="683"/>
+      <c r="O13" s="664"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10573,7 +10571,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14" s="683"/>
+      <c r="O14" s="664"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10670,7 +10668,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="683"/>
+      <c r="O15" s="664"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -10757,7 +10755,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="683"/>
+      <c r="O16" s="664"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10853,7 +10851,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O17" s="683"/>
+      <c r="O17" s="664"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -10937,7 +10935,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="683"/>
+      <c r="O18" s="664"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11004,21 +11002,23 @@
       <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="274"/>
+      <c r="H19" s="274">
+        <v>-1</v>
+      </c>
       <c r="K19" s="405" t="s">
         <v>309</v>
       </c>
       <c r="L19" s="118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="107">
         <v>0</v>
       </c>
       <c r="N19" s="299">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="683"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="664"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11038,19 +11038,19 @@
       </c>
       <c r="W19" s="527">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" s="302"/>
       <c r="Y19" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="296">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA19" s="296">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19" s="296">
         <f t="shared" si="4"/>
@@ -11063,21 +11063,21 @@
       <c r="AE19" s="302"/>
       <c r="AF19" s="302">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG19" s="348"/>
       <c r="AH19" s="158"/>
       <c r="AI19" s="314">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ19" s="315">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK19" s="316">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL19" s="6" t="s">
         <v>575</v>
@@ -11114,11 +11114,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O20" s="684"/>
+      <c r="O20" s="665"/>
       <c r="P20" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="610"/>
+      <c r="Q20" s="662"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11353,7 +11353,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="661" t="s">
+      <c r="E23" s="616" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11443,7 +11443,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="662"/>
+      <c r="E24" s="617"/>
       <c r="F24" s="176"/>
       <c r="K24" s="403" t="s">
         <v>301</v>
@@ -11456,12 +11456,12 @@
       </c>
       <c r="N24" s="299">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" s="559" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="610"/>
+      <c r="Q24" s="662"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -11482,14 +11482,14 @@
       <c r="X24" s="302"/>
       <c r="Y24" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="296">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="296">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="296">
         <f t="shared" si="4"/>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="AF24" s="302">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG24" s="348"/>
       <c r="AH24" s="158">
@@ -11514,15 +11514,15 @@
       </c>
       <c r="AI24" s="314">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ24" s="315">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK24" s="316">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL24" s="6" t="s">
         <v>528</v>
@@ -11989,7 +11989,7 @@
         <v>-1</v>
       </c>
       <c r="H31" s="42">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>436</v>
@@ -12526,12 +12526,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12541,6 +12535,12 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12577,12 +12577,12 @@
       <c r="B1" s="559" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="610"/>
+      <c r="C1" s="662"/>
       <c r="D1" s="209"/>
       <c r="J1" s="559" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="610"/>
+      <c r="K1" s="662"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -12973,7 +12973,7 @@
       <c r="V1" s="559" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="610"/>
+      <c r="W1" s="662"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12992,7 +12992,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="698" t="s">
+      <c r="AD1" s="705" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13009,10 +13009,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="697" t="s">
+      <c r="F2" s="736" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="725" t="s">
+      <c r="G2" s="693" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13040,10 +13040,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="666" t="s">
+      <c r="V2" s="669" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="667"/>
+      <c r="W2" s="670"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13062,7 +13062,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="699"/>
+      <c r="AD2" s="706"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13081,8 +13081,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="658"/>
-      <c r="G3" s="726"/>
+      <c r="F3" s="613"/>
+      <c r="G3" s="694"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13093,13 +13093,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="735" t="s">
+      <c r="O3" s="703" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="717" t="s">
+      <c r="P3" s="724" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="718"/>
+      <c r="Q3" s="725"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13109,15 +13109,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="699"/>
+      <c r="AD3" s="706"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="726"/>
+      <c r="G4" s="694"/>
       <c r="H4" s="6"/>
       <c r="L4" s="688" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="736"/>
+      <c r="O4" s="704"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13131,8 +13131,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="561"/>
-      <c r="AA4" s="610"/>
-      <c r="AD4" s="699"/>
+      <c r="AA4" s="662"/>
+      <c r="AD4" s="706"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13147,21 +13147,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="726"/>
+      <c r="G5" s="694"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="704" t="s">
+      <c r="K5" s="711" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="719"/>
+      <c r="L5" s="726"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="736"/>
+      <c r="O5" s="704"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13177,11 +13177,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="707" t="s">
+      <c r="Y5" s="714" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="708"/>
-      <c r="AD5" s="699"/>
+      <c r="Z5" s="715"/>
+      <c r="AD5" s="706"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13191,16 +13191,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="726"/>
+      <c r="G6" s="694"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="705"/>
-      <c r="L6" s="719"/>
-      <c r="O6" s="736"/>
+      <c r="K6" s="712"/>
+      <c r="L6" s="726"/>
+      <c r="O6" s="704"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13210,23 +13210,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="699"/>
+      <c r="AD6" s="706"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="726"/>
+      <c r="G7" s="694"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="705"/>
-      <c r="L7" s="719"/>
+      <c r="K7" s="712"/>
+      <c r="L7" s="726"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="736"/>
+      <c r="O7" s="704"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="699"/>
+      <c r="AD7" s="706"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13239,7 +13239,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="726"/>
+      <c r="G8" s="694"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13249,41 +13249,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="705"/>
-      <c r="L8" s="719"/>
-      <c r="O8" s="736"/>
+      <c r="K8" s="712"/>
+      <c r="L8" s="726"/>
+      <c r="O8" s="704"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="701" t="s">
+      <c r="S8" s="708" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="702"/>
-      <c r="U8" s="702"/>
-      <c r="V8" s="702"/>
-      <c r="W8" s="702"/>
-      <c r="X8" s="702"/>
-      <c r="Y8" s="702"/>
-      <c r="Z8" s="702"/>
-      <c r="AA8" s="702"/>
-      <c r="AB8" s="702"/>
-      <c r="AC8" s="703"/>
-      <c r="AD8" s="699"/>
+      <c r="T8" s="709"/>
+      <c r="U8" s="709"/>
+      <c r="V8" s="709"/>
+      <c r="W8" s="709"/>
+      <c r="X8" s="709"/>
+      <c r="Y8" s="709"/>
+      <c r="Z8" s="709"/>
+      <c r="AA8" s="709"/>
+      <c r="AB8" s="709"/>
+      <c r="AC8" s="710"/>
+      <c r="AD8" s="706"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="691"/>
-      <c r="G9" s="726"/>
+      <c r="C9" s="730"/>
+      <c r="G9" s="694"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="705"/>
-      <c r="L9" s="729" t="s">
+      <c r="K9" s="712"/>
+      <c r="L9" s="697" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="730"/>
-      <c r="N9" s="731"/>
-      <c r="O9" s="736"/>
+      <c r="M9" s="698"/>
+      <c r="N9" s="699"/>
+      <c r="O9" s="704"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="699"/>
+      <c r="AD9" s="706"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="692"/>
+      <c r="C10" s="731"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13291,7 +13291,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="726"/>
+      <c r="G10" s="694"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13299,33 +13299,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="705"/>
-      <c r="M10" s="694" t="s">
+      <c r="K10" s="712"/>
+      <c r="M10" s="733" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="695"/>
-      <c r="O10" s="695"/>
-      <c r="P10" s="695"/>
-      <c r="Q10" s="695"/>
-      <c r="R10" s="695"/>
-      <c r="S10" s="695"/>
-      <c r="T10" s="695"/>
-      <c r="U10" s="695"/>
-      <c r="V10" s="695"/>
-      <c r="W10" s="695"/>
-      <c r="X10" s="695"/>
-      <c r="Y10" s="695"/>
-      <c r="Z10" s="695"/>
-      <c r="AA10" s="695"/>
-      <c r="AB10" s="695"/>
-      <c r="AC10" s="696"/>
-      <c r="AD10" s="699"/>
+      <c r="N10" s="734"/>
+      <c r="O10" s="734"/>
+      <c r="P10" s="734"/>
+      <c r="Q10" s="734"/>
+      <c r="R10" s="734"/>
+      <c r="S10" s="734"/>
+      <c r="T10" s="734"/>
+      <c r="U10" s="734"/>
+      <c r="V10" s="734"/>
+      <c r="W10" s="734"/>
+      <c r="X10" s="734"/>
+      <c r="Y10" s="734"/>
+      <c r="Z10" s="734"/>
+      <c r="AA10" s="734"/>
+      <c r="AB10" s="734"/>
+      <c r="AC10" s="735"/>
+      <c r="AD10" s="706"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="693"/>
-      <c r="G11" s="726"/>
+      <c r="C11" s="732"/>
+      <c r="G11" s="694"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="705"/>
+      <c r="K11" s="712"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13333,17 +13333,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="715" t="s">
+      <c r="Z11" s="722" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="716"/>
+      <c r="AA11" s="723"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="699"/>
+      <c r="AD11" s="706"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13356,7 +13356,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="726"/>
+      <c r="G12" s="694"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13364,8 +13364,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="705"/>
-      <c r="L12" s="720" t="s">
+      <c r="K12" s="712"/>
+      <c r="L12" s="727" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13396,25 +13396,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="709" t="s">
+      <c r="AA12" s="716" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="710"/>
+      <c r="AB12" s="717"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="699"/>
+      <c r="AD12" s="706"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="691"/>
-      <c r="G13" s="726"/>
-      <c r="K13" s="705"/>
-      <c r="L13" s="721"/>
+      <c r="C13" s="730"/>
+      <c r="G13" s="694"/>
+      <c r="K13" s="712"/>
+      <c r="L13" s="728"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="728" t="s">
+      <c r="Q13" s="696" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="625"/>
+      <c r="R13" s="622"/>
       <c r="S13" s="555"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13423,17 +13423,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="711"/>
-      <c r="AB13" s="712"/>
-      <c r="AD13" s="699"/>
+      <c r="AA13" s="718"/>
+      <c r="AB13" s="719"/>
+      <c r="AD13" s="706"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="693"/>
+      <c r="C14" s="732"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="726"/>
+      <c r="G14" s="694"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13441,8 +13441,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="705"/>
-      <c r="L14" s="721"/>
+      <c r="K14" s="712"/>
+      <c r="L14" s="728"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13463,9 +13463,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="711"/>
-      <c r="AB14" s="712"/>
-      <c r="AD14" s="699"/>
+      <c r="AA14" s="718"/>
+      <c r="AB14" s="719"/>
+      <c r="AD14" s="706"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13480,19 +13480,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="726"/>
+      <c r="G15" s="694"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="705"/>
-      <c r="L15" s="722"/>
-      <c r="Q15" s="728" t="s">
+      <c r="K15" s="712"/>
+      <c r="L15" s="729"/>
+      <c r="Q15" s="696" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="625"/>
+      <c r="R15" s="622"/>
       <c r="S15" s="555"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13501,14 +13501,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="711"/>
-      <c r="AB15" s="712"/>
-      <c r="AD15" s="699"/>
+      <c r="AA15" s="718"/>
+      <c r="AB15" s="719"/>
+      <c r="AD15" s="706"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="726"/>
-      <c r="K16" s="705"/>
+      <c r="G16" s="694"/>
+      <c r="K16" s="712"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13527,24 +13527,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="711"/>
-      <c r="AB16" s="712"/>
-      <c r="AD16" s="699"/>
+      <c r="AA16" s="718"/>
+      <c r="AB16" s="719"/>
+      <c r="AD16" s="706"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="723" t="s">
+      <c r="F17" s="691" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="726"/>
+      <c r="G17" s="694"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="705"/>
+      <c r="K17" s="712"/>
       <c r="S17" s="555"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13552,9 +13552,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="711"/>
-      <c r="AB17" s="712"/>
-      <c r="AD17" s="699"/>
+      <c r="AA17" s="718"/>
+      <c r="AB17" s="719"/>
+      <c r="AD17" s="706"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13564,15 +13564,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="724"/>
-      <c r="G18" s="726"/>
+      <c r="F18" s="692"/>
+      <c r="G18" s="694"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="705"/>
+      <c r="K18" s="712"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13583,42 +13583,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="713"/>
-      <c r="AB18" s="714"/>
-      <c r="AD18" s="699"/>
+      <c r="AA18" s="720"/>
+      <c r="AB18" s="721"/>
+      <c r="AD18" s="706"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="727"/>
-      <c r="K19" s="706"/>
+      <c r="G19" s="695"/>
+      <c r="K19" s="713"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="732" t="s">
+      <c r="R19" s="700" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="733"/>
-      <c r="T19" s="734"/>
+      <c r="S19" s="701"/>
+      <c r="T19" s="702"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="700"/>
+      <c r="AD19" s="707"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13630,11 +13627,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>